<commit_message>
Terminator - Levels 1 & 2 done, 537 saved over v1.  Found a glitch at the beginning of level 3 saving 305 frames, 809 ahead total at this point.
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="119">
   <si>
     <t>Notes</t>
   </si>
@@ -474,6 +474,30 @@
   <si>
     <t>Every 10 Bonus Points given from Enemies Killed takes 1 frame to count down. 1 killed enemy = 1 frame more on score tally</t>
   </si>
+  <si>
+    <t>X &gt;= 557, Y =176</t>
+  </si>
+  <si>
+    <t>X &lt;= 1421, Y = 166</t>
+  </si>
+  <si>
+    <t>X &gt;= 1491, Y = 131</t>
+  </si>
+  <si>
+    <t>X&gt;= 2627, Y = 169</t>
+  </si>
+  <si>
+    <t>X&gt;= 3833, Y = 185</t>
+  </si>
+  <si>
+    <t>X&gt;= 3611, Y = 122</t>
+  </si>
+  <si>
+    <t>00FFF2B5 = 0</t>
+  </si>
+  <si>
+    <t>X = 281/280</t>
+  </si>
 </sst>
 </file>
 
@@ -483,10 +507,24 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1154,14 +1192,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1169,7 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1177,75 +1215,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1255,10 +1293,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1279,155 +1317,164 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1733,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O153"/>
+  <dimension ref="B1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1750,20 +1797,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="101" t="s">
+      <c r="C1" s="102"/>
+      <c r="D1" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="102"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="104"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
-        <f>SUM(H1:H65535)</f>
-        <v>0</v>
+        <f>SUM(H1:H65530)</f>
+        <v>225</v>
       </c>
       <c r="J1" s="71" t="s">
         <v>51</v>
@@ -1785,7 +1832,7 @@
       <c r="H2" s="70"/>
       <c r="I2" s="74">
         <f>IF(I1&lt;3600,I1/60,QUOTIENT(I1, 3600))</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="J2" s="71" t="str">
         <f>IF(I1&lt;3600,"Seconds","Minutes")</f>
@@ -1837,10 +1884,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="103"/>
+      <c r="E5" s="105"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -1877,7 +1924,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="106" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1897,7 +1944,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="105"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -1907,7 +1954,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="105"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -1918,7 +1965,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="105"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -1929,7 +1976,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="105"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -1940,7 +1987,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="105"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -1951,7 +1998,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="105"/>
+      <c r="B14" s="107"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -1962,7 +2009,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="105"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -1973,7 +2020,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="105"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2016,7 +2063,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="108" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2051,7 +2098,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="107"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2076,12 +2123,15 @@
         <f>K20-J20</f>
         <v>0</v>
       </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
       <c r="O20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="107"/>
+      <c r="B21" s="109"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2106,12 +2156,15 @@
         <f t="shared" ref="L21:L28" si="2">K21-J21</f>
         <v>0</v>
       </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
       <c r="O21">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="107"/>
+      <c r="B22" s="109"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2136,12 +2189,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
       <c r="O22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="107"/>
+      <c r="B23" s="109"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2166,16 +2222,21 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
       <c r="O23">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="107"/>
+      <c r="B24" s="109"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="30">
+        <v>3055</v>
+      </c>
       <c r="E24" s="30">
         <v>3055</v>
       </c>
@@ -2187,11 +2248,17 @@
       <c r="H24" t="s">
         <v>109</v>
       </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
       <c r="K24">
         <v>3</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
         <v>3</v>
       </c>
       <c r="O24">
@@ -2199,94 +2266,123 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="107"/>
+      <c r="B25" s="109"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="30">
+        <v>3436</v>
+      </c>
       <c r="E25" s="30">
         <v>3450</v>
       </c>
       <c r="F25" s="52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G25" s="34"/>
+      <c r="J25">
+        <v>13</v>
+      </c>
       <c r="K25">
         <v>13</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
       </c>
       <c r="O25">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="107"/>
+      <c r="B26" s="109"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="30"/>
+      <c r="D26" s="30">
+        <v>4176</v>
+      </c>
       <c r="E26" s="30">
         <v>4266</v>
       </c>
       <c r="F26" s="52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G26" s="34"/>
+      <c r="J26">
+        <v>9</v>
+      </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="L26">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-8</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
       </c>
       <c r="O26">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="107"/>
+      <c r="B27" s="109"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="30"/>
+      <c r="D27" s="30">
+        <v>5064</v>
+      </c>
       <c r="E27" s="30">
         <v>5218</v>
       </c>
       <c r="F27" s="52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="G27" s="34"/>
+      <c r="J27">
+        <v>5</v>
+      </c>
       <c r="K27">
         <v>1</v>
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-4</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
       </c>
       <c r="O27">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="107"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="28">
+        <v>5537</v>
+      </c>
       <c r="E28" s="28">
         <v>5762</v>
       </c>
       <c r="F28" s="54">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="G28" s="33"/>
+      <c r="J28">
+        <v>0</v>
+      </c>
       <c r="K28">
         <v>0</v>
       </c>
@@ -2294,18 +2390,21 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
       <c r="O28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="107"/>
+      <c r="B29" s="109"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="32">
         <f>D28-D20</f>
-        <v>-1978</v>
+        <v>3559</v>
       </c>
       <c r="E29" s="32">
         <f>E28-E20</f>
@@ -2313,19 +2412,19 @@
       </c>
       <c r="F29" s="55">
         <f>F28-F20</f>
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="G29" s="37"/>
       <c r="H29" s="41">
         <f>F29+H17</f>
-        <v>0</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="13.5" thickBot="1">
       <c r="B30" s="93"/>
     </row>
-    <row r="31" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B31" s="108" t="s">
+    <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B31" s="110" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2360,232 +2459,359 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="109"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
+      <c r="D32" s="28">
+        <v>5952</v>
+      </c>
+      <c r="E32" s="28">
+        <v>6178</v>
+      </c>
       <c r="F32" s="52">
-        <f t="shared" ref="F32:F45" si="3">IF(AND(D32&gt;0,E32&gt;0), E32-D32, 0)</f>
-        <v>0</v>
+        <f t="shared" ref="F32:F40" si="3">IF(AND(D32&gt;0,E32&gt;0), E32-D32, 0)</f>
+        <v>226</v>
       </c>
       <c r="G32" s="33"/>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B33" s="109"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
+      <c r="J32">
+        <v>40</v>
+      </c>
+      <c r="K32">
+        <v>40</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="15.75" thickTop="1">
+      <c r="B33" s="111"/>
+      <c r="C33" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="30">
+        <v>6283</v>
+      </c>
+      <c r="E33" s="30">
+        <v>6541</v>
+      </c>
       <c r="F33" s="53">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="2:8" ht="15">
-      <c r="B34" s="109"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
+      <c r="J33">
+        <v>32</v>
+      </c>
+      <c r="K33">
+        <v>36</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="15">
+      <c r="B34" s="111"/>
+      <c r="C34" s="100" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="30">
+        <v>6656</v>
+      </c>
+      <c r="E34" s="30">
+        <v>6898</v>
+      </c>
       <c r="F34" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="G34" s="34"/>
       <c r="H34" s="41"/>
-    </row>
-    <row r="35" spans="2:8" ht="15">
-      <c r="B35" s="109"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
+      <c r="J34">
+        <v>16</v>
+      </c>
+      <c r="K34">
+        <v>20</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+      <c r="O34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" ht="15">
+      <c r="B35" s="111"/>
+      <c r="C35" s="100" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="30">
+        <v>6793</v>
+      </c>
+      <c r="E35" s="30">
+        <v>7035</v>
+      </c>
       <c r="F35" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="G35" s="34"/>
-    </row>
-    <row r="36" spans="2:8" ht="15" customHeight="1">
-      <c r="B36" s="109"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="O35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" ht="15" customHeight="1">
+      <c r="B36" s="111"/>
+      <c r="C36" s="100" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="30">
+        <v>7176</v>
+      </c>
+      <c r="E36" s="30">
+        <v>7420</v>
+      </c>
       <c r="F36" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="G36" s="34"/>
-    </row>
-    <row r="37" spans="2:8" ht="15">
-      <c r="B37" s="109"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
+      <c r="O36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" ht="15">
+      <c r="B37" s="111"/>
+      <c r="C37" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="30">
+        <v>7634</v>
+      </c>
+      <c r="E37" s="30">
+        <v>7961</v>
+      </c>
       <c r="F37" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>327</v>
       </c>
       <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="2:8" ht="15">
-      <c r="B38" s="109"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
+      <c r="K37">
+        <v>14</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" ht="15">
+      <c r="B38" s="111"/>
+      <c r="C38" s="100" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="30">
+        <v>8182</v>
+      </c>
+      <c r="E38" s="30">
+        <v>8518</v>
+      </c>
       <c r="F38" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="2:8" ht="15">
-      <c r="B39" s="109"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
+      <c r="K38">
+        <v>12</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" ht="15">
+      <c r="B39" s="111"/>
+      <c r="C39" s="100" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="30">
+        <v>8593</v>
+      </c>
+      <c r="E39" s="30">
+        <v>9069</v>
+      </c>
       <c r="F39" s="52">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>476</v>
       </c>
       <c r="G39" s="34"/>
-    </row>
-    <row r="40" spans="2:8" ht="15">
-      <c r="B40" s="109"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="52">
+      <c r="K39">
+        <v>12</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B40" s="101"/>
+      <c r="C40" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="28">
+        <v>8846</v>
+      </c>
+      <c r="E40" s="28">
+        <v>9383</v>
+      </c>
+      <c r="F40" s="54">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="34"/>
-    </row>
-    <row r="41" spans="2:8" ht="15">
-      <c r="B41" s="109"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="34"/>
-    </row>
-    <row r="42" spans="2:8" ht="15">
-      <c r="B42" s="109"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="34"/>
-    </row>
-    <row r="43" spans="2:8" ht="15">
-      <c r="B43" s="109"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G43" s="34"/>
-    </row>
-    <row r="44" spans="2:8" ht="15">
+        <v>537</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B41" s="45">
+        <v>2</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="32">
+        <f>D40-D32</f>
+        <v>2894</v>
+      </c>
+      <c r="E41" s="32">
+        <f>E40-E32</f>
+        <v>3205</v>
+      </c>
+      <c r="F41" s="55">
+        <f>F40-F32</f>
+        <v>311</v>
+      </c>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
+    <row r="43" spans="2:15" ht="15">
+      <c r="B43" s="108" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" ht="15.75" thickBot="1">
       <c r="B44" s="109"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
+      <c r="C44" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="28">
+        <v>9312</v>
+      </c>
+      <c r="E44" s="28">
+        <v>9816</v>
+      </c>
       <c r="F44" s="52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G44" s="34"/>
-    </row>
-    <row r="45" spans="2:8" ht="15.75" thickBot="1">
+        <f t="shared" ref="F44:F57" si="4">IF(AND(D44&gt;0,E44&gt;0), E44-D44, 0)</f>
+        <v>504</v>
+      </c>
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="2:15" ht="15.75" thickTop="1">
       <c r="B45" s="109"/>
-      <c r="C45" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B46" s="45">
-        <v>2</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="32">
-        <f>D45-D32</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="32">
-        <f>E45-E32</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="55">
-        <f>F45-F32</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="36"/>
-    </row>
-    <row r="47" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="48" spans="2:8" ht="15">
-      <c r="B48" s="106" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B49" s="107"/>
-      <c r="C49" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="C45" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="30">
+        <v>9514</v>
+      </c>
+      <c r="E45" s="30">
+        <v>10323</v>
+      </c>
+      <c r="F45" s="53">
+        <f t="shared" si="4"/>
+        <v>809</v>
+      </c>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="2:15" ht="15">
+      <c r="B46" s="109"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="34"/>
+      <c r="H46" s="41"/>
+    </row>
+    <row r="47" spans="2:15" ht="15">
+      <c r="B47" s="109"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="2:15" ht="15" customHeight="1">
+      <c r="B48" s="109"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="34"/>
+    </row>
+    <row r="49" spans="2:8" ht="15">
+      <c r="B49" s="109"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
       <c r="F49" s="52">
-        <f t="shared" ref="F49:F62" si="4">IF(AND(D49&gt;0,E49&gt;0), E49-D49, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="33"/>
-    </row>
-    <row r="50" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B50" s="107"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="34"/>
+    </row>
+    <row r="50" spans="2:8" ht="15">
+      <c r="B50" s="109"/>
       <c r="C50" s="29"/>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
-      <c r="F50" s="53">
+      <c r="F50" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:8" ht="15">
-      <c r="B51" s="107"/>
+      <c r="B51" s="109"/>
       <c r="C51" s="29"/>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
@@ -2594,13 +2820,9 @@
         <v>0</v>
       </c>
       <c r="G51" s="34"/>
-      <c r="H51" s="41">
-        <f>F46</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="52" spans="2:8" ht="15">
-      <c r="B52" s="107"/>
+      <c r="B52" s="109"/>
       <c r="C52" s="29"/>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -2610,8 +2832,8 @@
       </c>
       <c r="G52" s="34"/>
     </row>
-    <row r="53" spans="2:8" ht="15" customHeight="1">
-      <c r="B53" s="107"/>
+    <row r="53" spans="2:8" ht="15">
+      <c r="B53" s="109"/>
       <c r="C53" s="29"/>
       <c r="D53" s="30"/>
       <c r="E53" s="30"/>
@@ -2622,7 +2844,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:8" ht="15">
-      <c r="B54" s="107"/>
+      <c r="B54" s="109"/>
       <c r="C54" s="29"/>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
@@ -2633,7 +2855,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:8" ht="15">
-      <c r="B55" s="107"/>
+      <c r="B55" s="109"/>
       <c r="C55" s="29"/>
       <c r="D55" s="30"/>
       <c r="E55" s="30"/>
@@ -2644,7 +2866,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:8" ht="15">
-      <c r="B56" s="107"/>
+      <c r="B56" s="109"/>
       <c r="C56" s="29"/>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -2654,142 +2876,143 @@
       </c>
       <c r="G56" s="34"/>
     </row>
-    <row r="57" spans="2:8" ht="15">
-      <c r="B57" s="107"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="52">
+    <row r="57" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B57" s="109"/>
+      <c r="C57" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G57" s="34"/>
-    </row>
-    <row r="58" spans="2:8" ht="15">
-      <c r="B58" s="107"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="52">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G58" s="34"/>
-    </row>
-    <row r="59" spans="2:8" ht="15">
-      <c r="B59" s="107"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="52">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G59" s="34"/>
-    </row>
+      <c r="G57" s="33"/>
+    </row>
+    <row r="58" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B58" s="46">
+        <v>3</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="32">
+        <f>D57-D44</f>
+        <v>-9312</v>
+      </c>
+      <c r="E58" s="32">
+        <f>E57-E44</f>
+        <v>-9816</v>
+      </c>
+      <c r="F58" s="55">
+        <f>F57-F44</f>
+        <v>-504</v>
+      </c>
+      <c r="G58" s="37"/>
+    </row>
+    <row r="59" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="60" spans="2:8" ht="15">
-      <c r="B60" s="107"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="52">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G60" s="34"/>
-    </row>
-    <row r="61" spans="2:8" ht="15">
-      <c r="B61" s="107"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
+      <c r="B60" s="110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B61" s="111"/>
+      <c r="C61" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="52">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G61" s="34"/>
-    </row>
-    <row r="62" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B62" s="107"/>
-      <c r="C62" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="54">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G62" s="33"/>
-    </row>
-    <row r="63" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B63" s="46">
-        <v>3</v>
-      </c>
-      <c r="C63" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" s="32">
-        <f>D62-D49</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="32">
-        <f>E62-E49</f>
-        <v>0</v>
-      </c>
-      <c r="F63" s="55">
-        <f>F62-F49</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="37"/>
-    </row>
-    <row r="64" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="65" spans="2:8" ht="15">
-      <c r="B65" s="108" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E65" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F65" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G65" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B66" s="109"/>
-      <c r="C66" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
+        <f t="shared" ref="F61:F74" si="5">IF(AND(D61&gt;0,E61&gt;0), E61-D61, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G61" s="33"/>
+    </row>
+    <row r="62" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B62" s="111"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="53">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="34"/>
+    </row>
+    <row r="63" spans="2:8" ht="15">
+      <c r="B63" s="111"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="34"/>
+      <c r="H63" s="41"/>
+    </row>
+    <row r="64" spans="2:8" ht="15">
+      <c r="B64" s="111"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="34"/>
+    </row>
+    <row r="65" spans="2:8" ht="15" customHeight="1">
+      <c r="B65" s="111"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="34"/>
+    </row>
+    <row r="66" spans="2:8" ht="15">
+      <c r="B66" s="111"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
       <c r="F66" s="52">
-        <f t="shared" ref="F66:F79" si="5">IF(AND(D66&gt;0,E66&gt;0), E66-D66, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G66" s="33"/>
-    </row>
-    <row r="67" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B67" s="109"/>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="34"/>
+    </row>
+    <row r="67" spans="2:8" ht="15">
+      <c r="B67" s="111"/>
       <c r="C67" s="29"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
-      <c r="F67" s="53">
+      <c r="F67" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G67" s="34"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="109"/>
+      <c r="B68" s="111"/>
       <c r="C68" s="29"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -2798,13 +3021,9 @@
         <v>0</v>
       </c>
       <c r="G68" s="34"/>
-      <c r="H68" s="41">
-        <f>F63</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="69" spans="2:8" ht="15">
-      <c r="B69" s="109"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="29"/>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -2814,8 +3033,8 @@
       </c>
       <c r="G69" s="34"/>
     </row>
-    <row r="70" spans="2:8" ht="15" customHeight="1">
-      <c r="B70" s="109"/>
+    <row r="70" spans="2:8" ht="15">
+      <c r="B70" s="111"/>
       <c r="C70" s="29"/>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -2826,7 +3045,7 @@
       <c r="G70" s="34"/>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="109"/>
+      <c r="B71" s="111"/>
       <c r="C71" s="29"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -2837,7 +3056,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="109"/>
+      <c r="B72" s="111"/>
       <c r="C72" s="29"/>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -2848,7 +3067,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="109"/>
+      <c r="B73" s="111"/>
       <c r="C73" s="29"/>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -2858,142 +3077,143 @@
       </c>
       <c r="G73" s="34"/>
     </row>
-    <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="109"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="52">
+    <row r="74" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B74" s="111"/>
+      <c r="C74" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="54">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G74" s="34"/>
-    </row>
-    <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="109"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G75" s="34"/>
-    </row>
-    <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="109"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G76" s="34"/>
-    </row>
+      <c r="G74" s="33"/>
+    </row>
+    <row r="75" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B75" s="45">
+        <v>4</v>
+      </c>
+      <c r="C75" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="32">
+        <f>D74-D61</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="32">
+        <f>E74-E61</f>
+        <v>0</v>
+      </c>
+      <c r="F75" s="55">
+        <f>F74-F61</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="36"/>
+    </row>
+    <row r="76" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="109"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G77" s="34"/>
-    </row>
-    <row r="78" spans="2:8" ht="15">
+      <c r="B77" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="15.75" thickBot="1">
       <c r="B78" s="109"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
+      <c r="C78" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
       <c r="F78" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G78" s="34"/>
-    </row>
-    <row r="79" spans="2:8" ht="15.75" thickBot="1">
+        <f t="shared" ref="F78:F91" si="6">IF(AND(D78&gt;0,E78&gt;0), E78-D78, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="33"/>
+    </row>
+    <row r="79" spans="2:8" ht="15.75" thickTop="1">
       <c r="B79" s="109"/>
-      <c r="C79" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="54">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G79" s="33"/>
-    </row>
-    <row r="80" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B80" s="45">
-        <v>4</v>
-      </c>
-      <c r="C80" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="32">
-        <f>D79-D66</f>
-        <v>0</v>
-      </c>
-      <c r="E80" s="32">
-        <f>E79-E66</f>
-        <v>0</v>
-      </c>
-      <c r="F80" s="55">
-        <f>F79-F66</f>
-        <v>0</v>
-      </c>
-      <c r="G80" s="36"/>
-    </row>
-    <row r="81" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="82" spans="2:8" ht="15">
-      <c r="B82" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="C82" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E82" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F82" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G82" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B83" s="107"/>
-      <c r="C83" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="53">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G79" s="34"/>
+    </row>
+    <row r="80" spans="2:8" ht="15">
+      <c r="B80" s="109"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G80" s="34"/>
+      <c r="H80" s="41"/>
+    </row>
+    <row r="81" spans="2:7" ht="15">
+      <c r="B81" s="109"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G81" s="34"/>
+    </row>
+    <row r="82" spans="2:7" ht="15" customHeight="1">
+      <c r="B82" s="109"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+      <c r="F82" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G82" s="34"/>
+    </row>
+    <row r="83" spans="2:7" ht="15">
+      <c r="B83" s="109"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="30"/>
       <c r="F83" s="52">
-        <f t="shared" ref="F83:F96" si="6">IF(AND(D83&gt;0,E83&gt;0), E83-D83, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G83" s="33"/>
-    </row>
-    <row r="84" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B84" s="107"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="34"/>
+    </row>
+    <row r="84" spans="2:7" ht="15">
+      <c r="B84" s="109"/>
       <c r="C84" s="29"/>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
-      <c r="F84" s="53">
+      <c r="F84" s="52">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:8" ht="15">
-      <c r="B85" s="107"/>
+    <row r="85" spans="2:7" ht="15">
+      <c r="B85" s="109"/>
       <c r="C85" s="29"/>
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
@@ -3002,13 +3222,9 @@
         <v>0</v>
       </c>
       <c r="G85" s="34"/>
-      <c r="H85" s="41">
-        <f>F80</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" ht="15">
-      <c r="B86" s="107"/>
+    </row>
+    <row r="86" spans="2:7" ht="15">
+      <c r="B86" s="109"/>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -3018,8 +3234,8 @@
       </c>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1">
-      <c r="B87" s="107"/>
+    <row r="87" spans="2:7" ht="15">
+      <c r="B87" s="109"/>
       <c r="C87" s="29"/>
       <c r="D87" s="30"/>
       <c r="E87" s="30"/>
@@ -3029,8 +3245,8 @@
       </c>
       <c r="G87" s="34"/>
     </row>
-    <row r="88" spans="2:8" ht="15">
-      <c r="B88" s="107"/>
+    <row r="88" spans="2:7" ht="15">
+      <c r="B88" s="109"/>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -3040,8 +3256,8 @@
       </c>
       <c r="G88" s="34"/>
     </row>
-    <row r="89" spans="2:8" ht="15">
-      <c r="B89" s="107"/>
+    <row r="89" spans="2:7" ht="15">
+      <c r="B89" s="109"/>
       <c r="C89" s="29"/>
       <c r="D89" s="30"/>
       <c r="E89" s="30"/>
@@ -3051,8 +3267,8 @@
       </c>
       <c r="G89" s="34"/>
     </row>
-    <row r="90" spans="2:8" ht="15">
-      <c r="B90" s="107"/>
+    <row r="90" spans="2:7" ht="15">
+      <c r="B90" s="109"/>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -3062,142 +3278,143 @@
       </c>
       <c r="G90" s="34"/>
     </row>
-    <row r="91" spans="2:8" ht="15">
-      <c r="B91" s="107"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="52">
+    <row r="91" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B91" s="109"/>
+      <c r="C91" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="54">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G91" s="34"/>
-    </row>
-    <row r="92" spans="2:8" ht="15">
-      <c r="B92" s="107"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G92" s="34"/>
-    </row>
-    <row r="93" spans="2:8" ht="15">
-      <c r="B93" s="107"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G93" s="34"/>
-    </row>
-    <row r="94" spans="2:8" ht="15">
-      <c r="B94" s="107"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G94" s="34"/>
-    </row>
-    <row r="95" spans="2:8" ht="15">
-      <c r="B95" s="107"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
+      <c r="G91" s="33"/>
+    </row>
+    <row r="92" spans="2:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B92" s="46">
+        <v>5</v>
+      </c>
+      <c r="C92" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="32">
+        <f>D91-D78</f>
+        <v>0</v>
+      </c>
+      <c r="E92" s="32">
+        <f>E91-E78</f>
+        <v>0</v>
+      </c>
+      <c r="F92" s="55">
+        <f>F91-F78</f>
+        <v>0</v>
+      </c>
+      <c r="G92" s="37"/>
+    </row>
+    <row r="93" spans="2:7" ht="13.5" thickBot="1"/>
+    <row r="94" spans="2:7" ht="15">
+      <c r="B94" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E94" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B95" s="111"/>
+      <c r="C95" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
       <c r="F95" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G95" s="34"/>
-    </row>
-    <row r="96" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B96" s="107"/>
-      <c r="C96" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="54">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G96" s="33"/>
-    </row>
-    <row r="97" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B97" s="46">
-        <v>5</v>
-      </c>
-      <c r="C97" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D97" s="32">
-        <f>D96-D83</f>
-        <v>0</v>
-      </c>
-      <c r="E97" s="32">
-        <f>E96-E83</f>
-        <v>0</v>
-      </c>
-      <c r="F97" s="55">
-        <f>F96-F83</f>
-        <v>0</v>
-      </c>
-      <c r="G97" s="37"/>
-    </row>
-    <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="108" t="s">
-        <v>18</v>
-      </c>
-      <c r="C99" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D99" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F99" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G99" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="109"/>
-      <c r="C100" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
+        <f t="shared" ref="F95:F108" si="7">IF(AND(D95&gt;0,E95&gt;0), E95-D95, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G95" s="33"/>
+    </row>
+    <row r="96" spans="2:7" ht="15.75" thickTop="1">
+      <c r="B96" s="111"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G96" s="34"/>
+    </row>
+    <row r="97" spans="2:8" ht="15">
+      <c r="B97" s="111"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G97" s="34"/>
+      <c r="H97" s="41"/>
+    </row>
+    <row r="98" spans="2:8" ht="15">
+      <c r="B98" s="111"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="30"/>
+      <c r="F98" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G98" s="34"/>
+    </row>
+    <row r="99" spans="2:8" ht="15" customHeight="1">
+      <c r="B99" s="111"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G99" s="34"/>
+    </row>
+    <row r="100" spans="2:8" ht="15">
+      <c r="B100" s="111"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="30"/>
       <c r="F100" s="52">
-        <f t="shared" ref="F100:F113" si="7">IF(AND(D100&gt;0,E100&gt;0), E100-D100, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G100" s="33"/>
-    </row>
-    <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="109"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G100" s="34"/>
+    </row>
+    <row r="101" spans="2:8" ht="15">
+      <c r="B101" s="111"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
-      <c r="F101" s="53">
+      <c r="F101" s="52">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="109"/>
+      <c r="B102" s="111"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -3206,13 +3423,9 @@
         <v>0</v>
       </c>
       <c r="G102" s="34"/>
-      <c r="H102" s="41">
-        <f>F97</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="109"/>
+      <c r="B103" s="111"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
       <c r="E103" s="30"/>
@@ -3222,8 +3435,8 @@
       </c>
       <c r="G103" s="34"/>
     </row>
-    <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="109"/>
+    <row r="104" spans="2:8" ht="15">
+      <c r="B104" s="111"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -3234,7 +3447,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="109"/>
+      <c r="B105" s="111"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
       <c r="E105" s="30"/>
@@ -3245,7 +3458,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="109"/>
+      <c r="B106" s="111"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -3256,7 +3469,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="109"/>
+      <c r="B107" s="111"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
@@ -3266,142 +3479,143 @@
       </c>
       <c r="G107" s="34"/>
     </row>
-    <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="109"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="30"/>
-      <c r="F108" s="52">
+    <row r="108" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B108" s="111"/>
+      <c r="C108" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="54">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G108" s="34"/>
-    </row>
-    <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="109"/>
-      <c r="C109" s="29"/>
-      <c r="D109" s="30"/>
-      <c r="E109" s="30"/>
-      <c r="F109" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G109" s="34"/>
-    </row>
-    <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="109"/>
-      <c r="C110" s="29"/>
-      <c r="D110" s="30"/>
-      <c r="E110" s="30"/>
-      <c r="F110" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G110" s="34"/>
-    </row>
+      <c r="G108" s="33"/>
+    </row>
+    <row r="109" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B109" s="45">
+        <v>6</v>
+      </c>
+      <c r="C109" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="32">
+        <f>D108-D95</f>
+        <v>0</v>
+      </c>
+      <c r="E109" s="32">
+        <f>E108-E95</f>
+        <v>0</v>
+      </c>
+      <c r="F109" s="32">
+        <f>F108-F95</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="36"/>
+    </row>
+    <row r="110" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="109"/>
-      <c r="C111" s="29"/>
-      <c r="D111" s="30"/>
-      <c r="E111" s="30"/>
-      <c r="F111" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G111" s="34"/>
-    </row>
-    <row r="112" spans="2:8" ht="15">
+      <c r="B111" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D111" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F111" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G111" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" ht="15.75" thickBot="1">
       <c r="B112" s="109"/>
-      <c r="C112" s="29"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="30"/>
+      <c r="C112" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
       <c r="F112" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G112" s="34"/>
-    </row>
-    <row r="113" spans="2:8" ht="15.75" thickBot="1">
+        <f t="shared" ref="F112:F125" si="8">IF(AND(D112&gt;0,E112&gt;0), E112-D112, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G112" s="33"/>
+    </row>
+    <row r="113" spans="2:8" ht="15.75" thickTop="1">
       <c r="B113" s="109"/>
-      <c r="C113" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="54">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G113" s="33"/>
-    </row>
-    <row r="114" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B114" s="45">
-        <v>6</v>
-      </c>
-      <c r="C114" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D114" s="32">
-        <f>D113-D100</f>
-        <v>0</v>
-      </c>
-      <c r="E114" s="32">
-        <f>E113-E100</f>
-        <v>0</v>
-      </c>
-      <c r="F114" s="32">
-        <f>F113-F100</f>
-        <v>0</v>
-      </c>
-      <c r="G114" s="36"/>
-    </row>
-    <row r="115" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="116" spans="2:8" ht="15">
-      <c r="B116" s="106" t="s">
-        <v>19</v>
-      </c>
-      <c r="C116" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D116" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E116" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F116" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G116" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B117" s="107"/>
-      <c r="C117" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D117" s="28"/>
-      <c r="E117" s="28"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="30"/>
+      <c r="F113" s="53">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G113" s="34"/>
+    </row>
+    <row r="114" spans="2:8" ht="15">
+      <c r="B114" s="109"/>
+      <c r="C114" s="29"/>
+      <c r="D114" s="30"/>
+      <c r="E114" s="30"/>
+      <c r="F114" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G114" s="34"/>
+      <c r="H114" s="41"/>
+    </row>
+    <row r="115" spans="2:8" ht="15">
+      <c r="B115" s="109"/>
+      <c r="C115" s="29"/>
+      <c r="D115" s="30"/>
+      <c r="E115" s="30"/>
+      <c r="F115" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G115" s="34"/>
+    </row>
+    <row r="116" spans="2:8" ht="15" customHeight="1">
+      <c r="B116" s="109"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="30"/>
+      <c r="F116" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="34"/>
+    </row>
+    <row r="117" spans="2:8" ht="15">
+      <c r="B117" s="109"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
       <c r="F117" s="52">
-        <f t="shared" ref="F117:F130" si="8">IF(AND(D117&gt;0,E117&gt;0), E117-D117, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G117" s="33"/>
-    </row>
-    <row r="118" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B118" s="107"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="34"/>
+    </row>
+    <row r="118" spans="2:8" ht="15">
+      <c r="B118" s="109"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
-      <c r="F118" s="53">
+      <c r="F118" s="52">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:8" ht="15">
-      <c r="B119" s="107"/>
+      <c r="B119" s="109"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
@@ -3410,13 +3624,9 @@
         <v>0</v>
       </c>
       <c r="G119" s="34"/>
-      <c r="H119" s="41">
-        <f>F114</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="120" spans="2:8" ht="15">
-      <c r="B120" s="107"/>
+      <c r="B120" s="109"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -3426,8 +3636,8 @@
       </c>
       <c r="G120" s="34"/>
     </row>
-    <row r="121" spans="2:8" ht="15" customHeight="1">
-      <c r="B121" s="107"/>
+    <row r="121" spans="2:8" ht="15">
+      <c r="B121" s="109"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
@@ -3438,7 +3648,7 @@
       <c r="G121" s="34"/>
     </row>
     <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="107"/>
+      <c r="B122" s="109"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -3449,7 +3659,7 @@
       <c r="G122" s="34"/>
     </row>
     <row r="123" spans="2:8" ht="15">
-      <c r="B123" s="107"/>
+      <c r="B123" s="109"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
@@ -3460,7 +3670,7 @@
       <c r="G123" s="34"/>
     </row>
     <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="107"/>
+      <c r="B124" s="109"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -3470,142 +3680,143 @@
       </c>
       <c r="G124" s="34"/>
     </row>
-    <row r="125" spans="2:8" ht="15">
-      <c r="B125" s="107"/>
-      <c r="C125" s="29"/>
-      <c r="D125" s="30"/>
-      <c r="E125" s="30"/>
-      <c r="F125" s="52">
+    <row r="125" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B125" s="109"/>
+      <c r="C125" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125" s="28"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="54">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G125" s="34"/>
-    </row>
-    <row r="126" spans="2:8" ht="15">
-      <c r="B126" s="107"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="30"/>
-      <c r="F126" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G126" s="34"/>
-    </row>
-    <row r="127" spans="2:8" ht="15">
-      <c r="B127" s="107"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="30"/>
-      <c r="E127" s="30"/>
-      <c r="F127" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G127" s="34"/>
-    </row>
+      <c r="G125" s="33"/>
+    </row>
+    <row r="126" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B126" s="46">
+        <v>7</v>
+      </c>
+      <c r="C126" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" s="32">
+        <f>D125-D112</f>
+        <v>0</v>
+      </c>
+      <c r="E126" s="32">
+        <f>E125-E112</f>
+        <v>0</v>
+      </c>
+      <c r="F126" s="32">
+        <f>F125-F112</f>
+        <v>0</v>
+      </c>
+      <c r="G126" s="37"/>
+    </row>
+    <row r="127" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="107"/>
-      <c r="C128" s="29"/>
-      <c r="D128" s="30"/>
-      <c r="E128" s="30"/>
-      <c r="F128" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G128" s="34"/>
-    </row>
-    <row r="129" spans="2:8" ht="15">
-      <c r="B129" s="107"/>
-      <c r="C129" s="29"/>
-      <c r="D129" s="30"/>
-      <c r="E129" s="30"/>
+      <c r="B128" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D128" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E128" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F128" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G128" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B129" s="111"/>
+      <c r="C129" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129" s="28"/>
+      <c r="E129" s="28"/>
       <c r="F129" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G129" s="34"/>
-    </row>
-    <row r="130" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B130" s="107"/>
-      <c r="C130" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D130" s="28"/>
-      <c r="E130" s="28"/>
-      <c r="F130" s="54">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G130" s="33"/>
-    </row>
-    <row r="131" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B131" s="46">
-        <v>7</v>
-      </c>
-      <c r="C131" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D131" s="32">
-        <f>D130-D117</f>
-        <v>0</v>
-      </c>
-      <c r="E131" s="32">
-        <f>E130-E117</f>
-        <v>0</v>
-      </c>
-      <c r="F131" s="32">
-        <f>F130-F117</f>
-        <v>0</v>
-      </c>
-      <c r="G131" s="37"/>
-    </row>
-    <row r="132" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="133" spans="2:8" ht="15">
-      <c r="B133" s="108" t="s">
-        <v>20</v>
-      </c>
-      <c r="C133" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D133" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E133" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F133" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G133" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="134" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B134" s="109"/>
-      <c r="C134" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D134" s="28"/>
-      <c r="E134" s="28"/>
+        <f t="shared" ref="F129:F142" si="9">IF(AND(D129&gt;0,E129&gt;0), E129-D129, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G129" s="33"/>
+    </row>
+    <row r="130" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B130" s="111"/>
+      <c r="C130" s="29"/>
+      <c r="D130" s="30"/>
+      <c r="E130" s="30"/>
+      <c r="F130" s="53">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G130" s="34"/>
+    </row>
+    <row r="131" spans="2:8" ht="15">
+      <c r="B131" s="111"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="30"/>
+      <c r="F131" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G131" s="34"/>
+      <c r="H131" s="41"/>
+    </row>
+    <row r="132" spans="2:8" ht="15">
+      <c r="B132" s="111"/>
+      <c r="C132" s="29"/>
+      <c r="D132" s="30"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G132" s="34"/>
+    </row>
+    <row r="133" spans="2:8" ht="15" customHeight="1">
+      <c r="B133" s="111"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="30"/>
+      <c r="E133" s="30"/>
+      <c r="F133" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G133" s="34"/>
+    </row>
+    <row r="134" spans="2:8" ht="15">
+      <c r="B134" s="111"/>
+      <c r="C134" s="29"/>
+      <c r="D134" s="30"/>
+      <c r="E134" s="30"/>
       <c r="F134" s="52">
-        <f t="shared" ref="F134:F147" si="9">IF(AND(D134&gt;0,E134&gt;0), E134-D134, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G134" s="33"/>
-    </row>
-    <row r="135" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B135" s="109"/>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G134" s="34"/>
+    </row>
+    <row r="135" spans="2:8" ht="15">
+      <c r="B135" s="111"/>
       <c r="C135" s="29"/>
       <c r="D135" s="30"/>
       <c r="E135" s="30"/>
-      <c r="F135" s="53">
+      <c r="F135" s="52">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G135" s="34"/>
     </row>
     <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="109"/>
+      <c r="B136" s="111"/>
       <c r="C136" s="29"/>
       <c r="D136" s="30"/>
       <c r="E136" s="30"/>
@@ -3614,13 +3825,9 @@
         <v>0</v>
       </c>
       <c r="G136" s="34"/>
-      <c r="H136" s="41">
-        <f>F131</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="137" spans="2:8" ht="15">
-      <c r="B137" s="109"/>
+      <c r="B137" s="111"/>
       <c r="C137" s="29"/>
       <c r="D137" s="30"/>
       <c r="E137" s="30"/>
@@ -3630,8 +3837,8 @@
       </c>
       <c r="G137" s="34"/>
     </row>
-    <row r="138" spans="2:8" ht="15" customHeight="1">
-      <c r="B138" s="109"/>
+    <row r="138" spans="2:8" ht="15">
+      <c r="B138" s="111"/>
       <c r="C138" s="29"/>
       <c r="D138" s="30"/>
       <c r="E138" s="30"/>
@@ -3642,7 +3849,7 @@
       <c r="G138" s="34"/>
     </row>
     <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="109"/>
+      <c r="B139" s="111"/>
       <c r="C139" s="29"/>
       <c r="D139" s="30"/>
       <c r="E139" s="30"/>
@@ -3653,7 +3860,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:8" ht="15">
-      <c r="B140" s="109"/>
+      <c r="B140" s="111"/>
       <c r="C140" s="29"/>
       <c r="D140" s="30"/>
       <c r="E140" s="30"/>
@@ -3664,7 +3871,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:8" ht="15">
-      <c r="B141" s="109"/>
+      <c r="B141" s="111"/>
       <c r="C141" s="29"/>
       <c r="D141" s="30"/>
       <c r="E141" s="30"/>
@@ -3674,115 +3881,57 @@
       </c>
       <c r="G141" s="34"/>
     </row>
-    <row r="142" spans="2:8" ht="15">
-      <c r="B142" s="109"/>
-      <c r="C142" s="29"/>
-      <c r="D142" s="30"/>
-      <c r="E142" s="30"/>
-      <c r="F142" s="52">
+    <row r="142" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B142" s="111"/>
+      <c r="C142" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142" s="28"/>
+      <c r="E142" s="28"/>
+      <c r="F142" s="54">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G142" s="34"/>
-    </row>
-    <row r="143" spans="2:8" ht="15">
-      <c r="B143" s="109"/>
-      <c r="C143" s="29"/>
-      <c r="D143" s="30"/>
-      <c r="E143" s="30"/>
-      <c r="F143" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G143" s="34"/>
-    </row>
-    <row r="144" spans="2:8" ht="15">
-      <c r="B144" s="109"/>
-      <c r="C144" s="29"/>
-      <c r="D144" s="30"/>
-      <c r="E144" s="30"/>
-      <c r="F144" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G144" s="34"/>
-    </row>
-    <row r="145" spans="2:8" ht="15">
-      <c r="B145" s="109"/>
-      <c r="C145" s="29"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="30"/>
-      <c r="F145" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G145" s="34"/>
-    </row>
-    <row r="146" spans="2:8" ht="15">
-      <c r="B146" s="109"/>
-      <c r="C146" s="29"/>
-      <c r="D146" s="30"/>
-      <c r="E146" s="30"/>
-      <c r="F146" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G146" s="34"/>
-    </row>
-    <row r="147" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B147" s="109"/>
-      <c r="C147" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D147" s="28"/>
-      <c r="E147" s="28"/>
-      <c r="F147" s="54">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G147" s="33"/>
-    </row>
-    <row r="148" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B148" s="45">
+      <c r="G142" s="33"/>
+    </row>
+    <row r="143" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B143" s="45">
         <v>8</v>
       </c>
-      <c r="C148" s="31" t="s">
+      <c r="C143" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D148" s="32">
-        <f>D147-D134</f>
-        <v>0</v>
-      </c>
-      <c r="E148" s="32">
-        <f>E147-E134</f>
-        <v>0</v>
-      </c>
-      <c r="F148" s="32">
-        <f>F147-F134</f>
-        <v>0</v>
-      </c>
-      <c r="G148" s="36"/>
-    </row>
-    <row r="153" spans="2:8">
-      <c r="H153" s="41">
-        <f>F148</f>
-        <v>0</v>
-      </c>
+      <c r="D143" s="32">
+        <f>D142-D129</f>
+        <v>0</v>
+      </c>
+      <c r="E143" s="32">
+        <f>E142-E129</f>
+        <v>0</v>
+      </c>
+      <c r="F143" s="32">
+        <f>F142-F129</f>
+        <v>0</v>
+      </c>
+      <c r="G143" s="36"/>
+    </row>
+    <row r="148" spans="8:8">
+      <c r="H148" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B133:B147"/>
+    <mergeCell ref="B128:B142"/>
     <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B31:B45"/>
-    <mergeCell ref="B48:B62"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="B82:B96"/>
-    <mergeCell ref="B99:B113"/>
+    <mergeCell ref="B43:B57"/>
+    <mergeCell ref="B60:B74"/>
+    <mergeCell ref="B77:B91"/>
+    <mergeCell ref="B94:B108"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B116:B130"/>
+    <mergeCell ref="B111:B125"/>
+    <mergeCell ref="B31:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3808,51 +3957,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="117"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="112"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="114"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -3966,19 +4115,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="112"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="114"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4092,19 +4241,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="112"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="114"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4218,19 +4367,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="112"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="114"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4344,19 +4493,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="111"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="111"/>
-      <c r="J35" s="111"/>
-      <c r="K35" s="112"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="114"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -4468,19 +4617,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="110" t="s">
+      <c r="A43" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="111"/>
-      <c r="C43" s="111"/>
-      <c r="D43" s="111"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="111"/>
-      <c r="G43" s="111"/>
-      <c r="H43" s="111"/>
-      <c r="I43" s="111"/>
-      <c r="J43" s="111"/>
-      <c r="K43" s="112"/>
+      <c r="B43" s="113"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="113"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="113"/>
+      <c r="H43" s="113"/>
+      <c r="I43" s="113"/>
+      <c r="J43" s="113"/>
+      <c r="K43" s="114"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -4594,19 +4743,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="110" t="s">
+      <c r="A51" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="111"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="112"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+      <c r="G51" s="113"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="113"/>
+      <c r="J51" s="113"/>
+      <c r="K51" s="114"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -4726,19 +4875,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="110" t="s">
+      <c r="A59" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="111"/>
-      <c r="C59" s="111"/>
-      <c r="D59" s="111"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="111"/>
-      <c r="I59" s="111"/>
-      <c r="J59" s="111"/>
-      <c r="K59" s="112"/>
+      <c r="B59" s="113"/>
+      <c r="C59" s="113"/>
+      <c r="D59" s="113"/>
+      <c r="E59" s="113"/>
+      <c r="F59" s="113"/>
+      <c r="G59" s="113"/>
+      <c r="H59" s="113"/>
+      <c r="I59" s="113"/>
+      <c r="J59" s="113"/>
+      <c r="K59" s="114"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -4848,19 +4997,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="110" t="s">
+      <c r="A67" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="111"/>
-      <c r="C67" s="111"/>
-      <c r="D67" s="111"/>
-      <c r="E67" s="111"/>
-      <c r="F67" s="111"/>
-      <c r="G67" s="111"/>
-      <c r="H67" s="111"/>
-      <c r="I67" s="111"/>
-      <c r="J67" s="111"/>
-      <c r="K67" s="112"/>
+      <c r="B67" s="113"/>
+      <c r="C67" s="113"/>
+      <c r="D67" s="113"/>
+      <c r="E67" s="113"/>
+      <c r="F67" s="113"/>
+      <c r="G67" s="113"/>
+      <c r="H67" s="113"/>
+      <c r="I67" s="113"/>
+      <c r="J67" s="113"/>
+      <c r="K67" s="114"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -4968,19 +5117,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="110" t="s">
+      <c r="A75" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="111"/>
-      <c r="C75" s="111"/>
-      <c r="D75" s="111"/>
-      <c r="E75" s="111"/>
-      <c r="F75" s="111"/>
-      <c r="G75" s="111"/>
-      <c r="H75" s="111"/>
-      <c r="I75" s="111"/>
-      <c r="J75" s="111"/>
-      <c r="K75" s="112"/>
+      <c r="B75" s="113"/>
+      <c r="C75" s="113"/>
+      <c r="D75" s="113"/>
+      <c r="E75" s="113"/>
+      <c r="F75" s="113"/>
+      <c r="G75" s="113"/>
+      <c r="H75" s="113"/>
+      <c r="I75" s="113"/>
+      <c r="J75" s="113"/>
+      <c r="K75" s="114"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5096,19 +5245,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="111"/>
-      <c r="C83" s="111"/>
-      <c r="D83" s="111"/>
-      <c r="E83" s="111"/>
-      <c r="F83" s="111"/>
-      <c r="G83" s="111"/>
-      <c r="H83" s="111"/>
-      <c r="I83" s="111"/>
-      <c r="J83" s="111"/>
-      <c r="K83" s="112"/>
+      <c r="B83" s="113"/>
+      <c r="C83" s="113"/>
+      <c r="D83" s="113"/>
+      <c r="E83" s="113"/>
+      <c r="F83" s="113"/>
+      <c r="G83" s="113"/>
+      <c r="H83" s="113"/>
+      <c r="I83" s="113"/>
+      <c r="J83" s="113"/>
+      <c r="K83" s="114"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5220,19 +5369,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="110" t="s">
+      <c r="A91" s="112" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="111"/>
-      <c r="C91" s="111"/>
-      <c r="D91" s="111"/>
-      <c r="E91" s="111"/>
-      <c r="F91" s="111"/>
-      <c r="G91" s="111"/>
-      <c r="H91" s="111"/>
-      <c r="I91" s="111"/>
-      <c r="J91" s="111"/>
-      <c r="K91" s="112"/>
+      <c r="B91" s="113"/>
+      <c r="C91" s="113"/>
+      <c r="D91" s="113"/>
+      <c r="E91" s="113"/>
+      <c r="F91" s="113"/>
+      <c r="G91" s="113"/>
+      <c r="H91" s="113"/>
+      <c r="I91" s="113"/>
+      <c r="J91" s="113"/>
+      <c r="K91" s="114"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5346,19 +5495,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="110" t="s">
+      <c r="A99" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="111"/>
-      <c r="C99" s="111"/>
-      <c r="D99" s="111"/>
-      <c r="E99" s="111"/>
-      <c r="F99" s="111"/>
-      <c r="G99" s="111"/>
-      <c r="H99" s="111"/>
-      <c r="I99" s="111"/>
-      <c r="J99" s="111"/>
-      <c r="K99" s="112"/>
+      <c r="B99" s="113"/>
+      <c r="C99" s="113"/>
+      <c r="D99" s="113"/>
+      <c r="E99" s="113"/>
+      <c r="F99" s="113"/>
+      <c r="G99" s="113"/>
+      <c r="H99" s="113"/>
+      <c r="I99" s="113"/>
+      <c r="J99" s="113"/>
+      <c r="K99" s="114"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -5462,19 +5611,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="110" t="s">
+      <c r="A107" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="111"/>
-      <c r="C107" s="111"/>
-      <c r="D107" s="111"/>
-      <c r="E107" s="111"/>
-      <c r="F107" s="111"/>
-      <c r="G107" s="111"/>
-      <c r="H107" s="111"/>
-      <c r="I107" s="111"/>
-      <c r="J107" s="111"/>
-      <c r="K107" s="112"/>
+      <c r="B107" s="113"/>
+      <c r="C107" s="113"/>
+      <c r="D107" s="113"/>
+      <c r="E107" s="113"/>
+      <c r="F107" s="113"/>
+      <c r="G107" s="113"/>
+      <c r="H107" s="113"/>
+      <c r="I107" s="113"/>
+      <c r="J107" s="113"/>
+      <c r="K107" s="114"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -5596,7 +5745,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -5811,7 +5960,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -5838,10 +5987,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="118"/>
+      <c r="C1" s="120"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -5852,7 +6001,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="121" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -5866,7 +6015,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="120"/>
+      <c r="A4" s="122"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -5878,7 +6027,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="120"/>
+      <c r="A5" s="122"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -5887,7 +6036,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="120"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -5899,7 +6048,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="120"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -5911,7 +6060,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="120"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -5920,7 +6069,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -5935,7 +6084,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="121" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -5949,7 +6098,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="120"/>
+      <c r="A12" s="122"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -5961,7 +6110,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="120"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -5970,7 +6119,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="120"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -5982,7 +6131,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="120"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -5994,7 +6143,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="120"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6003,7 +6152,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="121"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6018,7 +6167,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="119" t="s">
+      <c r="A19" s="121" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6027,7 +6176,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="120"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6037,14 +6186,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="120"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="120"/>
+      <c r="A22" s="122"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6054,7 +6203,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="120"/>
+      <c r="A23" s="122"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6064,14 +6213,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="120"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="121"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6084,7 +6233,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6106,147 +6255,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="133"/>
+      <c r="B1" s="135"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="139"/>
+      <c r="B2" s="141"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="139"/>
+      <c r="B3" s="141"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="136"/>
-      <c r="B4" s="137"/>
+      <c r="A4" s="138"/>
+      <c r="B4" s="139"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="135"/>
+      <c r="B5" s="137"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="127"/>
+      <c r="B7" s="129"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="129"/>
+      <c r="B9" s="131"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="130"/>
-      <c r="B10" s="131"/>
+      <c r="A10" s="132"/>
+      <c r="B10" s="133"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="123"/>
+      <c r="B11" s="125"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="123"/>
+      <c r="B12" s="125"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="123"/>
+      <c r="B13" s="125"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="123"/>
+      <c r="B14" s="125"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="123"/>
+      <c r="B15" s="125"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="123"/>
+      <c r="B16" s="125"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="125"/>
+      <c r="B17" s="127"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="127"/>
+      <c r="B19" s="129"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="128" t="s">
+      <c r="A21" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="129"/>
+      <c r="B21" s="131"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="130"/>
-      <c r="B22" s="131"/>
+      <c r="A22" s="132"/>
+      <c r="B22" s="133"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="123"/>
+      <c r="B23" s="125"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="122"/>
-      <c r="B24" s="123"/>
+      <c r="A24" s="124"/>
+      <c r="B24" s="125"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="122" t="s">
+      <c r="A25" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="123"/>
+      <c r="B25" s="125"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="122" t="s">
+      <c r="A26" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="123"/>
+      <c r="B26" s="125"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="124"/>
-      <c r="B27" s="125"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Terminator - some of level 3 done, but now I'm stuck due to terrible randomness
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="122">
   <si>
     <t>Notes</t>
   </si>
@@ -498,6 +498,15 @@
   <si>
     <t>X = 281/280</t>
   </si>
+  <si>
+    <t>Platform up</t>
+  </si>
+  <si>
+    <t>Begin Down ladder</t>
+  </si>
+  <si>
+    <t>Down ladder</t>
+  </si>
 </sst>
 </file>
 
@@ -507,10 +516,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1192,14 +1208,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1207,7 +1223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,75 +1231,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1293,10 +1309,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1317,162 +1333,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1782,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1797,16 +1816,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="103" t="s">
+      <c r="C1" s="107"/>
+      <c r="D1" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="109"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
         <f>SUM(H1:H65530)</f>
@@ -1884,10 +1903,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -1924,7 +1943,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="111" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1944,7 +1963,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="107"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -1954,7 +1973,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="107"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -1965,7 +1984,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="107"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -1976,7 +1995,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="107"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -1987,7 +2006,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="107"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -1998,7 +2017,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="107"/>
+      <c r="B14" s="112"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2009,7 +2028,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="107"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2020,7 +2039,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="107"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2063,7 +2082,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="105" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2098,7 +2117,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="109"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2131,7 +2150,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="109"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2164,7 +2183,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="109"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2197,7 +2216,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="109"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2230,7 +2249,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="109"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2266,7 +2285,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="109"/>
+      <c r="B25" s="106"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2299,7 +2318,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="109"/>
+      <c r="B26" s="106"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2332,7 +2351,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="109"/>
+      <c r="B27" s="106"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2365,7 +2384,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="109"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2398,7 +2417,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="109"/>
+      <c r="B29" s="106"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2424,7 +2443,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="103" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2459,7 +2478,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="111"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2488,7 +2507,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="111"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2517,7 +2536,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="111"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2547,7 +2566,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="111"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2567,7 +2586,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="111"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2587,7 +2606,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="111"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2610,7 +2629,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="111"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2633,7 +2652,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="111"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2701,7 +2720,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="105" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2721,7 +2740,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="109"/>
+      <c r="B44" s="106"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2738,8 +2757,8 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="109"/>
-      <c r="C45" s="143" t="s">
+      <c r="B45" s="106"/>
+      <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
       <c r="D45" s="30">
@@ -2755,41 +2774,59 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="109"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="102" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="30">
+        <v>9813</v>
+      </c>
+      <c r="E46" s="30">
+        <v>10630</v>
+      </c>
       <c r="F46" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>817</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="109"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="144" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="30">
+        <v>10271</v>
+      </c>
+      <c r="E47" s="30">
+        <v>11097</v>
+      </c>
       <c r="F47" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="109"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
+      <c r="B48" s="106"/>
+      <c r="C48" s="144" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="30">
+        <v>10785</v>
+      </c>
+      <c r="E48" s="30">
+        <v>11600</v>
+      </c>
       <c r="F48" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>815</v>
       </c>
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:8" ht="15">
-      <c r="B49" s="109"/>
+      <c r="B49" s="106"/>
       <c r="C49" s="29"/>
       <c r="D49" s="30"/>
       <c r="E49" s="30"/>
@@ -2800,7 +2837,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:8" ht="15">
-      <c r="B50" s="109"/>
+      <c r="B50" s="106"/>
       <c r="C50" s="29"/>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -2811,7 +2848,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:8" ht="15">
-      <c r="B51" s="109"/>
+      <c r="B51" s="106"/>
       <c r="C51" s="29"/>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
@@ -2822,7 +2859,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:8" ht="15">
-      <c r="B52" s="109"/>
+      <c r="B52" s="106"/>
       <c r="C52" s="29"/>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -2833,7 +2870,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:8" ht="15">
-      <c r="B53" s="109"/>
+      <c r="B53" s="106"/>
       <c r="C53" s="29"/>
       <c r="D53" s="30"/>
       <c r="E53" s="30"/>
@@ -2844,7 +2881,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:8" ht="15">
-      <c r="B54" s="109"/>
+      <c r="B54" s="106"/>
       <c r="C54" s="29"/>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
@@ -2855,7 +2892,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:8" ht="15">
-      <c r="B55" s="109"/>
+      <c r="B55" s="106"/>
       <c r="C55" s="29"/>
       <c r="D55" s="30"/>
       <c r="E55" s="30"/>
@@ -2866,7 +2903,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:8" ht="15">
-      <c r="B56" s="109"/>
+      <c r="B56" s="106"/>
       <c r="C56" s="29"/>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -2877,7 +2914,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B57" s="109"/>
+      <c r="B57" s="106"/>
       <c r="C57" s="27" t="s">
         <v>32</v>
       </c>
@@ -2912,7 +2949,7 @@
     </row>
     <row r="59" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="60" spans="2:8" ht="15">
-      <c r="B60" s="110" t="s">
+      <c r="B60" s="103" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="42" t="s">
@@ -2932,7 +2969,7 @@
       </c>
     </row>
     <row r="61" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B61" s="111"/>
+      <c r="B61" s="104"/>
       <c r="C61" s="27" t="s">
         <v>29</v>
       </c>
@@ -2945,7 +2982,7 @@
       <c r="G61" s="33"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B62" s="111"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="29"/>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -2956,7 +2993,7 @@
       <c r="G62" s="34"/>
     </row>
     <row r="63" spans="2:8" ht="15">
-      <c r="B63" s="111"/>
+      <c r="B63" s="104"/>
       <c r="C63" s="29"/>
       <c r="D63" s="30"/>
       <c r="E63" s="30"/>
@@ -2968,7 +3005,7 @@
       <c r="H63" s="41"/>
     </row>
     <row r="64" spans="2:8" ht="15">
-      <c r="B64" s="111"/>
+      <c r="B64" s="104"/>
       <c r="C64" s="29"/>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -2979,7 +3016,7 @@
       <c r="G64" s="34"/>
     </row>
     <row r="65" spans="2:8" ht="15" customHeight="1">
-      <c r="B65" s="111"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="29"/>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
@@ -2990,7 +3027,7 @@
       <c r="G65" s="34"/>
     </row>
     <row r="66" spans="2:8" ht="15">
-      <c r="B66" s="111"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="29"/>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -3001,7 +3038,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="111"/>
+      <c r="B67" s="104"/>
       <c r="C67" s="29"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -3012,7 +3049,7 @@
       <c r="G67" s="34"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="111"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="29"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -3023,7 +3060,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15">
-      <c r="B69" s="111"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="29"/>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -3034,7 +3071,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="111"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="29"/>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -3045,7 +3082,7 @@
       <c r="G70" s="34"/>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="111"/>
+      <c r="B71" s="104"/>
       <c r="C71" s="29"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -3056,7 +3093,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="111"/>
+      <c r="B72" s="104"/>
       <c r="C72" s="29"/>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3067,7 +3104,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="111"/>
+      <c r="B73" s="104"/>
       <c r="C73" s="29"/>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3078,7 +3115,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B74" s="111"/>
+      <c r="B74" s="104"/>
       <c r="C74" s="27" t="s">
         <v>32</v>
       </c>
@@ -3113,7 +3150,7 @@
     </row>
     <row r="76" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="108" t="s">
+      <c r="B77" s="105" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="38" t="s">
@@ -3133,7 +3170,7 @@
       </c>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="109"/>
+      <c r="B78" s="106"/>
       <c r="C78" s="27" t="s">
         <v>29</v>
       </c>
@@ -3146,7 +3183,7 @@
       <c r="G78" s="33"/>
     </row>
     <row r="79" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B79" s="109"/>
+      <c r="B79" s="106"/>
       <c r="C79" s="29"/>
       <c r="D79" s="30"/>
       <c r="E79" s="30"/>
@@ -3157,7 +3194,7 @@
       <c r="G79" s="34"/>
     </row>
     <row r="80" spans="2:8" ht="15">
-      <c r="B80" s="109"/>
+      <c r="B80" s="106"/>
       <c r="C80" s="29"/>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -3169,7 +3206,7 @@
       <c r="H80" s="41"/>
     </row>
     <row r="81" spans="2:7" ht="15">
-      <c r="B81" s="109"/>
+      <c r="B81" s="106"/>
       <c r="C81" s="29"/>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
@@ -3180,7 +3217,7 @@
       <c r="G81" s="34"/>
     </row>
     <row r="82" spans="2:7" ht="15" customHeight="1">
-      <c r="B82" s="109"/>
+      <c r="B82" s="106"/>
       <c r="C82" s="29"/>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -3191,7 +3228,7 @@
       <c r="G82" s="34"/>
     </row>
     <row r="83" spans="2:7" ht="15">
-      <c r="B83" s="109"/>
+      <c r="B83" s="106"/>
       <c r="C83" s="29"/>
       <c r="D83" s="30"/>
       <c r="E83" s="30"/>
@@ -3202,7 +3239,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:7" ht="15">
-      <c r="B84" s="109"/>
+      <c r="B84" s="106"/>
       <c r="C84" s="29"/>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
@@ -3213,7 +3250,7 @@
       <c r="G84" s="34"/>
     </row>
     <row r="85" spans="2:7" ht="15">
-      <c r="B85" s="109"/>
+      <c r="B85" s="106"/>
       <c r="C85" s="29"/>
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
@@ -3224,7 +3261,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:7" ht="15">
-      <c r="B86" s="109"/>
+      <c r="B86" s="106"/>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -3235,7 +3272,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:7" ht="15">
-      <c r="B87" s="109"/>
+      <c r="B87" s="106"/>
       <c r="C87" s="29"/>
       <c r="D87" s="30"/>
       <c r="E87" s="30"/>
@@ -3246,7 +3283,7 @@
       <c r="G87" s="34"/>
     </row>
     <row r="88" spans="2:7" ht="15">
-      <c r="B88" s="109"/>
+      <c r="B88" s="106"/>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -3257,7 +3294,7 @@
       <c r="G88" s="34"/>
     </row>
     <row r="89" spans="2:7" ht="15">
-      <c r="B89" s="109"/>
+      <c r="B89" s="106"/>
       <c r="C89" s="29"/>
       <c r="D89" s="30"/>
       <c r="E89" s="30"/>
@@ -3268,7 +3305,7 @@
       <c r="G89" s="34"/>
     </row>
     <row r="90" spans="2:7" ht="15">
-      <c r="B90" s="109"/>
+      <c r="B90" s="106"/>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -3279,7 +3316,7 @@
       <c r="G90" s="34"/>
     </row>
     <row r="91" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B91" s="109"/>
+      <c r="B91" s="106"/>
       <c r="C91" s="27" t="s">
         <v>32</v>
       </c>
@@ -3314,7 +3351,7 @@
     </row>
     <row r="93" spans="2:7" ht="13.5" thickBot="1"/>
     <row r="94" spans="2:7" ht="15">
-      <c r="B94" s="110" t="s">
+      <c r="B94" s="103" t="s">
         <v>18</v>
       </c>
       <c r="C94" s="42" t="s">
@@ -3334,7 +3371,7 @@
       </c>
     </row>
     <row r="95" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B95" s="111"/>
+      <c r="B95" s="104"/>
       <c r="C95" s="27" t="s">
         <v>29</v>
       </c>
@@ -3347,7 +3384,7 @@
       <c r="G95" s="33"/>
     </row>
     <row r="96" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B96" s="111"/>
+      <c r="B96" s="104"/>
       <c r="C96" s="29"/>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
@@ -3358,7 +3395,7 @@
       <c r="G96" s="34"/>
     </row>
     <row r="97" spans="2:8" ht="15">
-      <c r="B97" s="111"/>
+      <c r="B97" s="104"/>
       <c r="C97" s="29"/>
       <c r="D97" s="30"/>
       <c r="E97" s="30"/>
@@ -3370,7 +3407,7 @@
       <c r="H97" s="41"/>
     </row>
     <row r="98" spans="2:8" ht="15">
-      <c r="B98" s="111"/>
+      <c r="B98" s="104"/>
       <c r="C98" s="29"/>
       <c r="D98" s="30"/>
       <c r="E98" s="30"/>
@@ -3381,7 +3418,7 @@
       <c r="G98" s="34"/>
     </row>
     <row r="99" spans="2:8" ht="15" customHeight="1">
-      <c r="B99" s="111"/>
+      <c r="B99" s="104"/>
       <c r="C99" s="29"/>
       <c r="D99" s="30"/>
       <c r="E99" s="30"/>
@@ -3392,7 +3429,7 @@
       <c r="G99" s="34"/>
     </row>
     <row r="100" spans="2:8" ht="15">
-      <c r="B100" s="111"/>
+      <c r="B100" s="104"/>
       <c r="C100" s="29"/>
       <c r="D100" s="30"/>
       <c r="E100" s="30"/>
@@ -3403,7 +3440,7 @@
       <c r="G100" s="34"/>
     </row>
     <row r="101" spans="2:8" ht="15">
-      <c r="B101" s="111"/>
+      <c r="B101" s="104"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
@@ -3414,7 +3451,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="111"/>
+      <c r="B102" s="104"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -3425,7 +3462,7 @@
       <c r="G102" s="34"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="111"/>
+      <c r="B103" s="104"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
       <c r="E103" s="30"/>
@@ -3436,7 +3473,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15">
-      <c r="B104" s="111"/>
+      <c r="B104" s="104"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -3447,7 +3484,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="111"/>
+      <c r="B105" s="104"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
       <c r="E105" s="30"/>
@@ -3458,7 +3495,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="111"/>
+      <c r="B106" s="104"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -3469,7 +3506,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="111"/>
+      <c r="B107" s="104"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
@@ -3480,7 +3517,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B108" s="111"/>
+      <c r="B108" s="104"/>
       <c r="C108" s="27" t="s">
         <v>32</v>
       </c>
@@ -3515,7 +3552,7 @@
     </row>
     <row r="110" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="108" t="s">
+      <c r="B111" s="105" t="s">
         <v>19</v>
       </c>
       <c r="C111" s="38" t="s">
@@ -3535,7 +3572,7 @@
       </c>
     </row>
     <row r="112" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B112" s="109"/>
+      <c r="B112" s="106"/>
       <c r="C112" s="27" t="s">
         <v>29</v>
       </c>
@@ -3548,7 +3585,7 @@
       <c r="G112" s="33"/>
     </row>
     <row r="113" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B113" s="109"/>
+      <c r="B113" s="106"/>
       <c r="C113" s="29"/>
       <c r="D113" s="30"/>
       <c r="E113" s="30"/>
@@ -3559,7 +3596,7 @@
       <c r="G113" s="34"/>
     </row>
     <row r="114" spans="2:8" ht="15">
-      <c r="B114" s="109"/>
+      <c r="B114" s="106"/>
       <c r="C114" s="29"/>
       <c r="D114" s="30"/>
       <c r="E114" s="30"/>
@@ -3571,7 +3608,7 @@
       <c r="H114" s="41"/>
     </row>
     <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="109"/>
+      <c r="B115" s="106"/>
       <c r="C115" s="29"/>
       <c r="D115" s="30"/>
       <c r="E115" s="30"/>
@@ -3582,7 +3619,7 @@
       <c r="G115" s="34"/>
     </row>
     <row r="116" spans="2:8" ht="15" customHeight="1">
-      <c r="B116" s="109"/>
+      <c r="B116" s="106"/>
       <c r="C116" s="29"/>
       <c r="D116" s="30"/>
       <c r="E116" s="30"/>
@@ -3593,7 +3630,7 @@
       <c r="G116" s="34"/>
     </row>
     <row r="117" spans="2:8" ht="15">
-      <c r="B117" s="109"/>
+      <c r="B117" s="106"/>
       <c r="C117" s="29"/>
       <c r="D117" s="30"/>
       <c r="E117" s="30"/>
@@ -3604,7 +3641,7 @@
       <c r="G117" s="34"/>
     </row>
     <row r="118" spans="2:8" ht="15">
-      <c r="B118" s="109"/>
+      <c r="B118" s="106"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -3615,7 +3652,7 @@
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:8" ht="15">
-      <c r="B119" s="109"/>
+      <c r="B119" s="106"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
@@ -3626,7 +3663,7 @@
       <c r="G119" s="34"/>
     </row>
     <row r="120" spans="2:8" ht="15">
-      <c r="B120" s="109"/>
+      <c r="B120" s="106"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -3637,7 +3674,7 @@
       <c r="G120" s="34"/>
     </row>
     <row r="121" spans="2:8" ht="15">
-      <c r="B121" s="109"/>
+      <c r="B121" s="106"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
@@ -3648,7 +3685,7 @@
       <c r="G121" s="34"/>
     </row>
     <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="109"/>
+      <c r="B122" s="106"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -3659,7 +3696,7 @@
       <c r="G122" s="34"/>
     </row>
     <row r="123" spans="2:8" ht="15">
-      <c r="B123" s="109"/>
+      <c r="B123" s="106"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
@@ -3670,7 +3707,7 @@
       <c r="G123" s="34"/>
     </row>
     <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="109"/>
+      <c r="B124" s="106"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -3681,7 +3718,7 @@
       <c r="G124" s="34"/>
     </row>
     <row r="125" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B125" s="109"/>
+      <c r="B125" s="106"/>
       <c r="C125" s="27" t="s">
         <v>32</v>
       </c>
@@ -3716,7 +3753,7 @@
     </row>
     <row r="127" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="110" t="s">
+      <c r="B128" s="103" t="s">
         <v>20</v>
       </c>
       <c r="C128" s="42" t="s">
@@ -3736,7 +3773,7 @@
       </c>
     </row>
     <row r="129" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B129" s="111"/>
+      <c r="B129" s="104"/>
       <c r="C129" s="27" t="s">
         <v>29</v>
       </c>
@@ -3749,7 +3786,7 @@
       <c r="G129" s="33"/>
     </row>
     <row r="130" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B130" s="111"/>
+      <c r="B130" s="104"/>
       <c r="C130" s="29"/>
       <c r="D130" s="30"/>
       <c r="E130" s="30"/>
@@ -3760,7 +3797,7 @@
       <c r="G130" s="34"/>
     </row>
     <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="111"/>
+      <c r="B131" s="104"/>
       <c r="C131" s="29"/>
       <c r="D131" s="30"/>
       <c r="E131" s="30"/>
@@ -3772,7 +3809,7 @@
       <c r="H131" s="41"/>
     </row>
     <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="111"/>
+      <c r="B132" s="104"/>
       <c r="C132" s="29"/>
       <c r="D132" s="30"/>
       <c r="E132" s="30"/>
@@ -3783,7 +3820,7 @@
       <c r="G132" s="34"/>
     </row>
     <row r="133" spans="2:8" ht="15" customHeight="1">
-      <c r="B133" s="111"/>
+      <c r="B133" s="104"/>
       <c r="C133" s="29"/>
       <c r="D133" s="30"/>
       <c r="E133" s="30"/>
@@ -3794,7 +3831,7 @@
       <c r="G133" s="34"/>
     </row>
     <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="111"/>
+      <c r="B134" s="104"/>
       <c r="C134" s="29"/>
       <c r="D134" s="30"/>
       <c r="E134" s="30"/>
@@ -3805,7 +3842,7 @@
       <c r="G134" s="34"/>
     </row>
     <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="111"/>
+      <c r="B135" s="104"/>
       <c r="C135" s="29"/>
       <c r="D135" s="30"/>
       <c r="E135" s="30"/>
@@ -3816,7 +3853,7 @@
       <c r="G135" s="34"/>
     </row>
     <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="111"/>
+      <c r="B136" s="104"/>
       <c r="C136" s="29"/>
       <c r="D136" s="30"/>
       <c r="E136" s="30"/>
@@ -3827,7 +3864,7 @@
       <c r="G136" s="34"/>
     </row>
     <row r="137" spans="2:8" ht="15">
-      <c r="B137" s="111"/>
+      <c r="B137" s="104"/>
       <c r="C137" s="29"/>
       <c r="D137" s="30"/>
       <c r="E137" s="30"/>
@@ -3838,7 +3875,7 @@
       <c r="G137" s="34"/>
     </row>
     <row r="138" spans="2:8" ht="15">
-      <c r="B138" s="111"/>
+      <c r="B138" s="104"/>
       <c r="C138" s="29"/>
       <c r="D138" s="30"/>
       <c r="E138" s="30"/>
@@ -3849,7 +3886,7 @@
       <c r="G138" s="34"/>
     </row>
     <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="111"/>
+      <c r="B139" s="104"/>
       <c r="C139" s="29"/>
       <c r="D139" s="30"/>
       <c r="E139" s="30"/>
@@ -3860,7 +3897,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:8" ht="15">
-      <c r="B140" s="111"/>
+      <c r="B140" s="104"/>
       <c r="C140" s="29"/>
       <c r="D140" s="30"/>
       <c r="E140" s="30"/>
@@ -3871,7 +3908,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:8" ht="15">
-      <c r="B141" s="111"/>
+      <c r="B141" s="104"/>
       <c r="C141" s="29"/>
       <c r="D141" s="30"/>
       <c r="E141" s="30"/>
@@ -3882,7 +3919,7 @@
       <c r="G141" s="34"/>
     </row>
     <row r="142" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B142" s="111"/>
+      <c r="B142" s="104"/>
       <c r="C142" s="27" t="s">
         <v>32</v>
       </c>
@@ -3920,18 +3957,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B8:B16"/>
+    <mergeCell ref="B111:B125"/>
+    <mergeCell ref="B31:B39"/>
     <mergeCell ref="B128:B142"/>
     <mergeCell ref="B19:B29"/>
     <mergeCell ref="B43:B57"/>
     <mergeCell ref="B60:B74"/>
     <mergeCell ref="B77:B91"/>
     <mergeCell ref="B94:B108"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B111:B125"/>
-    <mergeCell ref="B31:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3957,51 +3994,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="117"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="113" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="114"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="115"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4115,19 +4152,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="113"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="114"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="115"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4241,19 +4278,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="112" t="s">
+      <c r="A19" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="114"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="114"/>
+      <c r="K19" s="115"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4367,19 +4404,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="112" t="s">
+      <c r="A27" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
-      <c r="G27" s="113"/>
-      <c r="H27" s="113"/>
-      <c r="I27" s="113"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="114"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="115"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4493,19 +4530,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="112" t="s">
+      <c r="A35" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="113"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="114"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="114"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="114"/>
+      <c r="G35" s="114"/>
+      <c r="H35" s="114"/>
+      <c r="I35" s="114"/>
+      <c r="J35" s="114"/>
+      <c r="K35" s="115"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -4617,19 +4654,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
-      <c r="D43" s="113"/>
-      <c r="E43" s="113"/>
-      <c r="F43" s="113"/>
-      <c r="G43" s="113"/>
-      <c r="H43" s="113"/>
-      <c r="I43" s="113"/>
-      <c r="J43" s="113"/>
-      <c r="K43" s="114"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="114"/>
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114"/>
+      <c r="J43" s="114"/>
+      <c r="K43" s="115"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -4743,19 +4780,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="112" t="s">
+      <c r="A51" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="113"/>
-      <c r="C51" s="113"/>
-      <c r="D51" s="113"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="113"/>
-      <c r="G51" s="113"/>
-      <c r="H51" s="113"/>
-      <c r="I51" s="113"/>
-      <c r="J51" s="113"/>
-      <c r="K51" s="114"/>
+      <c r="B51" s="114"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="114"/>
+      <c r="H51" s="114"/>
+      <c r="I51" s="114"/>
+      <c r="J51" s="114"/>
+      <c r="K51" s="115"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -4875,19 +4912,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="112" t="s">
+      <c r="A59" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="113"/>
-      <c r="C59" s="113"/>
-      <c r="D59" s="113"/>
-      <c r="E59" s="113"/>
-      <c r="F59" s="113"/>
-      <c r="G59" s="113"/>
-      <c r="H59" s="113"/>
-      <c r="I59" s="113"/>
-      <c r="J59" s="113"/>
-      <c r="K59" s="114"/>
+      <c r="B59" s="114"/>
+      <c r="C59" s="114"/>
+      <c r="D59" s="114"/>
+      <c r="E59" s="114"/>
+      <c r="F59" s="114"/>
+      <c r="G59" s="114"/>
+      <c r="H59" s="114"/>
+      <c r="I59" s="114"/>
+      <c r="J59" s="114"/>
+      <c r="K59" s="115"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -4997,19 +5034,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="112" t="s">
+      <c r="A67" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="113"/>
-      <c r="C67" s="113"/>
-      <c r="D67" s="113"/>
-      <c r="E67" s="113"/>
-      <c r="F67" s="113"/>
-      <c r="G67" s="113"/>
-      <c r="H67" s="113"/>
-      <c r="I67" s="113"/>
-      <c r="J67" s="113"/>
-      <c r="K67" s="114"/>
+      <c r="B67" s="114"/>
+      <c r="C67" s="114"/>
+      <c r="D67" s="114"/>
+      <c r="E67" s="114"/>
+      <c r="F67" s="114"/>
+      <c r="G67" s="114"/>
+      <c r="H67" s="114"/>
+      <c r="I67" s="114"/>
+      <c r="J67" s="114"/>
+      <c r="K67" s="115"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5117,19 +5154,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="112" t="s">
+      <c r="A75" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="113"/>
-      <c r="C75" s="113"/>
-      <c r="D75" s="113"/>
-      <c r="E75" s="113"/>
-      <c r="F75" s="113"/>
-      <c r="G75" s="113"/>
-      <c r="H75" s="113"/>
-      <c r="I75" s="113"/>
-      <c r="J75" s="113"/>
-      <c r="K75" s="114"/>
+      <c r="B75" s="114"/>
+      <c r="C75" s="114"/>
+      <c r="D75" s="114"/>
+      <c r="E75" s="114"/>
+      <c r="F75" s="114"/>
+      <c r="G75" s="114"/>
+      <c r="H75" s="114"/>
+      <c r="I75" s="114"/>
+      <c r="J75" s="114"/>
+      <c r="K75" s="115"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5245,19 +5282,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="112" t="s">
+      <c r="A83" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="113"/>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="113"/>
-      <c r="F83" s="113"/>
-      <c r="G83" s="113"/>
-      <c r="H83" s="113"/>
-      <c r="I83" s="113"/>
-      <c r="J83" s="113"/>
-      <c r="K83" s="114"/>
+      <c r="B83" s="114"/>
+      <c r="C83" s="114"/>
+      <c r="D83" s="114"/>
+      <c r="E83" s="114"/>
+      <c r="F83" s="114"/>
+      <c r="G83" s="114"/>
+      <c r="H83" s="114"/>
+      <c r="I83" s="114"/>
+      <c r="J83" s="114"/>
+      <c r="K83" s="115"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5369,19 +5406,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="112" t="s">
+      <c r="A91" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="113"/>
-      <c r="C91" s="113"/>
-      <c r="D91" s="113"/>
-      <c r="E91" s="113"/>
-      <c r="F91" s="113"/>
-      <c r="G91" s="113"/>
-      <c r="H91" s="113"/>
-      <c r="I91" s="113"/>
-      <c r="J91" s="113"/>
-      <c r="K91" s="114"/>
+      <c r="B91" s="114"/>
+      <c r="C91" s="114"/>
+      <c r="D91" s="114"/>
+      <c r="E91" s="114"/>
+      <c r="F91" s="114"/>
+      <c r="G91" s="114"/>
+      <c r="H91" s="114"/>
+      <c r="I91" s="114"/>
+      <c r="J91" s="114"/>
+      <c r="K91" s="115"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5495,19 +5532,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="112" t="s">
+      <c r="A99" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="113"/>
-      <c r="C99" s="113"/>
-      <c r="D99" s="113"/>
-      <c r="E99" s="113"/>
-      <c r="F99" s="113"/>
-      <c r="G99" s="113"/>
-      <c r="H99" s="113"/>
-      <c r="I99" s="113"/>
-      <c r="J99" s="113"/>
-      <c r="K99" s="114"/>
+      <c r="B99" s="114"/>
+      <c r="C99" s="114"/>
+      <c r="D99" s="114"/>
+      <c r="E99" s="114"/>
+      <c r="F99" s="114"/>
+      <c r="G99" s="114"/>
+      <c r="H99" s="114"/>
+      <c r="I99" s="114"/>
+      <c r="J99" s="114"/>
+      <c r="K99" s="115"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -5611,19 +5648,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="112" t="s">
+      <c r="A107" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="113"/>
-      <c r="C107" s="113"/>
-      <c r="D107" s="113"/>
-      <c r="E107" s="113"/>
-      <c r="F107" s="113"/>
-      <c r="G107" s="113"/>
-      <c r="H107" s="113"/>
-      <c r="I107" s="113"/>
-      <c r="J107" s="113"/>
-      <c r="K107" s="114"/>
+      <c r="B107" s="114"/>
+      <c r="C107" s="114"/>
+      <c r="D107" s="114"/>
+      <c r="E107" s="114"/>
+      <c r="F107" s="114"/>
+      <c r="G107" s="114"/>
+      <c r="H107" s="114"/>
+      <c r="I107" s="114"/>
+      <c r="J107" s="114"/>
+      <c r="K107" s="115"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -5728,24 +5765,24 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -5960,7 +5997,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -5987,10 +6024,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="120"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6001,7 +6038,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="122" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6015,7 +6052,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6027,7 +6064,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6036,7 +6073,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6048,7 +6085,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6060,7 +6097,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6069,7 +6106,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="123"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6084,7 +6121,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="122" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6098,7 +6135,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6110,7 +6147,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6119,7 +6156,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6131,7 +6168,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6143,7 +6180,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="122"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6152,7 +6189,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="123"/>
+      <c r="A17" s="124"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6167,7 +6204,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="122" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6176,7 +6213,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="122"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6186,14 +6223,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="122"/>
+      <c r="A21" s="123"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="122"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6203,7 +6240,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="122"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6213,14 +6250,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="122"/>
+      <c r="A24" s="123"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="123"/>
+      <c r="A25" s="124"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6233,7 +6270,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6264,17 +6301,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="141"/>
+      <c r="B2" s="132"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="141"/>
+      <c r="B3" s="132"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
@@ -6290,115 +6327,128 @@
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="128" t="s">
+      <c r="A7" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="129"/>
+      <c r="B7" s="143"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="130" t="s">
+      <c r="A9" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="131"/>
+      <c r="B9" s="141"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="132"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="128"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="125"/>
+      <c r="B11" s="130"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="129" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="125"/>
+      <c r="B12" s="130"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="125"/>
+      <c r="B13" s="130"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="125"/>
+      <c r="B14" s="130"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="125"/>
+      <c r="B15" s="130"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="125"/>
+      <c r="B16" s="130"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="127"/>
+      <c r="B17" s="126"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="128" t="s">
+      <c r="A19" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="129"/>
+      <c r="B19" s="143"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="130" t="s">
+      <c r="A21" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="131"/>
+      <c r="B21" s="141"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="132"/>
-      <c r="B22" s="133"/>
+      <c r="A22" s="127"/>
+      <c r="B22" s="128"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="125"/>
+      <c r="B23" s="130"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="124"/>
-      <c r="B24" s="125"/>
+      <c r="A24" s="129"/>
+      <c r="B24" s="130"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="125"/>
+      <c r="B25" s="130"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="125"/>
+      <c r="B26" s="130"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="126"/>
-      <c r="B27" s="127"/>
+      <c r="A27" s="125"/>
+      <c r="B27" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -6409,19 +6459,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - some redoing of level 3 by Cardboard, no longer stuck
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="123">
   <si>
     <t>Notes</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Down ladder</t>
+  </si>
+  <si>
+    <t>X = 1710</t>
   </si>
 </sst>
 </file>
@@ -1399,17 +1402,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1423,6 +1417,18 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1455,52 +1461,49 @@
     <xf numFmtId="0" fontId="32" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Färg1" xfId="2" builtinId="29"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Total" xfId="1" builtinId="25"/>
+    <cellStyle name="Summa" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1515,7 +1518,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1802,7 +1805,7 @@
   <dimension ref="B1:O148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1816,16 +1819,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="108" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="109"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="106"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
         <f>SUM(H1:H65530)</f>
@@ -1903,10 +1906,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="110"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -1943,7 +1946,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="108" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1963,7 +1966,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="112"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="112"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -1984,7 +1987,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="112"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -1995,7 +1998,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="112"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2006,7 +2009,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="112"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2017,7 +2020,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="112"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2028,7 +2031,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="112"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2039,7 +2042,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="112"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2082,7 +2085,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="110" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2117,7 +2120,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="106"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2150,7 +2153,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="106"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2183,7 +2186,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="106"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2216,7 +2219,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="106"/>
+      <c r="B23" s="111"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2249,7 +2252,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="106"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2285,7 +2288,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="106"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2318,7 +2321,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="106"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2351,7 +2354,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="106"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2384,7 +2387,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="106"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2417,7 +2420,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="106"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2443,7 +2446,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="103" t="s">
+      <c r="B31" s="112" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2478,7 +2481,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="104"/>
+      <c r="B32" s="113"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2507,7 +2510,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="104"/>
+      <c r="B33" s="113"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2536,7 +2539,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="104"/>
+      <c r="B34" s="113"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2566,7 +2569,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="104"/>
+      <c r="B35" s="113"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2586,7 +2589,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="104"/>
+      <c r="B36" s="113"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2606,7 +2609,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="104"/>
+      <c r="B37" s="113"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2629,7 +2632,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="104"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2652,7 +2655,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="104"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2720,7 +2723,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="110" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2740,7 +2743,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="106"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2757,7 +2760,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="106"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2774,7 +2777,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="106"/>
+      <c r="B46" s="111"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2792,52 +2795,58 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="106"/>
-      <c r="C47" s="144" t="s">
+      <c r="B47" s="111"/>
+      <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
       <c r="D47" s="30">
-        <v>10271</v>
+        <v>10260</v>
       </c>
       <c r="E47" s="30">
         <v>11097</v>
       </c>
       <c r="F47" s="52">
         <f t="shared" si="4"/>
-        <v>826</v>
+        <v>837</v>
       </c>
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="106"/>
-      <c r="C48" s="144" t="s">
+      <c r="B48" s="111"/>
+      <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
       <c r="D48" s="30">
-        <v>10785</v>
+        <v>10712</v>
       </c>
       <c r="E48" s="30">
         <v>11600</v>
       </c>
       <c r="F48" s="52">
         <f t="shared" si="4"/>
-        <v>815</v>
+        <v>888</v>
       </c>
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:8" ht="15">
-      <c r="B49" s="106"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="103" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="30">
+        <v>10897</v>
+      </c>
+      <c r="E49" s="30">
+        <v>11788</v>
+      </c>
       <c r="F49" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>891</v>
       </c>
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:8" ht="15">
-      <c r="B50" s="106"/>
+      <c r="B50" s="111"/>
       <c r="C50" s="29"/>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -2848,7 +2857,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:8" ht="15">
-      <c r="B51" s="106"/>
+      <c r="B51" s="111"/>
       <c r="C51" s="29"/>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
@@ -2859,7 +2868,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:8" ht="15">
-      <c r="B52" s="106"/>
+      <c r="B52" s="111"/>
       <c r="C52" s="29"/>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -2870,7 +2879,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:8" ht="15">
-      <c r="B53" s="106"/>
+      <c r="B53" s="111"/>
       <c r="C53" s="29"/>
       <c r="D53" s="30"/>
       <c r="E53" s="30"/>
@@ -2881,7 +2890,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:8" ht="15">
-      <c r="B54" s="106"/>
+      <c r="B54" s="111"/>
       <c r="C54" s="29"/>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
@@ -2892,7 +2901,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:8" ht="15">
-      <c r="B55" s="106"/>
+      <c r="B55" s="111"/>
       <c r="C55" s="29"/>
       <c r="D55" s="30"/>
       <c r="E55" s="30"/>
@@ -2903,7 +2912,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:8" ht="15">
-      <c r="B56" s="106"/>
+      <c r="B56" s="111"/>
       <c r="C56" s="29"/>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
@@ -2914,7 +2923,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B57" s="106"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="27" t="s">
         <v>32</v>
       </c>
@@ -2949,7 +2958,7 @@
     </row>
     <row r="59" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="60" spans="2:8" ht="15">
-      <c r="B60" s="103" t="s">
+      <c r="B60" s="112" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="42" t="s">
@@ -2969,7 +2978,7 @@
       </c>
     </row>
     <row r="61" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B61" s="104"/>
+      <c r="B61" s="113"/>
       <c r="C61" s="27" t="s">
         <v>29</v>
       </c>
@@ -2982,7 +2991,7 @@
       <c r="G61" s="33"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B62" s="104"/>
+      <c r="B62" s="113"/>
       <c r="C62" s="29"/>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -2993,7 +3002,7 @@
       <c r="G62" s="34"/>
     </row>
     <row r="63" spans="2:8" ht="15">
-      <c r="B63" s="104"/>
+      <c r="B63" s="113"/>
       <c r="C63" s="29"/>
       <c r="D63" s="30"/>
       <c r="E63" s="30"/>
@@ -3005,7 +3014,7 @@
       <c r="H63" s="41"/>
     </row>
     <row r="64" spans="2:8" ht="15">
-      <c r="B64" s="104"/>
+      <c r="B64" s="113"/>
       <c r="C64" s="29"/>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -3016,7 +3025,7 @@
       <c r="G64" s="34"/>
     </row>
     <row r="65" spans="2:8" ht="15" customHeight="1">
-      <c r="B65" s="104"/>
+      <c r="B65" s="113"/>
       <c r="C65" s="29"/>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
@@ -3027,7 +3036,7 @@
       <c r="G65" s="34"/>
     </row>
     <row r="66" spans="2:8" ht="15">
-      <c r="B66" s="104"/>
+      <c r="B66" s="113"/>
       <c r="C66" s="29"/>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -3038,7 +3047,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="104"/>
+      <c r="B67" s="113"/>
       <c r="C67" s="29"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -3049,7 +3058,7 @@
       <c r="G67" s="34"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="104"/>
+      <c r="B68" s="113"/>
       <c r="C68" s="29"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -3060,7 +3069,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15">
-      <c r="B69" s="104"/>
+      <c r="B69" s="113"/>
       <c r="C69" s="29"/>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -3071,7 +3080,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="104"/>
+      <c r="B70" s="113"/>
       <c r="C70" s="29"/>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -3082,7 +3091,7 @@
       <c r="G70" s="34"/>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="104"/>
+      <c r="B71" s="113"/>
       <c r="C71" s="29"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -3093,7 +3102,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="104"/>
+      <c r="B72" s="113"/>
       <c r="C72" s="29"/>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3104,7 +3113,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="104"/>
+      <c r="B73" s="113"/>
       <c r="C73" s="29"/>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3115,7 +3124,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B74" s="104"/>
+      <c r="B74" s="113"/>
       <c r="C74" s="27" t="s">
         <v>32</v>
       </c>
@@ -3150,7 +3159,7 @@
     </row>
     <row r="76" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="105" t="s">
+      <c r="B77" s="110" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="38" t="s">
@@ -3170,7 +3179,7 @@
       </c>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="106"/>
+      <c r="B78" s="111"/>
       <c r="C78" s="27" t="s">
         <v>29</v>
       </c>
@@ -3183,7 +3192,7 @@
       <c r="G78" s="33"/>
     </row>
     <row r="79" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B79" s="106"/>
+      <c r="B79" s="111"/>
       <c r="C79" s="29"/>
       <c r="D79" s="30"/>
       <c r="E79" s="30"/>
@@ -3194,7 +3203,7 @@
       <c r="G79" s="34"/>
     </row>
     <row r="80" spans="2:8" ht="15">
-      <c r="B80" s="106"/>
+      <c r="B80" s="111"/>
       <c r="C80" s="29"/>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -3206,7 +3215,7 @@
       <c r="H80" s="41"/>
     </row>
     <row r="81" spans="2:7" ht="15">
-      <c r="B81" s="106"/>
+      <c r="B81" s="111"/>
       <c r="C81" s="29"/>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
@@ -3217,7 +3226,7 @@
       <c r="G81" s="34"/>
     </row>
     <row r="82" spans="2:7" ht="15" customHeight="1">
-      <c r="B82" s="106"/>
+      <c r="B82" s="111"/>
       <c r="C82" s="29"/>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -3228,7 +3237,7 @@
       <c r="G82" s="34"/>
     </row>
     <row r="83" spans="2:7" ht="15">
-      <c r="B83" s="106"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="29"/>
       <c r="D83" s="30"/>
       <c r="E83" s="30"/>
@@ -3239,7 +3248,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:7" ht="15">
-      <c r="B84" s="106"/>
+      <c r="B84" s="111"/>
       <c r="C84" s="29"/>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
@@ -3250,7 +3259,7 @@
       <c r="G84" s="34"/>
     </row>
     <row r="85" spans="2:7" ht="15">
-      <c r="B85" s="106"/>
+      <c r="B85" s="111"/>
       <c r="C85" s="29"/>
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
@@ -3261,7 +3270,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:7" ht="15">
-      <c r="B86" s="106"/>
+      <c r="B86" s="111"/>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -3272,7 +3281,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:7" ht="15">
-      <c r="B87" s="106"/>
+      <c r="B87" s="111"/>
       <c r="C87" s="29"/>
       <c r="D87" s="30"/>
       <c r="E87" s="30"/>
@@ -3283,7 +3292,7 @@
       <c r="G87" s="34"/>
     </row>
     <row r="88" spans="2:7" ht="15">
-      <c r="B88" s="106"/>
+      <c r="B88" s="111"/>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -3294,7 +3303,7 @@
       <c r="G88" s="34"/>
     </row>
     <row r="89" spans="2:7" ht="15">
-      <c r="B89" s="106"/>
+      <c r="B89" s="111"/>
       <c r="C89" s="29"/>
       <c r="D89" s="30"/>
       <c r="E89" s="30"/>
@@ -3305,7 +3314,7 @@
       <c r="G89" s="34"/>
     </row>
     <row r="90" spans="2:7" ht="15">
-      <c r="B90" s="106"/>
+      <c r="B90" s="111"/>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -3316,7 +3325,7 @@
       <c r="G90" s="34"/>
     </row>
     <row r="91" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B91" s="106"/>
+      <c r="B91" s="111"/>
       <c r="C91" s="27" t="s">
         <v>32</v>
       </c>
@@ -3351,7 +3360,7 @@
     </row>
     <row r="93" spans="2:7" ht="13.5" thickBot="1"/>
     <row r="94" spans="2:7" ht="15">
-      <c r="B94" s="103" t="s">
+      <c r="B94" s="112" t="s">
         <v>18</v>
       </c>
       <c r="C94" s="42" t="s">
@@ -3371,7 +3380,7 @@
       </c>
     </row>
     <row r="95" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B95" s="104"/>
+      <c r="B95" s="113"/>
       <c r="C95" s="27" t="s">
         <v>29</v>
       </c>
@@ -3384,7 +3393,7 @@
       <c r="G95" s="33"/>
     </row>
     <row r="96" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B96" s="104"/>
+      <c r="B96" s="113"/>
       <c r="C96" s="29"/>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
@@ -3395,7 +3404,7 @@
       <c r="G96" s="34"/>
     </row>
     <row r="97" spans="2:8" ht="15">
-      <c r="B97" s="104"/>
+      <c r="B97" s="113"/>
       <c r="C97" s="29"/>
       <c r="D97" s="30"/>
       <c r="E97" s="30"/>
@@ -3407,7 +3416,7 @@
       <c r="H97" s="41"/>
     </row>
     <row r="98" spans="2:8" ht="15">
-      <c r="B98" s="104"/>
+      <c r="B98" s="113"/>
       <c r="C98" s="29"/>
       <c r="D98" s="30"/>
       <c r="E98" s="30"/>
@@ -3418,7 +3427,7 @@
       <c r="G98" s="34"/>
     </row>
     <row r="99" spans="2:8" ht="15" customHeight="1">
-      <c r="B99" s="104"/>
+      <c r="B99" s="113"/>
       <c r="C99" s="29"/>
       <c r="D99" s="30"/>
       <c r="E99" s="30"/>
@@ -3429,7 +3438,7 @@
       <c r="G99" s="34"/>
     </row>
     <row r="100" spans="2:8" ht="15">
-      <c r="B100" s="104"/>
+      <c r="B100" s="113"/>
       <c r="C100" s="29"/>
       <c r="D100" s="30"/>
       <c r="E100" s="30"/>
@@ -3440,7 +3449,7 @@
       <c r="G100" s="34"/>
     </row>
     <row r="101" spans="2:8" ht="15">
-      <c r="B101" s="104"/>
+      <c r="B101" s="113"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
@@ -3451,7 +3460,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="104"/>
+      <c r="B102" s="113"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -3462,7 +3471,7 @@
       <c r="G102" s="34"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="104"/>
+      <c r="B103" s="113"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
       <c r="E103" s="30"/>
@@ -3473,7 +3482,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15">
-      <c r="B104" s="104"/>
+      <c r="B104" s="113"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -3484,7 +3493,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="104"/>
+      <c r="B105" s="113"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
       <c r="E105" s="30"/>
@@ -3495,7 +3504,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="104"/>
+      <c r="B106" s="113"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -3506,7 +3515,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="104"/>
+      <c r="B107" s="113"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
@@ -3517,7 +3526,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B108" s="104"/>
+      <c r="B108" s="113"/>
       <c r="C108" s="27" t="s">
         <v>32</v>
       </c>
@@ -3552,7 +3561,7 @@
     </row>
     <row r="110" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="105" t="s">
+      <c r="B111" s="110" t="s">
         <v>19</v>
       </c>
       <c r="C111" s="38" t="s">
@@ -3572,7 +3581,7 @@
       </c>
     </row>
     <row r="112" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B112" s="106"/>
+      <c r="B112" s="111"/>
       <c r="C112" s="27" t="s">
         <v>29</v>
       </c>
@@ -3585,7 +3594,7 @@
       <c r="G112" s="33"/>
     </row>
     <row r="113" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B113" s="106"/>
+      <c r="B113" s="111"/>
       <c r="C113" s="29"/>
       <c r="D113" s="30"/>
       <c r="E113" s="30"/>
@@ -3596,7 +3605,7 @@
       <c r="G113" s="34"/>
     </row>
     <row r="114" spans="2:8" ht="15">
-      <c r="B114" s="106"/>
+      <c r="B114" s="111"/>
       <c r="C114" s="29"/>
       <c r="D114" s="30"/>
       <c r="E114" s="30"/>
@@ -3608,7 +3617,7 @@
       <c r="H114" s="41"/>
     </row>
     <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="106"/>
+      <c r="B115" s="111"/>
       <c r="C115" s="29"/>
       <c r="D115" s="30"/>
       <c r="E115" s="30"/>
@@ -3619,7 +3628,7 @@
       <c r="G115" s="34"/>
     </row>
     <row r="116" spans="2:8" ht="15" customHeight="1">
-      <c r="B116" s="106"/>
+      <c r="B116" s="111"/>
       <c r="C116" s="29"/>
       <c r="D116" s="30"/>
       <c r="E116" s="30"/>
@@ -3630,7 +3639,7 @@
       <c r="G116" s="34"/>
     </row>
     <row r="117" spans="2:8" ht="15">
-      <c r="B117" s="106"/>
+      <c r="B117" s="111"/>
       <c r="C117" s="29"/>
       <c r="D117" s="30"/>
       <c r="E117" s="30"/>
@@ -3641,7 +3650,7 @@
       <c r="G117" s="34"/>
     </row>
     <row r="118" spans="2:8" ht="15">
-      <c r="B118" s="106"/>
+      <c r="B118" s="111"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -3652,7 +3661,7 @@
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:8" ht="15">
-      <c r="B119" s="106"/>
+      <c r="B119" s="111"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
@@ -3663,7 +3672,7 @@
       <c r="G119" s="34"/>
     </row>
     <row r="120" spans="2:8" ht="15">
-      <c r="B120" s="106"/>
+      <c r="B120" s="111"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -3674,7 +3683,7 @@
       <c r="G120" s="34"/>
     </row>
     <row r="121" spans="2:8" ht="15">
-      <c r="B121" s="106"/>
+      <c r="B121" s="111"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
@@ -3685,7 +3694,7 @@
       <c r="G121" s="34"/>
     </row>
     <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="106"/>
+      <c r="B122" s="111"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -3696,7 +3705,7 @@
       <c r="G122" s="34"/>
     </row>
     <row r="123" spans="2:8" ht="15">
-      <c r="B123" s="106"/>
+      <c r="B123" s="111"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
@@ -3707,7 +3716,7 @@
       <c r="G123" s="34"/>
     </row>
     <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="106"/>
+      <c r="B124" s="111"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -3718,7 +3727,7 @@
       <c r="G124" s="34"/>
     </row>
     <row r="125" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B125" s="106"/>
+      <c r="B125" s="111"/>
       <c r="C125" s="27" t="s">
         <v>32</v>
       </c>
@@ -3753,7 +3762,7 @@
     </row>
     <row r="127" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="103" t="s">
+      <c r="B128" s="112" t="s">
         <v>20</v>
       </c>
       <c r="C128" s="42" t="s">
@@ -3773,7 +3782,7 @@
       </c>
     </row>
     <row r="129" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B129" s="104"/>
+      <c r="B129" s="113"/>
       <c r="C129" s="27" t="s">
         <v>29</v>
       </c>
@@ -3786,7 +3795,7 @@
       <c r="G129" s="33"/>
     </row>
     <row r="130" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B130" s="104"/>
+      <c r="B130" s="113"/>
       <c r="C130" s="29"/>
       <c r="D130" s="30"/>
       <c r="E130" s="30"/>
@@ -3797,7 +3806,7 @@
       <c r="G130" s="34"/>
     </row>
     <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="104"/>
+      <c r="B131" s="113"/>
       <c r="C131" s="29"/>
       <c r="D131" s="30"/>
       <c r="E131" s="30"/>
@@ -3809,7 +3818,7 @@
       <c r="H131" s="41"/>
     </row>
     <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="104"/>
+      <c r="B132" s="113"/>
       <c r="C132" s="29"/>
       <c r="D132" s="30"/>
       <c r="E132" s="30"/>
@@ -3820,7 +3829,7 @@
       <c r="G132" s="34"/>
     </row>
     <row r="133" spans="2:8" ht="15" customHeight="1">
-      <c r="B133" s="104"/>
+      <c r="B133" s="113"/>
       <c r="C133" s="29"/>
       <c r="D133" s="30"/>
       <c r="E133" s="30"/>
@@ -3831,7 +3840,7 @@
       <c r="G133" s="34"/>
     </row>
     <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="104"/>
+      <c r="B134" s="113"/>
       <c r="C134" s="29"/>
       <c r="D134" s="30"/>
       <c r="E134" s="30"/>
@@ -3842,7 +3851,7 @@
       <c r="G134" s="34"/>
     </row>
     <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="104"/>
+      <c r="B135" s="113"/>
       <c r="C135" s="29"/>
       <c r="D135" s="30"/>
       <c r="E135" s="30"/>
@@ -3853,7 +3862,7 @@
       <c r="G135" s="34"/>
     </row>
     <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="104"/>
+      <c r="B136" s="113"/>
       <c r="C136" s="29"/>
       <c r="D136" s="30"/>
       <c r="E136" s="30"/>
@@ -3864,7 +3873,7 @@
       <c r="G136" s="34"/>
     </row>
     <row r="137" spans="2:8" ht="15">
-      <c r="B137" s="104"/>
+      <c r="B137" s="113"/>
       <c r="C137" s="29"/>
       <c r="D137" s="30"/>
       <c r="E137" s="30"/>
@@ -3875,7 +3884,7 @@
       <c r="G137" s="34"/>
     </row>
     <row r="138" spans="2:8" ht="15">
-      <c r="B138" s="104"/>
+      <c r="B138" s="113"/>
       <c r="C138" s="29"/>
       <c r="D138" s="30"/>
       <c r="E138" s="30"/>
@@ -3886,7 +3895,7 @@
       <c r="G138" s="34"/>
     </row>
     <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="104"/>
+      <c r="B139" s="113"/>
       <c r="C139" s="29"/>
       <c r="D139" s="30"/>
       <c r="E139" s="30"/>
@@ -3897,7 +3906,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:8" ht="15">
-      <c r="B140" s="104"/>
+      <c r="B140" s="113"/>
       <c r="C140" s="29"/>
       <c r="D140" s="30"/>
       <c r="E140" s="30"/>
@@ -3908,7 +3917,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:8" ht="15">
-      <c r="B141" s="104"/>
+      <c r="B141" s="113"/>
       <c r="C141" s="29"/>
       <c r="D141" s="30"/>
       <c r="E141" s="30"/>
@@ -3919,7 +3928,7 @@
       <c r="G141" s="34"/>
     </row>
     <row r="142" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B142" s="104"/>
+      <c r="B142" s="113"/>
       <c r="C142" s="27" t="s">
         <v>32</v>
       </c>
@@ -3957,18 +3966,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B128:B142"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B43:B57"/>
+    <mergeCell ref="B60:B74"/>
+    <mergeCell ref="B77:B91"/>
+    <mergeCell ref="B94:B108"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
     <mergeCell ref="B111:B125"/>
     <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B128:B142"/>
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B43:B57"/>
-    <mergeCell ref="B60:B74"/>
-    <mergeCell ref="B77:B91"/>
-    <mergeCell ref="B94:B108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3984,8 +3993,8 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3994,51 +4003,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="119"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="115"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="116"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4152,19 +4161,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="113" t="s">
+      <c r="A11" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="114"/>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="114"/>
-      <c r="K11" s="115"/>
+      <c r="B11" s="115"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="116"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4278,19 +4287,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="114"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="114"/>
-      <c r="K19" s="115"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="115"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="116"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4404,19 +4413,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="113" t="s">
+      <c r="A27" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="115"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="116"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4530,19 +4539,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="113" t="s">
+      <c r="A35" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="114"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="114"/>
-      <c r="G35" s="114"/>
-      <c r="H35" s="114"/>
-      <c r="I35" s="114"/>
-      <c r="J35" s="114"/>
-      <c r="K35" s="115"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="115"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="115"/>
+      <c r="G35" s="115"/>
+      <c r="H35" s="115"/>
+      <c r="I35" s="115"/>
+      <c r="J35" s="115"/>
+      <c r="K35" s="116"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -4654,19 +4663,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="113" t="s">
+      <c r="A43" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="115"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="115"/>
+      <c r="G43" s="115"/>
+      <c r="H43" s="115"/>
+      <c r="I43" s="115"/>
+      <c r="J43" s="115"/>
+      <c r="K43" s="116"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -4780,19 +4789,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="113" t="s">
+      <c r="A51" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="114"/>
-      <c r="C51" s="114"/>
-      <c r="D51" s="114"/>
-      <c r="E51" s="114"/>
-      <c r="F51" s="114"/>
-      <c r="G51" s="114"/>
-      <c r="H51" s="114"/>
-      <c r="I51" s="114"/>
-      <c r="J51" s="114"/>
-      <c r="K51" s="115"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="115"/>
+      <c r="E51" s="115"/>
+      <c r="F51" s="115"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="115"/>
+      <c r="J51" s="115"/>
+      <c r="K51" s="116"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -4912,19 +4921,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="113" t="s">
+      <c r="A59" s="114" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="114"/>
-      <c r="C59" s="114"/>
-      <c r="D59" s="114"/>
-      <c r="E59" s="114"/>
-      <c r="F59" s="114"/>
-      <c r="G59" s="114"/>
-      <c r="H59" s="114"/>
-      <c r="I59" s="114"/>
-      <c r="J59" s="114"/>
-      <c r="K59" s="115"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="115"/>
+      <c r="G59" s="115"/>
+      <c r="H59" s="115"/>
+      <c r="I59" s="115"/>
+      <c r="J59" s="115"/>
+      <c r="K59" s="116"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -5034,19 +5043,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="113" t="s">
+      <c r="A67" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="114"/>
-      <c r="C67" s="114"/>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114"/>
-      <c r="F67" s="114"/>
-      <c r="G67" s="114"/>
-      <c r="H67" s="114"/>
-      <c r="I67" s="114"/>
-      <c r="J67" s="114"/>
-      <c r="K67" s="115"/>
+      <c r="B67" s="115"/>
+      <c r="C67" s="115"/>
+      <c r="D67" s="115"/>
+      <c r="E67" s="115"/>
+      <c r="F67" s="115"/>
+      <c r="G67" s="115"/>
+      <c r="H67" s="115"/>
+      <c r="I67" s="115"/>
+      <c r="J67" s="115"/>
+      <c r="K67" s="116"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5154,19 +5163,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="113" t="s">
+      <c r="A75" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="114"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="114"/>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
-      <c r="G75" s="114"/>
-      <c r="H75" s="114"/>
-      <c r="I75" s="114"/>
-      <c r="J75" s="114"/>
-      <c r="K75" s="115"/>
+      <c r="B75" s="115"/>
+      <c r="C75" s="115"/>
+      <c r="D75" s="115"/>
+      <c r="E75" s="115"/>
+      <c r="F75" s="115"/>
+      <c r="G75" s="115"/>
+      <c r="H75" s="115"/>
+      <c r="I75" s="115"/>
+      <c r="J75" s="115"/>
+      <c r="K75" s="116"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5282,19 +5291,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="113" t="s">
+      <c r="A83" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="114"/>
-      <c r="C83" s="114"/>
-      <c r="D83" s="114"/>
-      <c r="E83" s="114"/>
-      <c r="F83" s="114"/>
-      <c r="G83" s="114"/>
-      <c r="H83" s="114"/>
-      <c r="I83" s="114"/>
-      <c r="J83" s="114"/>
-      <c r="K83" s="115"/>
+      <c r="B83" s="115"/>
+      <c r="C83" s="115"/>
+      <c r="D83" s="115"/>
+      <c r="E83" s="115"/>
+      <c r="F83" s="115"/>
+      <c r="G83" s="115"/>
+      <c r="H83" s="115"/>
+      <c r="I83" s="115"/>
+      <c r="J83" s="115"/>
+      <c r="K83" s="116"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5406,19 +5415,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="113" t="s">
+      <c r="A91" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="114"/>
-      <c r="C91" s="114"/>
-      <c r="D91" s="114"/>
-      <c r="E91" s="114"/>
-      <c r="F91" s="114"/>
-      <c r="G91" s="114"/>
-      <c r="H91" s="114"/>
-      <c r="I91" s="114"/>
-      <c r="J91" s="114"/>
-      <c r="K91" s="115"/>
+      <c r="B91" s="115"/>
+      <c r="C91" s="115"/>
+      <c r="D91" s="115"/>
+      <c r="E91" s="115"/>
+      <c r="F91" s="115"/>
+      <c r="G91" s="115"/>
+      <c r="H91" s="115"/>
+      <c r="I91" s="115"/>
+      <c r="J91" s="115"/>
+      <c r="K91" s="116"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5532,19 +5541,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="113" t="s">
+      <c r="A99" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="114"/>
-      <c r="C99" s="114"/>
-      <c r="D99" s="114"/>
-      <c r="E99" s="114"/>
-      <c r="F99" s="114"/>
-      <c r="G99" s="114"/>
-      <c r="H99" s="114"/>
-      <c r="I99" s="114"/>
-      <c r="J99" s="114"/>
-      <c r="K99" s="115"/>
+      <c r="B99" s="115"/>
+      <c r="C99" s="115"/>
+      <c r="D99" s="115"/>
+      <c r="E99" s="115"/>
+      <c r="F99" s="115"/>
+      <c r="G99" s="115"/>
+      <c r="H99" s="115"/>
+      <c r="I99" s="115"/>
+      <c r="J99" s="115"/>
+      <c r="K99" s="116"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -5648,19 +5657,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="113" t="s">
+      <c r="A107" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="114"/>
-      <c r="C107" s="114"/>
-      <c r="D107" s="114"/>
-      <c r="E107" s="114"/>
-      <c r="F107" s="114"/>
-      <c r="G107" s="114"/>
-      <c r="H107" s="114"/>
-      <c r="I107" s="114"/>
-      <c r="J107" s="114"/>
-      <c r="K107" s="115"/>
+      <c r="B107" s="115"/>
+      <c r="C107" s="115"/>
+      <c r="D107" s="115"/>
+      <c r="E107" s="115"/>
+      <c r="F107" s="115"/>
+      <c r="G107" s="115"/>
+      <c r="H107" s="115"/>
+      <c r="I107" s="115"/>
+      <c r="J107" s="115"/>
+      <c r="K107" s="116"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -5765,22 +5774,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6024,10 +6033,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="121"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6038,7 +6047,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="123" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6052,7 +6061,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="123"/>
+      <c r="A4" s="124"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6064,7 +6073,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="123"/>
+      <c r="A5" s="124"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6073,7 +6082,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="123"/>
+      <c r="A6" s="124"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6085,7 +6094,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="123"/>
+      <c r="A7" s="124"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6097,7 +6106,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="123"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6106,7 +6115,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="124"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6121,7 +6130,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="123" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6135,7 +6144,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="123"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6147,7 +6156,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="123"/>
+      <c r="A13" s="124"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6156,7 +6165,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="123"/>
+      <c r="A14" s="124"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6168,7 +6177,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="123"/>
+      <c r="A15" s="124"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6180,7 +6189,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="123"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6189,7 +6198,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="124"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6204,7 +6213,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="123" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6213,7 +6222,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="123"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6223,14 +6232,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="123"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="123"/>
+      <c r="A22" s="124"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6240,7 +6249,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="123"/>
+      <c r="A23" s="124"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6250,14 +6259,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="123"/>
+      <c r="A24" s="124"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="124"/>
+      <c r="A25" s="125"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6292,163 +6301,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="135"/>
+      <c r="B1" s="137"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="132"/>
+      <c r="B3" s="143"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="138"/>
-      <c r="B4" s="139"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="141"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="137"/>
+      <c r="B5" s="139"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="143"/>
+      <c r="B7" s="131"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="132" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="141"/>
+      <c r="B9" s="133"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="127"/>
-      <c r="B10" s="128"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="135"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="130"/>
+      <c r="B11" s="127"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="127"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="130"/>
+      <c r="B13" s="127"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="129" t="s">
+      <c r="A14" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="130"/>
+      <c r="B14" s="127"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="130"/>
+      <c r="B15" s="127"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="130"/>
+      <c r="B16" s="127"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="125" t="s">
+      <c r="A17" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="126"/>
+      <c r="B17" s="129"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="142" t="s">
+      <c r="A19" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="143"/>
+      <c r="B19" s="131"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="140" t="s">
+      <c r="A21" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="141"/>
+      <c r="B21" s="133"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="128"/>
+      <c r="A22" s="134"/>
+      <c r="B22" s="135"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="130"/>
+      <c r="B23" s="127"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="129"/>
-      <c r="B24" s="130"/>
+      <c r="A24" s="126"/>
+      <c r="B24" s="127"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="129" t="s">
+      <c r="A25" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="130"/>
+      <c r="B25" s="127"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="129" t="s">
+      <c r="A26" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="130"/>
+      <c r="B26" s="127"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="125"/>
-      <c r="B27" s="126"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -6459,6 +6455,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - Level 3 done
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="133">
   <si>
     <t>Notes</t>
   </si>
@@ -510,6 +510,36 @@
   <si>
     <t>X = 1710</t>
   </si>
+  <si>
+    <t>X = 2401</t>
+  </si>
+  <si>
+    <t>X=2821</t>
+  </si>
+  <si>
+    <t>X=2978(going left)</t>
+  </si>
+  <si>
+    <t>X=2702</t>
+  </si>
+  <si>
+    <t>X=2536(top)</t>
+  </si>
+  <si>
+    <t>Begin down elevator</t>
+  </si>
+  <si>
+    <t>X = 4593</t>
+  </si>
+  <si>
+    <t>End level</t>
+  </si>
+  <si>
+    <t>After level stats</t>
+  </si>
+  <si>
+    <t>Begin = Kyle appears</t>
+  </si>
 </sst>
 </file>
 
@@ -519,10 +549,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1211,14 +1248,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1226,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1234,75 +1271,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,10 +1349,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1336,174 +1373,177 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Färg1" xfId="2" builtinId="29"/>
-    <cellStyle name="Hyperlänk" xfId="3" builtinId="8"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Summa" xfId="1" builtinId="25"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,7 +1558,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1802,15 +1842,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O148"/>
+  <dimension ref="B1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="6.5703125" customWidth="1"/>
@@ -1819,19 +1859,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="108"/>
+      <c r="D1" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="106"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="110"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
-        <f>SUM(H1:H65530)</f>
+        <f>SUM(H1:H65534)</f>
         <v>225</v>
       </c>
       <c r="J1" s="71" t="s">
@@ -1906,10 +1946,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="107"/>
+      <c r="E5" s="111"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -1946,7 +1986,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="112" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1966,7 +2006,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="109"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -1976,7 +2016,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="109"/>
+      <c r="B10" s="113"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -1987,7 +2027,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="109"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -1998,7 +2038,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="109"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2009,7 +2049,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="109"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2020,7 +2060,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="109"/>
+      <c r="B14" s="113"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2031,7 +2071,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="109"/>
+      <c r="B15" s="113"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2042,7 +2082,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="109"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2085,7 +2125,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="106" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2120,7 +2160,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="111"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2153,7 +2193,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="111"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2186,7 +2226,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="111"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2219,7 +2259,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="111"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2252,7 +2292,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="111"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2288,7 +2328,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="111"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2321,7 +2361,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="111"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2354,7 +2394,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="111"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2387,7 +2427,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="111"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2420,7 +2460,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="111"/>
+      <c r="B29" s="107"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2446,7 +2486,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="112" t="s">
+      <c r="B31" s="104" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2481,7 +2521,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="113"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2510,7 +2550,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="113"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2539,7 +2579,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="113"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2569,7 +2609,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="113"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2589,7 +2629,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="113"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2609,7 +2649,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="113"/>
+      <c r="B37" s="105"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2632,7 +2672,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="113"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2655,7 +2695,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="113"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2723,7 +2763,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="110" t="s">
+      <c r="B43" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2743,7 +2783,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="111"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2754,13 +2794,13 @@
         <v>9816</v>
       </c>
       <c r="F44" s="52">
-        <f t="shared" ref="F44:F57" si="4">IF(AND(D44&gt;0,E44&gt;0), E44-D44, 0)</f>
+        <f t="shared" ref="F44:F61" si="4">IF(AND(D44&gt;0,E44&gt;0), E44-D44, 0)</f>
         <v>504</v>
       </c>
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="111"/>
+      <c r="B45" s="107"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2777,7 +2817,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="111"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2795,7 +2835,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="111"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -2812,7 +2852,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="111"/>
+      <c r="B48" s="107"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -2828,8 +2868,8 @@
       </c>
       <c r="G48" s="34"/>
     </row>
-    <row r="49" spans="2:8" ht="15">
-      <c r="B49" s="111"/>
+    <row r="49" spans="2:7" ht="15">
+      <c r="B49" s="107"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -2845,209 +2885,291 @@
       </c>
       <c r="G49" s="34"/>
     </row>
-    <row r="50" spans="2:8" ht="15">
-      <c r="B50" s="111"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
+    <row r="50" spans="2:7" ht="15">
+      <c r="B50" s="107"/>
+      <c r="C50" s="145" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="30">
+        <v>11176</v>
+      </c>
+      <c r="E50" s="30">
+        <v>12078</v>
+      </c>
       <c r="F50" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>902</v>
       </c>
       <c r="G50" s="34"/>
     </row>
-    <row r="51" spans="2:8" ht="15">
-      <c r="B51" s="111"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
+    <row r="51" spans="2:7" ht="15">
+      <c r="B51" s="107"/>
+      <c r="C51" s="145" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="30">
+        <v>11348</v>
+      </c>
+      <c r="E51" s="30">
+        <v>12261</v>
+      </c>
       <c r="F51" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>913</v>
       </c>
       <c r="G51" s="34"/>
     </row>
-    <row r="52" spans="2:8" ht="15">
-      <c r="B52" s="111"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
+    <row r="52" spans="2:7" ht="15">
+      <c r="B52" s="107"/>
+      <c r="C52" s="145" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="30">
+        <v>11448</v>
+      </c>
+      <c r="E52" s="30">
+        <v>12362</v>
+      </c>
       <c r="F52" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>914</v>
       </c>
       <c r="G52" s="34"/>
     </row>
-    <row r="53" spans="2:8" ht="15">
-      <c r="B53" s="111"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
+    <row r="53" spans="2:7" ht="15">
+      <c r="B53" s="107"/>
+      <c r="C53" s="145" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="30">
+        <v>11560</v>
+      </c>
+      <c r="E53" s="30">
+        <v>12485</v>
+      </c>
       <c r="F53" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>925</v>
       </c>
       <c r="G53" s="34"/>
     </row>
-    <row r="54" spans="2:8" ht="15">
-      <c r="B54" s="111"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
+    <row r="54" spans="2:7" ht="15">
+      <c r="B54" s="107"/>
+      <c r="C54" s="145" t="s">
+        <v>127</v>
+      </c>
+      <c r="D54" s="30">
+        <v>11789</v>
+      </c>
+      <c r="E54" s="30">
+        <v>12812</v>
+      </c>
       <c r="F54" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1023</v>
       </c>
       <c r="G54" s="34"/>
     </row>
-    <row r="55" spans="2:8" ht="15">
-      <c r="B55" s="111"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
+    <row r="55" spans="2:7" ht="15">
+      <c r="B55" s="107"/>
+      <c r="C55" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="30">
+        <v>12097</v>
+      </c>
+      <c r="E55" s="30">
+        <v>13214</v>
+      </c>
       <c r="F55" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1117</v>
       </c>
       <c r="G55" s="34"/>
     </row>
-    <row r="56" spans="2:8" ht="15">
-      <c r="B56" s="111"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
+    <row r="56" spans="2:7" ht="15">
+      <c r="B56" s="107"/>
+      <c r="C56" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="30">
+        <v>12300</v>
+      </c>
+      <c r="E56" s="30">
+        <v>13430</v>
+      </c>
       <c r="F56" s="52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="G56" s="34"/>
     </row>
-    <row r="57" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B57" s="111"/>
-      <c r="C57" s="27" t="s">
+    <row r="57" spans="2:7" ht="15">
+      <c r="B57" s="107"/>
+      <c r="C57" s="145" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="30">
+        <v>12678</v>
+      </c>
+      <c r="E57" s="30">
+        <v>13820</v>
+      </c>
+      <c r="F57" s="52">
+        <f t="shared" si="4"/>
+        <v>1142</v>
+      </c>
+      <c r="G57" s="34"/>
+    </row>
+    <row r="58" spans="2:7" ht="15">
+      <c r="B58" s="107"/>
+      <c r="C58" s="145" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="30">
+        <v>12795</v>
+      </c>
+      <c r="E58" s="30">
+        <v>14167</v>
+      </c>
+      <c r="F58" s="52">
+        <f t="shared" si="4"/>
+        <v>1372</v>
+      </c>
+      <c r="G58" s="34"/>
+    </row>
+    <row r="59" spans="2:7" ht="15">
+      <c r="B59" s="107"/>
+      <c r="C59" s="145" t="s">
+        <v>130</v>
+      </c>
+      <c r="D59" s="30">
+        <v>12982</v>
+      </c>
+      <c r="E59" s="30">
+        <v>14406</v>
+      </c>
+      <c r="F59" s="52">
+        <f t="shared" si="4"/>
+        <v>1424</v>
+      </c>
+      <c r="G59" s="34"/>
+    </row>
+    <row r="60" spans="2:7" ht="15">
+      <c r="B60" s="107"/>
+      <c r="C60" s="145" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" s="30">
+        <v>13157</v>
+      </c>
+      <c r="E60" s="30">
+        <v>14563</v>
+      </c>
+      <c r="F60" s="52">
+        <f t="shared" si="4"/>
+        <v>1406</v>
+      </c>
+      <c r="G60" s="34"/>
+    </row>
+    <row r="61" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B61" s="107"/>
+      <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="54">
+      <c r="D61" s="28">
+        <v>13567</v>
+      </c>
+      <c r="E61" s="28">
+        <v>14973</v>
+      </c>
+      <c r="F61" s="54">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="33"/>
-    </row>
-    <row r="58" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B58" s="46">
+        <v>1406</v>
+      </c>
+      <c r="G61" s="33"/>
+    </row>
+    <row r="62" spans="2:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B62" s="46">
         <v>3</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C62" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="32">
-        <f>D57-D44</f>
-        <v>-9312</v>
-      </c>
-      <c r="E58" s="32">
-        <f>E57-E44</f>
-        <v>-9816</v>
-      </c>
-      <c r="F58" s="55">
-        <f>F57-F44</f>
-        <v>-504</v>
-      </c>
-      <c r="G58" s="37"/>
-    </row>
-    <row r="59" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="60" spans="2:8" ht="15">
-      <c r="B60" s="112" t="s">
+      <c r="D62" s="32">
+        <f>D61-D44</f>
+        <v>4255</v>
+      </c>
+      <c r="E62" s="32">
+        <f>E61-E44</f>
+        <v>5157</v>
+      </c>
+      <c r="F62" s="55">
+        <f>F61-F44</f>
+        <v>902</v>
+      </c>
+      <c r="G62" s="37"/>
+    </row>
+    <row r="63" spans="2:7" ht="13.5" thickBot="1"/>
+    <row r="64" spans="2:7" ht="15">
+      <c r="B64" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="42" t="s">
+      <c r="C64" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D60" s="43" t="s">
+      <c r="D64" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E64" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F60" s="43" t="s">
+      <c r="F64" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G60" s="44" t="s">
+      <c r="G64" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B61" s="113"/>
-      <c r="C61" s="27" t="s">
+    <row r="65" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B65" s="105"/>
+      <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="52">
-        <f t="shared" ref="F61:F74" si="5">IF(AND(D61&gt;0,E61&gt;0), E61-D61, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="33"/>
-    </row>
-    <row r="62" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B62" s="113"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="53">
+      <c r="D65" s="28">
+        <v>13567</v>
+      </c>
+      <c r="E65" s="28">
+        <v>14973</v>
+      </c>
+      <c r="F65" s="52">
+        <f t="shared" ref="F65:F78" si="5">IF(AND(D65&gt;0,E65&gt;0), E65-D65, 0)</f>
+        <v>1406</v>
+      </c>
+      <c r="G65" s="33"/>
+      <c r="H65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B66" s="105"/>
+      <c r="C66" s="145" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="30">
+        <v>13636</v>
+      </c>
+      <c r="E66" s="30">
+        <v>15042</v>
+      </c>
+      <c r="F66" s="53">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G62" s="34"/>
-    </row>
-    <row r="63" spans="2:8" ht="15">
-      <c r="B63" s="113"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="34"/>
-      <c r="H63" s="41"/>
-    </row>
-    <row r="64" spans="2:8" ht="15">
-      <c r="B64" s="113"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G64" s="34"/>
-    </row>
-    <row r="65" spans="2:8" ht="15" customHeight="1">
-      <c r="B65" s="113"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G65" s="34"/>
-    </row>
-    <row r="66" spans="2:8" ht="15">
-      <c r="B66" s="113"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1406</v>
       </c>
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="113"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="29"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -3056,9 +3178,10 @@
         <v>0</v>
       </c>
       <c r="G67" s="34"/>
+      <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="113"/>
+      <c r="B68" s="105"/>
       <c r="C68" s="29"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -3068,8 +3191,8 @@
       </c>
       <c r="G68" s="34"/>
     </row>
-    <row r="69" spans="2:8" ht="15">
-      <c r="B69" s="113"/>
+    <row r="69" spans="2:8" ht="15" customHeight="1">
+      <c r="B69" s="105"/>
       <c r="C69" s="29"/>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -3080,7 +3203,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="113"/>
+      <c r="B70" s="105"/>
       <c r="C70" s="29"/>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -3091,7 +3214,7 @@
       <c r="G70" s="34"/>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="113"/>
+      <c r="B71" s="105"/>
       <c r="C71" s="29"/>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -3102,7 +3225,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="113"/>
+      <c r="B72" s="105"/>
       <c r="C72" s="29"/>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3113,7 +3236,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="113"/>
+      <c r="B73" s="105"/>
       <c r="C73" s="29"/>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3123,132 +3246,131 @@
       </c>
       <c r="G73" s="34"/>
     </row>
-    <row r="74" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B74" s="113"/>
-      <c r="C74" s="27" t="s">
+    <row r="74" spans="2:8" ht="15">
+      <c r="B74" s="105"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G74" s="34"/>
+    </row>
+    <row r="75" spans="2:8" ht="15">
+      <c r="B75" s="105"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G75" s="34"/>
+    </row>
+    <row r="76" spans="2:8" ht="15">
+      <c r="B76" s="105"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="34"/>
+    </row>
+    <row r="77" spans="2:8" ht="15">
+      <c r="B77" s="105"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G77" s="34"/>
+    </row>
+    <row r="78" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B78" s="105"/>
+      <c r="C78" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="54">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G74" s="33"/>
-    </row>
-    <row r="75" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B75" s="45">
-        <v>4</v>
-      </c>
-      <c r="C75" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" s="32">
-        <f>D74-D61</f>
-        <v>0</v>
-      </c>
-      <c r="E75" s="32">
-        <f>E74-E61</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="55">
-        <f>F74-F61</f>
-        <v>0</v>
-      </c>
-      <c r="G75" s="36"/>
-    </row>
-    <row r="76" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="110" t="s">
-        <v>17</v>
-      </c>
-      <c r="C77" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D77" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E77" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F77" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G77" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="111"/>
-      <c r="C78" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="D78" s="28"/>
       <c r="E78" s="28"/>
-      <c r="F78" s="52">
-        <f t="shared" ref="F78:F91" si="6">IF(AND(D78&gt;0,E78&gt;0), E78-D78, 0)</f>
+      <c r="F78" s="54">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G78" s="33"/>
     </row>
-    <row r="79" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B79" s="111"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="53">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G79" s="34"/>
-    </row>
-    <row r="80" spans="2:8" ht="15">
-      <c r="B80" s="111"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G80" s="34"/>
-      <c r="H80" s="41"/>
-    </row>
-    <row r="81" spans="2:7" ht="15">
-      <c r="B81" s="111"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G81" s="34"/>
-    </row>
-    <row r="82" spans="2:7" ht="15" customHeight="1">
-      <c r="B82" s="111"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
+    <row r="79" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B79" s="45">
+        <v>4</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" s="32">
+        <f>D78-D65</f>
+        <v>-13567</v>
+      </c>
+      <c r="E79" s="32">
+        <f>E78-E65</f>
+        <v>-14973</v>
+      </c>
+      <c r="F79" s="55">
+        <f>F78-F65</f>
+        <v>-1406</v>
+      </c>
+      <c r="G79" s="36"/>
+    </row>
+    <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
+    <row r="81" spans="2:8" ht="15">
+      <c r="B81" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G81" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B82" s="107"/>
+      <c r="C82" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
       <c r="F82" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G82" s="34"/>
-    </row>
-    <row r="83" spans="2:7" ht="15">
-      <c r="B83" s="111"/>
+        <f t="shared" ref="F82:F95" si="6">IF(AND(D82&gt;0,E82&gt;0), E82-D82, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G82" s="33"/>
+    </row>
+    <row r="83" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B83" s="107"/>
       <c r="C83" s="29"/>
       <c r="D83" s="30"/>
       <c r="E83" s="30"/>
-      <c r="F83" s="52">
+      <c r="F83" s="53">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G83" s="34"/>
     </row>
-    <row r="84" spans="2:7" ht="15">
-      <c r="B84" s="111"/>
+    <row r="84" spans="2:8" ht="15">
+      <c r="B84" s="107"/>
       <c r="C84" s="29"/>
       <c r="D84" s="30"/>
       <c r="E84" s="30"/>
@@ -3257,9 +3379,10 @@
         <v>0</v>
       </c>
       <c r="G84" s="34"/>
-    </row>
-    <row r="85" spans="2:7" ht="15">
-      <c r="B85" s="111"/>
+      <c r="H84" s="41"/>
+    </row>
+    <row r="85" spans="2:8" ht="15">
+      <c r="B85" s="107"/>
       <c r="C85" s="29"/>
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
@@ -3269,8 +3392,8 @@
       </c>
       <c r="G85" s="34"/>
     </row>
-    <row r="86" spans="2:7" ht="15">
-      <c r="B86" s="111"/>
+    <row r="86" spans="2:8" ht="15" customHeight="1">
+      <c r="B86" s="107"/>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
@@ -3280,8 +3403,8 @@
       </c>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:7" ht="15">
-      <c r="B87" s="111"/>
+    <row r="87" spans="2:8" ht="15">
+      <c r="B87" s="107"/>
       <c r="C87" s="29"/>
       <c r="D87" s="30"/>
       <c r="E87" s="30"/>
@@ -3291,8 +3414,8 @@
       </c>
       <c r="G87" s="34"/>
     </row>
-    <row r="88" spans="2:7" ht="15">
-      <c r="B88" s="111"/>
+    <row r="88" spans="2:8" ht="15">
+      <c r="B88" s="107"/>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="30"/>
@@ -3302,8 +3425,8 @@
       </c>
       <c r="G88" s="34"/>
     </row>
-    <row r="89" spans="2:7" ht="15">
-      <c r="B89" s="111"/>
+    <row r="89" spans="2:8" ht="15">
+      <c r="B89" s="107"/>
       <c r="C89" s="29"/>
       <c r="D89" s="30"/>
       <c r="E89" s="30"/>
@@ -3313,8 +3436,8 @@
       </c>
       <c r="G89" s="34"/>
     </row>
-    <row r="90" spans="2:7" ht="15">
-      <c r="B90" s="111"/>
+    <row r="90" spans="2:8" ht="15">
+      <c r="B90" s="107"/>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
@@ -3324,132 +3447,131 @@
       </c>
       <c r="G90" s="34"/>
     </row>
-    <row r="91" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B91" s="111"/>
-      <c r="C91" s="27" t="s">
+    <row r="91" spans="2:8" ht="15">
+      <c r="B91" s="107"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="34"/>
+    </row>
+    <row r="92" spans="2:8" ht="15">
+      <c r="B92" s="107"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="34"/>
+    </row>
+    <row r="93" spans="2:8" ht="15">
+      <c r="B93" s="107"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="34"/>
+    </row>
+    <row r="94" spans="2:8" ht="15">
+      <c r="B94" s="107"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G94" s="34"/>
+    </row>
+    <row r="95" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B95" s="107"/>
+      <c r="C95" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="D91" s="28"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="54">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="33"/>
-    </row>
-    <row r="92" spans="2:7" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B92" s="46">
-        <v>5</v>
-      </c>
-      <c r="C92" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D92" s="32">
-        <f>D91-D78</f>
-        <v>0</v>
-      </c>
-      <c r="E92" s="32">
-        <f>E91-E78</f>
-        <v>0</v>
-      </c>
-      <c r="F92" s="55">
-        <f>F91-F78</f>
-        <v>0</v>
-      </c>
-      <c r="G92" s="37"/>
-    </row>
-    <row r="93" spans="2:7" ht="13.5" thickBot="1"/>
-    <row r="94" spans="2:7" ht="15">
-      <c r="B94" s="112" t="s">
-        <v>18</v>
-      </c>
-      <c r="C94" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D94" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F94" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B95" s="113"/>
-      <c r="C95" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="D95" s="28"/>
       <c r="E95" s="28"/>
-      <c r="F95" s="52">
-        <f t="shared" ref="F95:F108" si="7">IF(AND(D95&gt;0,E95&gt;0), E95-D95, 0)</f>
+      <c r="F95" s="54">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G95" s="33"/>
     </row>
-    <row r="96" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B96" s="113"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="53">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G96" s="34"/>
-    </row>
-    <row r="97" spans="2:8" ht="15">
-      <c r="B97" s="113"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G97" s="34"/>
-      <c r="H97" s="41"/>
-    </row>
+    <row r="96" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B96" s="46">
+        <v>5</v>
+      </c>
+      <c r="C96" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="32">
+        <f>D95-D82</f>
+        <v>0</v>
+      </c>
+      <c r="E96" s="32">
+        <f>E95-E82</f>
+        <v>0</v>
+      </c>
+      <c r="F96" s="55">
+        <f>F95-F82</f>
+        <v>0</v>
+      </c>
+      <c r="G96" s="37"/>
+    </row>
+    <row r="97" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="98" spans="2:8" ht="15">
-      <c r="B98" s="113"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G98" s="34"/>
-    </row>
-    <row r="99" spans="2:8" ht="15" customHeight="1">
-      <c r="B99" s="113"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="30"/>
-      <c r="E99" s="30"/>
+      <c r="B98" s="104" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G98" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B99" s="105"/>
+      <c r="C99" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
       <c r="F99" s="52">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G99" s="34"/>
-    </row>
-    <row r="100" spans="2:8" ht="15">
-      <c r="B100" s="113"/>
+        <f t="shared" ref="F99:F112" si="7">IF(AND(D99&gt;0,E99&gt;0), E99-D99, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G99" s="33"/>
+    </row>
+    <row r="100" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B100" s="105"/>
       <c r="C100" s="29"/>
       <c r="D100" s="30"/>
       <c r="E100" s="30"/>
-      <c r="F100" s="52">
+      <c r="F100" s="53">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G100" s="34"/>
     </row>
     <row r="101" spans="2:8" ht="15">
-      <c r="B101" s="113"/>
+      <c r="B101" s="105"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
@@ -3458,9 +3580,10 @@
         <v>0</v>
       </c>
       <c r="G101" s="34"/>
+      <c r="H101" s="41"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="113"/>
+      <c r="B102" s="105"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
@@ -3470,8 +3593,8 @@
       </c>
       <c r="G102" s="34"/>
     </row>
-    <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="113"/>
+    <row r="103" spans="2:8" ht="15" customHeight="1">
+      <c r="B103" s="105"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
       <c r="E103" s="30"/>
@@ -3482,7 +3605,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15">
-      <c r="B104" s="113"/>
+      <c r="B104" s="105"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
@@ -3493,7 +3616,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="113"/>
+      <c r="B105" s="105"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
       <c r="E105" s="30"/>
@@ -3504,7 +3627,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="113"/>
+      <c r="B106" s="105"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
@@ -3515,7 +3638,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="113"/>
+      <c r="B107" s="105"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
@@ -3525,132 +3648,131 @@
       </c>
       <c r="G107" s="34"/>
     </row>
-    <row r="108" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B108" s="113"/>
-      <c r="C108" s="27" t="s">
+    <row r="108" spans="2:8" ht="15">
+      <c r="B108" s="105"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="30"/>
+      <c r="E108" s="30"/>
+      <c r="F108" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G108" s="34"/>
+    </row>
+    <row r="109" spans="2:8" ht="15">
+      <c r="B109" s="105"/>
+      <c r="C109" s="29"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="30"/>
+      <c r="F109" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G109" s="34"/>
+    </row>
+    <row r="110" spans="2:8" ht="15">
+      <c r="B110" s="105"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="30"/>
+      <c r="E110" s="30"/>
+      <c r="F110" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G110" s="34"/>
+    </row>
+    <row r="111" spans="2:8" ht="15">
+      <c r="B111" s="105"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="30"/>
+      <c r="F111" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G111" s="34"/>
+    </row>
+    <row r="112" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B112" s="105"/>
+      <c r="C112" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="D108" s="28"/>
-      <c r="E108" s="28"/>
-      <c r="F108" s="54">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G108" s="33"/>
-    </row>
-    <row r="109" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B109" s="45">
-        <v>6</v>
-      </c>
-      <c r="C109" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D109" s="32">
-        <f>D108-D95</f>
-        <v>0</v>
-      </c>
-      <c r="E109" s="32">
-        <f>E108-E95</f>
-        <v>0</v>
-      </c>
-      <c r="F109" s="32">
-        <f>F108-F95</f>
-        <v>0</v>
-      </c>
-      <c r="G109" s="36"/>
-    </row>
-    <row r="110" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="C111" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D111" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E111" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F111" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G111" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="112" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B112" s="111"/>
-      <c r="C112" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
-      <c r="F112" s="52">
-        <f t="shared" ref="F112:F125" si="8">IF(AND(D112&gt;0,E112&gt;0), E112-D112, 0)</f>
+      <c r="F112" s="54">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G112" s="33"/>
     </row>
-    <row r="113" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B113" s="111"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="53">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G113" s="34"/>
-    </row>
-    <row r="114" spans="2:8" ht="15">
-      <c r="B114" s="111"/>
-      <c r="C114" s="29"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="30"/>
-      <c r="F114" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G114" s="34"/>
-      <c r="H114" s="41"/>
-    </row>
+    <row r="113" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B113" s="45">
+        <v>6</v>
+      </c>
+      <c r="C113" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" s="32">
+        <f>D112-D99</f>
+        <v>0</v>
+      </c>
+      <c r="E113" s="32">
+        <f>E112-E99</f>
+        <v>0</v>
+      </c>
+      <c r="F113" s="32">
+        <f>F112-F99</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="36"/>
+    </row>
+    <row r="114" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="111"/>
-      <c r="C115" s="29"/>
-      <c r="D115" s="30"/>
-      <c r="E115" s="30"/>
-      <c r="F115" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G115" s="34"/>
-    </row>
-    <row r="116" spans="2:8" ht="15" customHeight="1">
-      <c r="B116" s="111"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="30"/>
-      <c r="E116" s="30"/>
+      <c r="B115" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D115" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E115" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G115" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B116" s="107"/>
+      <c r="C116" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
       <c r="F116" s="52">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G116" s="34"/>
-    </row>
-    <row r="117" spans="2:8" ht="15">
-      <c r="B117" s="111"/>
+        <f t="shared" ref="F116:F129" si="8">IF(AND(D116&gt;0,E116&gt;0), E116-D116, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="33"/>
+    </row>
+    <row r="117" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B117" s="107"/>
       <c r="C117" s="29"/>
       <c r="D117" s="30"/>
       <c r="E117" s="30"/>
-      <c r="F117" s="52">
+      <c r="F117" s="53">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G117" s="34"/>
     </row>
     <row r="118" spans="2:8" ht="15">
-      <c r="B118" s="111"/>
+      <c r="B118" s="107"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -3659,9 +3781,10 @@
         <v>0</v>
       </c>
       <c r="G118" s="34"/>
+      <c r="H118" s="41"/>
     </row>
     <row r="119" spans="2:8" ht="15">
-      <c r="B119" s="111"/>
+      <c r="B119" s="107"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
@@ -3671,8 +3794,8 @@
       </c>
       <c r="G119" s="34"/>
     </row>
-    <row r="120" spans="2:8" ht="15">
-      <c r="B120" s="111"/>
+    <row r="120" spans="2:8" ht="15" customHeight="1">
+      <c r="B120" s="107"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -3683,7 +3806,7 @@
       <c r="G120" s="34"/>
     </row>
     <row r="121" spans="2:8" ht="15">
-      <c r="B121" s="111"/>
+      <c r="B121" s="107"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
@@ -3694,7 +3817,7 @@
       <c r="G121" s="34"/>
     </row>
     <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="111"/>
+      <c r="B122" s="107"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -3705,7 +3828,7 @@
       <c r="G122" s="34"/>
     </row>
     <row r="123" spans="2:8" ht="15">
-      <c r="B123" s="111"/>
+      <c r="B123" s="107"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
@@ -3716,7 +3839,7 @@
       <c r="G123" s="34"/>
     </row>
     <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="111"/>
+      <c r="B124" s="107"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -3726,132 +3849,131 @@
       </c>
       <c r="G124" s="34"/>
     </row>
-    <row r="125" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B125" s="111"/>
-      <c r="C125" s="27" t="s">
+    <row r="125" spans="2:8" ht="15">
+      <c r="B125" s="107"/>
+      <c r="C125" s="29"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G125" s="34"/>
+    </row>
+    <row r="126" spans="2:8" ht="15">
+      <c r="B126" s="107"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="30"/>
+      <c r="E126" s="30"/>
+      <c r="F126" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G126" s="34"/>
+    </row>
+    <row r="127" spans="2:8" ht="15">
+      <c r="B127" s="107"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="30"/>
+      <c r="F127" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G127" s="34"/>
+    </row>
+    <row r="128" spans="2:8" ht="15">
+      <c r="B128" s="107"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="30"/>
+      <c r="E128" s="30"/>
+      <c r="F128" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G128" s="34"/>
+    </row>
+    <row r="129" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B129" s="107"/>
+      <c r="C129" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="D125" s="28"/>
-      <c r="E125" s="28"/>
-      <c r="F125" s="54">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G125" s="33"/>
-    </row>
-    <row r="126" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B126" s="46">
-        <v>7</v>
-      </c>
-      <c r="C126" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D126" s="32">
-        <f>D125-D112</f>
-        <v>0</v>
-      </c>
-      <c r="E126" s="32">
-        <f>E125-E112</f>
-        <v>0</v>
-      </c>
-      <c r="F126" s="32">
-        <f>F125-F112</f>
-        <v>0</v>
-      </c>
-      <c r="G126" s="37"/>
-    </row>
-    <row r="127" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="112" t="s">
-        <v>20</v>
-      </c>
-      <c r="C128" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D128" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E128" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F128" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G128" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="129" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B129" s="113"/>
-      <c r="C129" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="D129" s="28"/>
       <c r="E129" s="28"/>
-      <c r="F129" s="52">
-        <f t="shared" ref="F129:F142" si="9">IF(AND(D129&gt;0,E129&gt;0), E129-D129, 0)</f>
+      <c r="F129" s="54">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G129" s="33"/>
     </row>
-    <row r="130" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B130" s="113"/>
-      <c r="C130" s="29"/>
-      <c r="D130" s="30"/>
-      <c r="E130" s="30"/>
-      <c r="F130" s="53">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G130" s="34"/>
-    </row>
-    <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="113"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="30"/>
-      <c r="E131" s="30"/>
-      <c r="F131" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G131" s="34"/>
-      <c r="H131" s="41"/>
-    </row>
+    <row r="130" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B130" s="46">
+        <v>7</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D130" s="32">
+        <f>D129-D116</f>
+        <v>0</v>
+      </c>
+      <c r="E130" s="32">
+        <f>E129-E116</f>
+        <v>0</v>
+      </c>
+      <c r="F130" s="32">
+        <f>F129-F116</f>
+        <v>0</v>
+      </c>
+      <c r="G130" s="37"/>
+    </row>
+    <row r="131" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="113"/>
-      <c r="C132" s="29"/>
-      <c r="D132" s="30"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G132" s="34"/>
-    </row>
-    <row r="133" spans="2:8" ht="15" customHeight="1">
-      <c r="B133" s="113"/>
-      <c r="C133" s="29"/>
-      <c r="D133" s="30"/>
-      <c r="E133" s="30"/>
+      <c r="B132" s="104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D132" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E132" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F132" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G132" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B133" s="105"/>
+      <c r="C133" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D133" s="28"/>
+      <c r="E133" s="28"/>
       <c r="F133" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G133" s="34"/>
-    </row>
-    <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="113"/>
+        <f t="shared" ref="F133:F146" si="9">IF(AND(D133&gt;0,E133&gt;0), E133-D133, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G133" s="33"/>
+    </row>
+    <row r="134" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B134" s="105"/>
       <c r="C134" s="29"/>
       <c r="D134" s="30"/>
       <c r="E134" s="30"/>
-      <c r="F134" s="52">
+      <c r="F134" s="53">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G134" s="34"/>
     </row>
     <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="113"/>
+      <c r="B135" s="105"/>
       <c r="C135" s="29"/>
       <c r="D135" s="30"/>
       <c r="E135" s="30"/>
@@ -3860,9 +3982,10 @@
         <v>0</v>
       </c>
       <c r="G135" s="34"/>
+      <c r="H135" s="41"/>
     </row>
     <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="113"/>
+      <c r="B136" s="105"/>
       <c r="C136" s="29"/>
       <c r="D136" s="30"/>
       <c r="E136" s="30"/>
@@ -3872,8 +3995,8 @@
       </c>
       <c r="G136" s="34"/>
     </row>
-    <row r="137" spans="2:8" ht="15">
-      <c r="B137" s="113"/>
+    <row r="137" spans="2:8" ht="15" customHeight="1">
+      <c r="B137" s="105"/>
       <c r="C137" s="29"/>
       <c r="D137" s="30"/>
       <c r="E137" s="30"/>
@@ -3884,7 +4007,7 @@
       <c r="G137" s="34"/>
     </row>
     <row r="138" spans="2:8" ht="15">
-      <c r="B138" s="113"/>
+      <c r="B138" s="105"/>
       <c r="C138" s="29"/>
       <c r="D138" s="30"/>
       <c r="E138" s="30"/>
@@ -3895,7 +4018,7 @@
       <c r="G138" s="34"/>
     </row>
     <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="113"/>
+      <c r="B139" s="105"/>
       <c r="C139" s="29"/>
       <c r="D139" s="30"/>
       <c r="E139" s="30"/>
@@ -3906,7 +4029,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:8" ht="15">
-      <c r="B140" s="113"/>
+      <c r="B140" s="105"/>
       <c r="C140" s="29"/>
       <c r="D140" s="30"/>
       <c r="E140" s="30"/>
@@ -3917,7 +4040,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:8" ht="15">
-      <c r="B141" s="113"/>
+      <c r="B141" s="105"/>
       <c r="C141" s="29"/>
       <c r="D141" s="30"/>
       <c r="E141" s="30"/>
@@ -3927,57 +4050,101 @@
       </c>
       <c r="G141" s="34"/>
     </row>
-    <row r="142" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B142" s="113"/>
-      <c r="C142" s="27" t="s">
+    <row r="142" spans="2:8" ht="15">
+      <c r="B142" s="105"/>
+      <c r="C142" s="29"/>
+      <c r="D142" s="30"/>
+      <c r="E142" s="30"/>
+      <c r="F142" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G142" s="34"/>
+    </row>
+    <row r="143" spans="2:8" ht="15">
+      <c r="B143" s="105"/>
+      <c r="C143" s="29"/>
+      <c r="D143" s="30"/>
+      <c r="E143" s="30"/>
+      <c r="F143" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G143" s="34"/>
+    </row>
+    <row r="144" spans="2:8" ht="15">
+      <c r="B144" s="105"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="30"/>
+      <c r="E144" s="30"/>
+      <c r="F144" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G144" s="34"/>
+    </row>
+    <row r="145" spans="2:8" ht="15">
+      <c r="B145" s="105"/>
+      <c r="C145" s="29"/>
+      <c r="D145" s="30"/>
+      <c r="E145" s="30"/>
+      <c r="F145" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G145" s="34"/>
+    </row>
+    <row r="146" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B146" s="105"/>
+      <c r="C146" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D142" s="28"/>
-      <c r="E142" s="28"/>
-      <c r="F142" s="54">
+      <c r="D146" s="28"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="54">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G142" s="33"/>
-    </row>
-    <row r="143" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B143" s="45">
+      <c r="G146" s="33"/>
+    </row>
+    <row r="147" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B147" s="45">
         <v>8</v>
       </c>
-      <c r="C143" s="31" t="s">
+      <c r="C147" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D143" s="32">
-        <f>D142-D129</f>
-        <v>0</v>
-      </c>
-      <c r="E143" s="32">
-        <f>E142-E129</f>
-        <v>0</v>
-      </c>
-      <c r="F143" s="32">
-        <f>F142-F129</f>
-        <v>0</v>
-      </c>
-      <c r="G143" s="36"/>
-    </row>
-    <row r="148" spans="8:8">
-      <c r="H148" s="41"/>
+      <c r="D147" s="32">
+        <f>D146-D133</f>
+        <v>0</v>
+      </c>
+      <c r="E147" s="32">
+        <f>E146-E133</f>
+        <v>0</v>
+      </c>
+      <c r="F147" s="32">
+        <f>F146-F133</f>
+        <v>0</v>
+      </c>
+      <c r="G147" s="36"/>
+    </row>
+    <row r="152" spans="2:8">
+      <c r="H152" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B128:B142"/>
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B43:B57"/>
-    <mergeCell ref="B60:B74"/>
-    <mergeCell ref="B77:B91"/>
-    <mergeCell ref="B94:B108"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B111:B125"/>
+    <mergeCell ref="B115:B129"/>
     <mergeCell ref="B31:B39"/>
+    <mergeCell ref="B132:B146"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B43:B61"/>
+    <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B81:B95"/>
+    <mergeCell ref="B98:B112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5774,24 +5941,24 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6006,7 +6173,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6279,7 +6446,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6301,150 +6468,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="137"/>
+      <c r="B1" s="136"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="133"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="143"/>
+      <c r="B3" s="133"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="140"/>
-      <c r="B4" s="141"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="140"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="138" t="s">
+      <c r="A5" s="137" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="139"/>
+      <c r="B5" s="138"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="131"/>
+      <c r="B7" s="144"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="142"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="134"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="129"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="126" t="s">
+      <c r="A11" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="127"/>
+      <c r="B11" s="131"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="126" t="s">
+      <c r="A12" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="127"/>
+      <c r="B12" s="131"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="127"/>
+      <c r="B13" s="131"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="127"/>
+      <c r="B14" s="131"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="126" t="s">
+      <c r="A15" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="127"/>
+      <c r="B15" s="131"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="126" t="s">
+      <c r="A16" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="127"/>
+      <c r="B16" s="131"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="128" t="s">
+      <c r="A17" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="129"/>
+      <c r="B17" s="127"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="130" t="s">
+      <c r="A19" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="131"/>
+      <c r="B19" s="144"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="132" t="s">
+      <c r="A21" s="141" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="133"/>
+      <c r="B21" s="142"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="134"/>
-      <c r="B22" s="135"/>
+      <c r="A22" s="128"/>
+      <c r="B22" s="129"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="126" t="s">
+      <c r="A23" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="127"/>
+      <c r="B23" s="131"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="126"/>
-      <c r="B24" s="127"/>
+      <c r="A24" s="130"/>
+      <c r="B24" s="131"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="126" t="s">
+      <c r="A25" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="127"/>
+      <c r="B25" s="131"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="126" t="s">
+      <c r="A26" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="127"/>
+      <c r="B26" s="131"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="128"/>
-      <c r="B27" s="129"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -6455,19 +6635,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - most of level 4 done, over 2000 ahead of v1
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="139">
   <si>
     <t>Notes</t>
   </si>
@@ -539,6 +539,24 @@
   </si>
   <si>
     <t>Begin = Kyle appears</t>
+  </si>
+  <si>
+    <t>X = 220</t>
+  </si>
+  <si>
+    <t>X =990</t>
+  </si>
+  <si>
+    <t>Forgoes weapon upgrade</t>
+  </si>
+  <si>
+    <t>X=1057 (top)</t>
+  </si>
+  <si>
+    <t>Begin elevator down</t>
+  </si>
+  <si>
+    <t>X = 2046 (top shaft)</t>
   </si>
 </sst>
 </file>
@@ -1844,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3170,7 +3188,9 @@
     </row>
     <row r="67" spans="2:8" ht="15">
       <c r="B67" s="105"/>
-      <c r="C67" s="29"/>
+      <c r="C67" s="145" t="s">
+        <v>121</v>
+      </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
       <c r="F67" s="52">
@@ -3182,78 +3202,123 @@
     </row>
     <row r="68" spans="2:8" ht="15">
       <c r="B68" s="105"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
+      <c r="C68" s="145" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="30">
+        <v>13928</v>
+      </c>
+      <c r="E68" s="30">
+        <v>15367</v>
+      </c>
       <c r="F68" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1439</v>
       </c>
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
       <c r="B69" s="105"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
+      <c r="C69" s="145" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" s="30">
+        <v>14086</v>
+      </c>
+      <c r="E69" s="30">
+        <v>15527</v>
+      </c>
       <c r="F69" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
       <c r="B70" s="105"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
+      <c r="C70" s="145" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" s="30">
+        <v>14290</v>
+      </c>
+      <c r="E70" s="30">
+        <v>16248</v>
+      </c>
       <c r="F70" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1958</v>
       </c>
       <c r="G70" s="34"/>
+      <c r="H70" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="71" spans="2:8" ht="15">
       <c r="B71" s="105"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
+      <c r="C71" s="145" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="30">
+        <v>14474</v>
+      </c>
+      <c r="E71" s="30">
+        <v>16459</v>
+      </c>
       <c r="F71" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
       <c r="B72" s="105"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
+      <c r="C72" s="145" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" s="30">
+        <v>14904</v>
+      </c>
+      <c r="E72" s="30">
+        <v>16923</v>
+      </c>
       <c r="F72" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
       <c r="B73" s="105"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
+      <c r="C73" s="145" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="30">
+        <v>15282</v>
+      </c>
+      <c r="E73" s="30">
+        <v>17347</v>
+      </c>
       <c r="F73" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2065</v>
       </c>
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
       <c r="B74" s="105"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
+      <c r="C74" s="145" t="s">
+        <v>138</v>
+      </c>
+      <c r="D74" s="30">
+        <v>15696</v>
+      </c>
+      <c r="E74" s="30">
+        <v>17762</v>
+      </c>
       <c r="F74" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2066</v>
       </c>
       <c r="G74" s="34"/>
     </row>

</xml_diff>

<commit_message>
Terminator - Up to the beginning of level 7, done by Cardboard
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="150">
   <si>
     <t>Notes</t>
   </si>
@@ -558,6 +558,39 @@
   <si>
     <t>X = 2046 (top shaft)</t>
   </si>
+  <si>
+    <t>X = 2452</t>
+  </si>
+  <si>
+    <t>Health pack disappear</t>
+  </si>
+  <si>
+    <t>Grab ladder</t>
+  </si>
+  <si>
+    <t>X = 2000</t>
+  </si>
+  <si>
+    <t>X &gt; 1900, Y = 145</t>
+  </si>
+  <si>
+    <t>X &gt; 3800</t>
+  </si>
+  <si>
+    <t>X &gt; 5025, Y = 153</t>
+  </si>
+  <si>
+    <t>6 grenades</t>
+  </si>
+  <si>
+    <t>X = 1454, Y = 161</t>
+  </si>
+  <si>
+    <t>X = 3389, Y = 159</t>
+  </si>
+  <si>
+    <t>X = 4394, Y = 131</t>
+  </si>
 </sst>
 </file>
 
@@ -567,10 +600,24 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1266,14 +1313,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1281,7 +1328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1289,75 +1336,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1367,10 +1414,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1391,132 +1438,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1524,44 +1577,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Färg1" xfId="2" builtinId="29"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Total" xfId="1" builtinId="25"/>
+    <cellStyle name="Summa" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1576,7 +1632,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1860,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O152"/>
+  <dimension ref="B1:O136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1877,19 +1933,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="109" t="s">
+      <c r="C1" s="110"/>
+      <c r="D1" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="110"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="112"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
-        <f>SUM(H1:H65534)</f>
+        <f>SUM(H1:H65518)</f>
         <v>225</v>
       </c>
       <c r="J1" s="71" t="s">
@@ -1964,10 +2020,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="111"/>
+      <c r="E5" s="113"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2004,7 +2060,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="114" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2024,7 +2080,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="113"/>
+      <c r="B9" s="115"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2034,7 +2090,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="113"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2045,7 +2101,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="113"/>
+      <c r="B11" s="115"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2056,7 +2112,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="113"/>
+      <c r="B12" s="115"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2067,7 +2123,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="113"/>
+      <c r="B13" s="115"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2078,7 +2134,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="113"/>
+      <c r="B14" s="115"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2089,7 +2145,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="113"/>
+      <c r="B15" s="115"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2100,7 +2156,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="113"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2143,7 +2199,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="108" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2178,7 +2234,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="107"/>
+      <c r="B20" s="109"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2211,7 +2267,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="107"/>
+      <c r="B21" s="109"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2244,7 +2300,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="107"/>
+      <c r="B22" s="109"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2277,7 +2333,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="107"/>
+      <c r="B23" s="109"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2310,7 +2366,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="107"/>
+      <c r="B24" s="109"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2346,7 +2402,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="107"/>
+      <c r="B25" s="109"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2379,7 +2435,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="107"/>
+      <c r="B26" s="109"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2412,7 +2468,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="107"/>
+      <c r="B27" s="109"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2445,7 +2501,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="107"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2478,7 +2534,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="107"/>
+      <c r="B29" s="109"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2504,7 +2560,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="106" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2539,7 +2595,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="105"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2568,7 +2624,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="105"/>
+      <c r="B33" s="107"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2597,7 +2653,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="105"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2627,7 +2683,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="105"/>
+      <c r="B35" s="107"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2647,7 +2703,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="105"/>
+      <c r="B36" s="107"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2667,7 +2723,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="105"/>
+      <c r="B37" s="107"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2690,7 +2746,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="105"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2713,7 +2769,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="105"/>
+      <c r="B39" s="107"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2781,7 +2837,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="106" t="s">
+      <c r="B43" s="108" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2801,7 +2857,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="107"/>
+      <c r="B44" s="109"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2818,7 +2874,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="107"/>
+      <c r="B45" s="109"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2835,7 +2891,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="107"/>
+      <c r="B46" s="109"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2853,7 +2909,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="107"/>
+      <c r="B47" s="109"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -2870,7 +2926,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="107"/>
+      <c r="B48" s="109"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -2886,8 +2942,8 @@
       </c>
       <c r="G48" s="34"/>
     </row>
-    <row r="49" spans="2:7" ht="15">
-      <c r="B49" s="107"/>
+    <row r="49" spans="2:13" ht="15">
+      <c r="B49" s="109"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -2903,9 +2959,9 @@
       </c>
       <c r="G49" s="34"/>
     </row>
-    <row r="50" spans="2:7" ht="15">
-      <c r="B50" s="107"/>
-      <c r="C50" s="145" t="s">
+    <row r="50" spans="2:13" ht="15">
+      <c r="B50" s="109"/>
+      <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
       <c r="D50" s="30">
@@ -2920,9 +2976,9 @@
       </c>
       <c r="G50" s="34"/>
     </row>
-    <row r="51" spans="2:7" ht="15">
-      <c r="B51" s="107"/>
-      <c r="C51" s="145" t="s">
+    <row r="51" spans="2:13" ht="15">
+      <c r="B51" s="109"/>
+      <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
       <c r="D51" s="30">
@@ -2937,9 +2993,9 @@
       </c>
       <c r="G51" s="34"/>
     </row>
-    <row r="52" spans="2:7" ht="15">
-      <c r="B52" s="107"/>
-      <c r="C52" s="145" t="s">
+    <row r="52" spans="2:13" ht="15">
+      <c r="B52" s="109"/>
+      <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
       <c r="D52" s="30">
@@ -2954,9 +3010,9 @@
       </c>
       <c r="G52" s="34"/>
     </row>
-    <row r="53" spans="2:7" ht="15">
-      <c r="B53" s="107"/>
-      <c r="C53" s="145" t="s">
+    <row r="53" spans="2:13" ht="15">
+      <c r="B53" s="109"/>
+      <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
       <c r="D53" s="30">
@@ -2971,9 +3027,9 @@
       </c>
       <c r="G53" s="34"/>
     </row>
-    <row r="54" spans="2:7" ht="15">
-      <c r="B54" s="107"/>
-      <c r="C54" s="145" t="s">
+    <row r="54" spans="2:13" ht="15">
+      <c r="B54" s="109"/>
+      <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
       <c r="D54" s="30">
@@ -2988,9 +3044,9 @@
       </c>
       <c r="G54" s="34"/>
     </row>
-    <row r="55" spans="2:7" ht="15">
-      <c r="B55" s="107"/>
-      <c r="C55" s="145" t="s">
+    <row r="55" spans="2:13" ht="15">
+      <c r="B55" s="109"/>
+      <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
       <c r="D55" s="30">
@@ -3005,9 +3061,9 @@
       </c>
       <c r="G55" s="34"/>
     </row>
-    <row r="56" spans="2:7" ht="15">
-      <c r="B56" s="107"/>
-      <c r="C56" s="145" t="s">
+    <row r="56" spans="2:13" ht="15">
+      <c r="B56" s="109"/>
+      <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
       <c r="D56" s="30">
@@ -3022,9 +3078,9 @@
       </c>
       <c r="G56" s="34"/>
     </row>
-    <row r="57" spans="2:7" ht="15">
-      <c r="B57" s="107"/>
-      <c r="C57" s="145" t="s">
+    <row r="57" spans="2:13" ht="15">
+      <c r="B57" s="109"/>
+      <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
       <c r="D57" s="30">
@@ -3039,9 +3095,9 @@
       </c>
       <c r="G57" s="34"/>
     </row>
-    <row r="58" spans="2:7" ht="15">
-      <c r="B58" s="107"/>
-      <c r="C58" s="145" t="s">
+    <row r="58" spans="2:13" ht="15">
+      <c r="B58" s="109"/>
+      <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="30">
@@ -3055,10 +3111,13 @@
         <v>1372</v>
       </c>
       <c r="G58" s="34"/>
-    </row>
-    <row r="59" spans="2:7" ht="15">
-      <c r="B59" s="107"/>
-      <c r="C59" s="145" t="s">
+      <c r="M58">
+        <v>18638</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" ht="15">
+      <c r="B59" s="109"/>
+      <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
       <c r="D59" s="30">
@@ -3073,9 +3132,9 @@
       </c>
       <c r="G59" s="34"/>
     </row>
-    <row r="60" spans="2:7" ht="15">
-      <c r="B60" s="107"/>
-      <c r="C60" s="145" t="s">
+    <row r="60" spans="2:13" ht="15">
+      <c r="B60" s="109"/>
+      <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
       <c r="D60" s="30">
@@ -3090,8 +3149,8 @@
       </c>
       <c r="G60" s="34"/>
     </row>
-    <row r="61" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B61" s="107"/>
+    <row r="61" spans="2:13" ht="15.75" thickBot="1">
+      <c r="B61" s="109"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3107,7 +3166,7 @@
       </c>
       <c r="G61" s="33"/>
     </row>
-    <row r="62" spans="2:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="62" spans="2:13" ht="17.25" thickTop="1" thickBot="1">
       <c r="B62" s="46">
         <v>3</v>
       </c>
@@ -3128,9 +3187,9 @@
       </c>
       <c r="G62" s="37"/>
     </row>
-    <row r="63" spans="2:7" ht="13.5" thickBot="1"/>
-    <row r="64" spans="2:7" ht="15">
-      <c r="B64" s="104" t="s">
+    <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
+    <row r="64" spans="2:13" ht="15">
+      <c r="B64" s="106" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3150,7 +3209,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="105"/>
+      <c r="B65" s="107"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3170,8 +3229,8 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="105"/>
-      <c r="C66" s="145" t="s">
+      <c r="B66" s="107"/>
+      <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
       <c r="D66" s="30">
@@ -3187,8 +3246,8 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="105"/>
-      <c r="C67" s="145" t="s">
+      <c r="B67" s="107"/>
+      <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
       <c r="D67" s="30"/>
@@ -3201,8 +3260,8 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="105"/>
-      <c r="C68" s="145" t="s">
+      <c r="B68" s="107"/>
+      <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
       <c r="D68" s="30">
@@ -3218,8 +3277,8 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="105"/>
-      <c r="C69" s="145" t="s">
+      <c r="B69" s="107"/>
+      <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
       <c r="D69" s="30">
@@ -3235,8 +3294,8 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="105"/>
-      <c r="C70" s="145" t="s">
+      <c r="B70" s="107"/>
+      <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
       <c r="D70" s="30">
@@ -3255,8 +3314,8 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="105"/>
-      <c r="C71" s="145" t="s">
+      <c r="B71" s="107"/>
+      <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
       <c r="D71" s="30">
@@ -3272,8 +3331,8 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="105"/>
-      <c r="C72" s="145" t="s">
+      <c r="B72" s="107"/>
+      <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
       <c r="D72" s="30">
@@ -3289,8 +3348,8 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="105"/>
-      <c r="C73" s="145" t="s">
+      <c r="B73" s="107"/>
+      <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
       <c r="D73" s="30">
@@ -3306,8 +3365,8 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="105"/>
-      <c r="C74" s="145" t="s">
+      <c r="B74" s="107"/>
+      <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
       <c r="D74" s="30">
@@ -3323,29 +3382,41 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="105"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
+      <c r="B75" s="107"/>
+      <c r="C75" s="105" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75" s="30">
+        <v>16567</v>
+      </c>
+      <c r="E75" s="30">
+        <v>18638</v>
+      </c>
       <c r="F75" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2071</v>
       </c>
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="105"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
+      <c r="B76" s="107"/>
+      <c r="C76" s="105" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76" s="30">
+        <v>17053</v>
+      </c>
+      <c r="E76" s="30">
+        <v>19407</v>
+      </c>
       <c r="F76" s="52">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2354</v>
       </c>
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="105"/>
+      <c r="B77" s="107"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3356,15 +3427,19 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="105"/>
+      <c r="B78" s="107"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
+      <c r="D78" s="28">
+        <v>18005</v>
+      </c>
+      <c r="E78" s="28">
+        <v>20429</v>
+      </c>
       <c r="F78" s="54">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2424</v>
       </c>
       <c r="G78" s="33"/>
     </row>
@@ -3377,21 +3452,21 @@
       </c>
       <c r="D79" s="32">
         <f>D78-D65</f>
-        <v>-13567</v>
+        <v>4438</v>
       </c>
       <c r="E79" s="32">
         <f>E78-E65</f>
-        <v>-14973</v>
+        <v>5456</v>
       </c>
       <c r="F79" s="55">
         <f>F78-F65</f>
-        <v>-1406</v>
+        <v>1018</v>
       </c>
       <c r="G79" s="36"/>
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="81" spans="2:8" ht="15">
-      <c r="B81" s="106" t="s">
+    <row r="81" spans="2:9" ht="15" customHeight="1">
+      <c r="B81" s="108" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3410,35 +3485,49 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B82" s="107"/>
+    <row r="82" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B82" s="109"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D82" s="28"/>
-      <c r="E82" s="28"/>
+      <c r="D82" s="28">
+        <v>18419</v>
+      </c>
+      <c r="E82" s="28">
+        <v>20859</v>
+      </c>
       <c r="F82" s="52">
-        <f t="shared" ref="F82:F95" si="6">IF(AND(D82&gt;0,E82&gt;0), E82-D82, 0)</f>
-        <v>0</v>
+        <f t="shared" ref="F82:F88" si="6">IF(AND(D82&gt;0,E82&gt;0), E82-D82, 0)</f>
+        <v>2440</v>
       </c>
       <c r="G82" s="33"/>
     </row>
-    <row r="83" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B83" s="107"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
+    <row r="83" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B83" s="109"/>
+      <c r="C83" s="147" t="s">
+        <v>141</v>
+      </c>
+      <c r="D83" s="30">
+        <v>18995</v>
+      </c>
+      <c r="E83" s="30">
+        <v>21505</v>
+      </c>
       <c r="F83" s="53">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2510</v>
       </c>
       <c r="G83" s="34"/>
     </row>
-    <row r="84" spans="2:8" ht="15">
-      <c r="B84" s="107"/>
-      <c r="C84" s="29"/>
+    <row r="84" spans="2:9" ht="15">
+      <c r="B84" s="109"/>
+      <c r="C84" s="147" t="s">
+        <v>142</v>
+      </c>
       <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
+      <c r="E84" s="30">
+        <v>22294</v>
+      </c>
       <c r="F84" s="52">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3446,407 +3535,473 @@
       <c r="G84" s="34"/>
       <c r="H84" s="41"/>
     </row>
-    <row r="85" spans="2:8" ht="15">
-      <c r="B85" s="107"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
+    <row r="85" spans="2:9" ht="15">
+      <c r="B85" s="109"/>
+      <c r="C85" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="D85" s="30">
+        <v>20269</v>
+      </c>
+      <c r="E85" s="30">
+        <v>23022</v>
+      </c>
       <c r="F85" s="52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2753</v>
       </c>
       <c r="G85" s="34"/>
     </row>
-    <row r="86" spans="2:8" ht="15" customHeight="1">
-      <c r="B86" s="107"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
+    <row r="86" spans="2:9" ht="15" customHeight="1">
+      <c r="B86" s="109"/>
+      <c r="C86" s="147" t="s">
+        <v>144</v>
+      </c>
+      <c r="D86" s="30">
+        <v>21047</v>
+      </c>
+      <c r="E86" s="30">
+        <v>24045</v>
+      </c>
       <c r="F86" s="52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2998</v>
       </c>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:8" ht="15">
-      <c r="B87" s="107"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
+    <row r="87" spans="2:9" ht="15">
+      <c r="B87" s="109"/>
+      <c r="C87" s="147" t="s">
+        <v>145</v>
+      </c>
+      <c r="D87" s="30">
+        <v>22250</v>
+      </c>
+      <c r="E87" s="30">
+        <v>25436</v>
+      </c>
       <c r="F87" s="52">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3186</v>
       </c>
       <c r="G87" s="34"/>
     </row>
-    <row r="88" spans="2:8" ht="15">
-      <c r="B88" s="107"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="52">
+    <row r="88" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B88" s="148"/>
+      <c r="C88" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D88" s="28">
+        <v>23109</v>
+      </c>
+      <c r="E88" s="28">
+        <v>26334</v>
+      </c>
+      <c r="F88" s="54">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G88" s="34"/>
-    </row>
-    <row r="89" spans="2:8" ht="15">
-      <c r="B89" s="107"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G89" s="34"/>
-    </row>
-    <row r="90" spans="2:8" ht="15">
-      <c r="B90" s="107"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G90" s="34"/>
-    </row>
-    <row r="91" spans="2:8" ht="15">
-      <c r="B91" s="107"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="34"/>
-    </row>
-    <row r="92" spans="2:8" ht="15">
+        <v>3225</v>
+      </c>
+      <c r="G88" s="33"/>
+      <c r="I88" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B89" s="46">
+        <v>5</v>
+      </c>
+      <c r="C89" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" s="32">
+        <f>D88-D82</f>
+        <v>4690</v>
+      </c>
+      <c r="E89" s="32">
+        <f>E88-E82</f>
+        <v>5475</v>
+      </c>
+      <c r="F89" s="55">
+        <f>F88-F82</f>
+        <v>785</v>
+      </c>
+      <c r="G89" s="37"/>
+    </row>
+    <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
+    <row r="91" spans="2:9" ht="15" customHeight="1">
+      <c r="B91" s="106" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" ht="15.75" thickBot="1">
       <c r="B92" s="107"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
+      <c r="C92" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="28">
+        <v>23549</v>
+      </c>
+      <c r="E92" s="28">
+        <v>26774</v>
+      </c>
       <c r="F92" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G92" s="34"/>
-    </row>
-    <row r="93" spans="2:8" ht="15">
+        <f t="shared" ref="F92:F96" si="7">IF(AND(D92&gt;0,E92&gt;0), E92-D92, 0)</f>
+        <v>3225</v>
+      </c>
+      <c r="G92" s="33"/>
+    </row>
+    <row r="93" spans="2:9" ht="15.75" thickTop="1">
       <c r="B93" s="107"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="C93" s="147" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="30">
+        <v>24723</v>
+      </c>
+      <c r="E93" s="30">
+        <v>28104</v>
+      </c>
+      <c r="F93" s="53">
+        <f t="shared" si="7"/>
+        <v>3381</v>
       </c>
       <c r="G93" s="34"/>
     </row>
-    <row r="94" spans="2:8" ht="15">
+    <row r="94" spans="2:9" ht="15">
       <c r="B94" s="107"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
+      <c r="C94" s="147" t="s">
+        <v>148</v>
+      </c>
+      <c r="D94" s="30">
+        <v>25507</v>
+      </c>
+      <c r="E94" s="30">
+        <v>29197</v>
+      </c>
       <c r="F94" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>3690</v>
       </c>
       <c r="G94" s="34"/>
-    </row>
-    <row r="95" spans="2:8" ht="15.75" thickBot="1">
+      <c r="H94" s="41"/>
+    </row>
+    <row r="95" spans="2:9" ht="15">
       <c r="B95" s="107"/>
-      <c r="C95" s="27" t="s">
+      <c r="C95" s="147" t="s">
+        <v>149</v>
+      </c>
+      <c r="D95" s="30"/>
+      <c r="E95" s="30">
+        <v>29955</v>
+      </c>
+      <c r="F95" s="52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G95" s="34"/>
+    </row>
+    <row r="96" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B96" s="101"/>
+      <c r="C96" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="54">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G95" s="33"/>
-    </row>
-    <row r="96" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B96" s="46">
-        <v>5</v>
-      </c>
-      <c r="C96" s="31" t="s">
+      <c r="D96" s="28">
+        <v>26769</v>
+      </c>
+      <c r="E96" s="28">
+        <v>30582</v>
+      </c>
+      <c r="F96" s="54">
+        <f t="shared" si="7"/>
+        <v>3813</v>
+      </c>
+      <c r="G96" s="33"/>
+    </row>
+    <row r="97" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B97" s="45">
+        <v>6</v>
+      </c>
+      <c r="C97" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D96" s="32">
-        <f>D95-D82</f>
-        <v>0</v>
-      </c>
-      <c r="E96" s="32">
-        <f>E95-E82</f>
-        <v>0</v>
-      </c>
-      <c r="F96" s="55">
-        <f>F95-F82</f>
-        <v>0</v>
-      </c>
-      <c r="G96" s="37"/>
-    </row>
-    <row r="97" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="98" spans="2:8" ht="15">
-      <c r="B98" s="104" t="s">
-        <v>18</v>
-      </c>
-      <c r="C98" s="42" t="s">
+      <c r="D97" s="32">
+        <f>D96-D92</f>
+        <v>3220</v>
+      </c>
+      <c r="E97" s="32">
+        <f>E96-E92</f>
+        <v>3808</v>
+      </c>
+      <c r="F97" s="32">
+        <f>F96-F92</f>
+        <v>588</v>
+      </c>
+      <c r="G97" s="36"/>
+    </row>
+    <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
+    <row r="99" spans="2:8" ht="15">
+      <c r="B99" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D98" s="43" t="s">
+      <c r="D99" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E98" s="43" t="s">
+      <c r="E99" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F98" s="43" t="s">
+      <c r="F99" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G98" s="44" t="s">
+      <c r="G99" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B99" s="105"/>
-      <c r="C99" s="27" t="s">
+    <row r="100" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B100" s="109"/>
+      <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="52">
-        <f t="shared" ref="F99:F112" si="7">IF(AND(D99&gt;0,E99&gt;0), E99-D99, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G99" s="33"/>
-    </row>
-    <row r="100" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B100" s="105"/>
-      <c r="C100" s="29"/>
-      <c r="D100" s="30"/>
-      <c r="E100" s="30"/>
-      <c r="F100" s="53">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G100" s="34"/>
-    </row>
-    <row r="101" spans="2:8" ht="15">
-      <c r="B101" s="105"/>
+      <c r="D100" s="28">
+        <v>27273</v>
+      </c>
+      <c r="E100" s="28">
+        <v>31052</v>
+      </c>
+      <c r="F100" s="52">
+        <f t="shared" ref="F100:F113" si="8">IF(AND(D100&gt;0,E100&gt;0), E100-D100, 0)</f>
+        <v>3779</v>
+      </c>
+      <c r="G100" s="33"/>
+    </row>
+    <row r="101" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B101" s="109"/>
       <c r="C101" s="29"/>
       <c r="D101" s="30"/>
       <c r="E101" s="30"/>
-      <c r="F101" s="52">
-        <f t="shared" si="7"/>
+      <c r="F101" s="53">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G101" s="34"/>
-      <c r="H101" s="41"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="105"/>
+      <c r="B102" s="109"/>
       <c r="C102" s="29"/>
       <c r="D102" s="30"/>
       <c r="E102" s="30"/>
       <c r="F102" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G102" s="34"/>
-    </row>
-    <row r="103" spans="2:8" ht="15" customHeight="1">
-      <c r="B103" s="105"/>
+      <c r="H102" s="41"/>
+    </row>
+    <row r="103" spans="2:8" ht="15">
+      <c r="B103" s="109"/>
       <c r="C103" s="29"/>
       <c r="D103" s="30"/>
       <c r="E103" s="30"/>
       <c r="F103" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G103" s="34"/>
     </row>
-    <row r="104" spans="2:8" ht="15">
-      <c r="B104" s="105"/>
+    <row r="104" spans="2:8" ht="15" customHeight="1">
+      <c r="B104" s="109"/>
       <c r="C104" s="29"/>
       <c r="D104" s="30"/>
       <c r="E104" s="30"/>
       <c r="F104" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="105"/>
+      <c r="B105" s="109"/>
       <c r="C105" s="29"/>
       <c r="D105" s="30"/>
       <c r="E105" s="30"/>
       <c r="F105" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="105"/>
+      <c r="B106" s="109"/>
       <c r="C106" s="29"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
       <c r="F106" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="105"/>
+      <c r="B107" s="109"/>
       <c r="C107" s="29"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
       <c r="F107" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="105"/>
+      <c r="B108" s="109"/>
       <c r="C108" s="29"/>
       <c r="D108" s="30"/>
       <c r="E108" s="30"/>
       <c r="F108" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="105"/>
+      <c r="B109" s="109"/>
       <c r="C109" s="29"/>
       <c r="D109" s="30"/>
       <c r="E109" s="30"/>
       <c r="F109" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="105"/>
+      <c r="B110" s="109"/>
       <c r="C110" s="29"/>
       <c r="D110" s="30"/>
       <c r="E110" s="30"/>
       <c r="F110" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="105"/>
+      <c r="B111" s="109"/>
       <c r="C111" s="29"/>
       <c r="D111" s="30"/>
       <c r="E111" s="30"/>
       <c r="F111" s="52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G111" s="34"/>
     </row>
-    <row r="112" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B112" s="105"/>
-      <c r="C112" s="27" t="s">
+    <row r="112" spans="2:8" ht="15">
+      <c r="B112" s="109"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="30"/>
+      <c r="F112" s="52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G112" s="34"/>
+    </row>
+    <row r="113" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B113" s="109"/>
+      <c r="C113" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-      <c r="F112" s="54">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G112" s="33"/>
-    </row>
-    <row r="113" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B113" s="45">
-        <v>6</v>
-      </c>
-      <c r="C113" s="31" t="s">
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="54">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G113" s="33"/>
+    </row>
+    <row r="114" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B114" s="46">
+        <v>7</v>
+      </c>
+      <c r="C114" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D113" s="32">
-        <f>D112-D99</f>
-        <v>0</v>
-      </c>
-      <c r="E113" s="32">
-        <f>E112-E99</f>
-        <v>0</v>
-      </c>
-      <c r="F113" s="32">
-        <f>F112-F99</f>
-        <v>0</v>
-      </c>
-      <c r="G113" s="36"/>
-    </row>
-    <row r="114" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="106" t="s">
-        <v>19</v>
-      </c>
-      <c r="C115" s="38" t="s">
+      <c r="D114" s="32">
+        <f>D113-D100</f>
+        <v>-27273</v>
+      </c>
+      <c r="E114" s="32">
+        <f>E113-E100</f>
+        <v>-31052</v>
+      </c>
+      <c r="F114" s="32">
+        <f>F113-F100</f>
+        <v>-3779</v>
+      </c>
+      <c r="G114" s="37"/>
+    </row>
+    <row r="115" spans="2:8" ht="13.5" thickBot="1"/>
+    <row r="116" spans="2:8" ht="15">
+      <c r="B116" s="106" t="s">
+        <v>20</v>
+      </c>
+      <c r="C116" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D115" s="39" t="s">
+      <c r="D116" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E115" s="39" t="s">
+      <c r="E116" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F115" s="39" t="s">
+      <c r="F116" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G115" s="40" t="s">
+      <c r="G116" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B116" s="107"/>
-      <c r="C116" s="27" t="s">
+    <row r="117" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B117" s="107"/>
+      <c r="C117" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="52">
-        <f t="shared" ref="F116:F129" si="8">IF(AND(D116&gt;0,E116&gt;0), E116-D116, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G116" s="33"/>
-    </row>
-    <row r="117" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B117" s="107"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="53">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G117" s="34"/>
-    </row>
-    <row r="118" spans="2:8" ht="15">
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="52">
+        <f t="shared" ref="F117:F130" si="9">IF(AND(D117&gt;0,E117&gt;0), E117-D117, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G117" s="33"/>
+    </row>
+    <row r="118" spans="2:8" ht="15.75" thickTop="1">
       <c r="B118" s="107"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
-      <c r="F118" s="52">
-        <f t="shared" si="8"/>
+      <c r="F118" s="53">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G118" s="34"/>
-      <c r="H118" s="41"/>
     </row>
     <row r="119" spans="2:8" ht="15">
       <c r="B119" s="107"/>
@@ -3854,29 +4009,30 @@
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
       <c r="F119" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G119" s="34"/>
-    </row>
-    <row r="120" spans="2:8" ht="15" customHeight="1">
+      <c r="H119" s="41"/>
+    </row>
+    <row r="120" spans="2:8" ht="15">
       <c r="B120" s="107"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
       <c r="F120" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G120" s="34"/>
     </row>
-    <row r="121" spans="2:8" ht="15">
+    <row r="121" spans="2:8" ht="15" customHeight="1">
       <c r="B121" s="107"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
       <c r="F121" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G121" s="34"/>
@@ -3887,7 +4043,7 @@
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
       <c r="F122" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G122" s="34"/>
@@ -3898,7 +4054,7 @@
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
       <c r="F123" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G123" s="34"/>
@@ -3909,7 +4065,7 @@
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
       <c r="F124" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G124" s="34"/>
@@ -3920,7 +4076,7 @@
       <c r="D125" s="30"/>
       <c r="E125" s="30"/>
       <c r="F125" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G125" s="34"/>
@@ -3931,7 +4087,7 @@
       <c r="D126" s="30"/>
       <c r="E126" s="30"/>
       <c r="F126" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G126" s="34"/>
@@ -3942,7 +4098,7 @@
       <c r="D127" s="30"/>
       <c r="E127" s="30"/>
       <c r="F127" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G127" s="34"/>
@@ -3953,248 +4109,58 @@
       <c r="D128" s="30"/>
       <c r="E128" s="30"/>
       <c r="F128" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G128" s="34"/>
     </row>
-    <row r="129" spans="2:8" ht="15.75" thickBot="1">
+    <row r="129" spans="2:8" ht="15">
       <c r="B129" s="107"/>
-      <c r="C129" s="27" t="s">
+      <c r="C129" s="29"/>
+      <c r="D129" s="30"/>
+      <c r="E129" s="30"/>
+      <c r="F129" s="52">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G129" s="34"/>
+    </row>
+    <row r="130" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B130" s="107"/>
+      <c r="C130" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D129" s="28"/>
-      <c r="E129" s="28"/>
-      <c r="F129" s="54">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G129" s="33"/>
-    </row>
-    <row r="130" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B130" s="46">
-        <v>7</v>
-      </c>
-      <c r="C130" s="31" t="s">
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G130" s="33"/>
+    </row>
+    <row r="131" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B131" s="45">
+        <v>8</v>
+      </c>
+      <c r="C131" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D130" s="32">
-        <f>D129-D116</f>
-        <v>0</v>
-      </c>
-      <c r="E130" s="32">
-        <f>E129-E116</f>
-        <v>0</v>
-      </c>
-      <c r="F130" s="32">
-        <f>F129-F116</f>
-        <v>0</v>
-      </c>
-      <c r="G130" s="37"/>
-    </row>
-    <row r="131" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="104" t="s">
-        <v>20</v>
-      </c>
-      <c r="C132" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D132" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E132" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="F132" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G132" s="44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="133" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B133" s="105"/>
-      <c r="C133" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D133" s="28"/>
-      <c r="E133" s="28"/>
-      <c r="F133" s="52">
-        <f t="shared" ref="F133:F146" si="9">IF(AND(D133&gt;0,E133&gt;0), E133-D133, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G133" s="33"/>
-    </row>
-    <row r="134" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B134" s="105"/>
-      <c r="C134" s="29"/>
-      <c r="D134" s="30"/>
-      <c r="E134" s="30"/>
-      <c r="F134" s="53">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G134" s="34"/>
-    </row>
-    <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="105"/>
-      <c r="C135" s="29"/>
-      <c r="D135" s="30"/>
-      <c r="E135" s="30"/>
-      <c r="F135" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G135" s="34"/>
-      <c r="H135" s="41"/>
-    </row>
-    <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="105"/>
-      <c r="C136" s="29"/>
-      <c r="D136" s="30"/>
-      <c r="E136" s="30"/>
-      <c r="F136" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G136" s="34"/>
-    </row>
-    <row r="137" spans="2:8" ht="15" customHeight="1">
-      <c r="B137" s="105"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="30"/>
-      <c r="E137" s="30"/>
-      <c r="F137" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G137" s="34"/>
-    </row>
-    <row r="138" spans="2:8" ht="15">
-      <c r="B138" s="105"/>
-      <c r="C138" s="29"/>
-      <c r="D138" s="30"/>
-      <c r="E138" s="30"/>
-      <c r="F138" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G138" s="34"/>
-    </row>
-    <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="105"/>
-      <c r="C139" s="29"/>
-      <c r="D139" s="30"/>
-      <c r="E139" s="30"/>
-      <c r="F139" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G139" s="34"/>
-    </row>
-    <row r="140" spans="2:8" ht="15">
-      <c r="B140" s="105"/>
-      <c r="C140" s="29"/>
-      <c r="D140" s="30"/>
-      <c r="E140" s="30"/>
-      <c r="F140" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G140" s="34"/>
-    </row>
-    <row r="141" spans="2:8" ht="15">
-      <c r="B141" s="105"/>
-      <c r="C141" s="29"/>
-      <c r="D141" s="30"/>
-      <c r="E141" s="30"/>
-      <c r="F141" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G141" s="34"/>
-    </row>
-    <row r="142" spans="2:8" ht="15">
-      <c r="B142" s="105"/>
-      <c r="C142" s="29"/>
-      <c r="D142" s="30"/>
-      <c r="E142" s="30"/>
-      <c r="F142" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G142" s="34"/>
-    </row>
-    <row r="143" spans="2:8" ht="15">
-      <c r="B143" s="105"/>
-      <c r="C143" s="29"/>
-      <c r="D143" s="30"/>
-      <c r="E143" s="30"/>
-      <c r="F143" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G143" s="34"/>
-    </row>
-    <row r="144" spans="2:8" ht="15">
-      <c r="B144" s="105"/>
-      <c r="C144" s="29"/>
-      <c r="D144" s="30"/>
-      <c r="E144" s="30"/>
-      <c r="F144" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G144" s="34"/>
-    </row>
-    <row r="145" spans="2:8" ht="15">
-      <c r="B145" s="105"/>
-      <c r="C145" s="29"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="30"/>
-      <c r="F145" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G145" s="34"/>
-    </row>
-    <row r="146" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B146" s="105"/>
-      <c r="C146" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D146" s="28"/>
-      <c r="E146" s="28"/>
-      <c r="F146" s="54">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G146" s="33"/>
-    </row>
-    <row r="147" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B147" s="45">
-        <v>8</v>
-      </c>
-      <c r="C147" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D147" s="32">
-        <f>D146-D133</f>
-        <v>0</v>
-      </c>
-      <c r="E147" s="32">
-        <f>E146-E133</f>
-        <v>0</v>
-      </c>
-      <c r="F147" s="32">
-        <f>F146-F133</f>
-        <v>0</v>
-      </c>
-      <c r="G147" s="36"/>
-    </row>
-    <row r="152" spans="2:8">
-      <c r="H152" s="41"/>
+      <c r="D131" s="32">
+        <f>D130-D117</f>
+        <v>0</v>
+      </c>
+      <c r="E131" s="32">
+        <f>E130-E117</f>
+        <v>0</v>
+      </c>
+      <c r="F131" s="32">
+        <f>F130-F117</f>
+        <v>0</v>
+      </c>
+      <c r="G131" s="36"/>
+    </row>
+    <row r="136" spans="2:8">
+      <c r="H136" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4202,14 +4168,14 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B115:B129"/>
+    <mergeCell ref="B99:B113"/>
     <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B132:B146"/>
+    <mergeCell ref="B81:B87"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B116:B130"/>
     <mergeCell ref="B19:B29"/>
     <mergeCell ref="B43:B61"/>
     <mergeCell ref="B64:B78"/>
-    <mergeCell ref="B81:B95"/>
-    <mergeCell ref="B98:B112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4235,51 +4201,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="119"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="121"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="116"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="118"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4393,19 +4359,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="114" t="s">
+      <c r="A11" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="115"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="116"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="118"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4519,19 +4485,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="114" t="s">
+      <c r="A19" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="115"/>
-      <c r="I19" s="115"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="116"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="118"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4645,19 +4611,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="114" t="s">
+      <c r="A27" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="115"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="116"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="118"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4771,19 +4737,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="114" t="s">
+      <c r="A35" s="116" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="115"/>
-      <c r="C35" s="115"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="115"/>
-      <c r="F35" s="115"/>
-      <c r="G35" s="115"/>
-      <c r="H35" s="115"/>
-      <c r="I35" s="115"/>
-      <c r="J35" s="115"/>
-      <c r="K35" s="116"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="118"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -4895,19 +4861,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="114" t="s">
+      <c r="A43" s="116" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="115"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="115"/>
-      <c r="E43" s="115"/>
-      <c r="F43" s="115"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="115"/>
-      <c r="I43" s="115"/>
-      <c r="J43" s="115"/>
-      <c r="K43" s="116"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="117"/>
+      <c r="F43" s="117"/>
+      <c r="G43" s="117"/>
+      <c r="H43" s="117"/>
+      <c r="I43" s="117"/>
+      <c r="J43" s="117"/>
+      <c r="K43" s="118"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -5021,19 +4987,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="115"/>
-      <c r="C51" s="115"/>
-      <c r="D51" s="115"/>
-      <c r="E51" s="115"/>
-      <c r="F51" s="115"/>
-      <c r="G51" s="115"/>
-      <c r="H51" s="115"/>
-      <c r="I51" s="115"/>
-      <c r="J51" s="115"/>
-      <c r="K51" s="116"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="117"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="117"/>
+      <c r="G51" s="117"/>
+      <c r="H51" s="117"/>
+      <c r="I51" s="117"/>
+      <c r="J51" s="117"/>
+      <c r="K51" s="118"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -5153,19 +5119,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="114" t="s">
+      <c r="A59" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="115"/>
-      <c r="C59" s="115"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="115"/>
-      <c r="F59" s="115"/>
-      <c r="G59" s="115"/>
-      <c r="H59" s="115"/>
-      <c r="I59" s="115"/>
-      <c r="J59" s="115"/>
-      <c r="K59" s="116"/>
+      <c r="B59" s="117"/>
+      <c r="C59" s="117"/>
+      <c r="D59" s="117"/>
+      <c r="E59" s="117"/>
+      <c r="F59" s="117"/>
+      <c r="G59" s="117"/>
+      <c r="H59" s="117"/>
+      <c r="I59" s="117"/>
+      <c r="J59" s="117"/>
+      <c r="K59" s="118"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -5275,19 +5241,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="114" t="s">
+      <c r="A67" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="115"/>
-      <c r="C67" s="115"/>
-      <c r="D67" s="115"/>
-      <c r="E67" s="115"/>
-      <c r="F67" s="115"/>
-      <c r="G67" s="115"/>
-      <c r="H67" s="115"/>
-      <c r="I67" s="115"/>
-      <c r="J67" s="115"/>
-      <c r="K67" s="116"/>
+      <c r="B67" s="117"/>
+      <c r="C67" s="117"/>
+      <c r="D67" s="117"/>
+      <c r="E67" s="117"/>
+      <c r="F67" s="117"/>
+      <c r="G67" s="117"/>
+      <c r="H67" s="117"/>
+      <c r="I67" s="117"/>
+      <c r="J67" s="117"/>
+      <c r="K67" s="118"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5395,19 +5361,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="114" t="s">
+      <c r="A75" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="115"/>
-      <c r="C75" s="115"/>
-      <c r="D75" s="115"/>
-      <c r="E75" s="115"/>
-      <c r="F75" s="115"/>
-      <c r="G75" s="115"/>
-      <c r="H75" s="115"/>
-      <c r="I75" s="115"/>
-      <c r="J75" s="115"/>
-      <c r="K75" s="116"/>
+      <c r="B75" s="117"/>
+      <c r="C75" s="117"/>
+      <c r="D75" s="117"/>
+      <c r="E75" s="117"/>
+      <c r="F75" s="117"/>
+      <c r="G75" s="117"/>
+      <c r="H75" s="117"/>
+      <c r="I75" s="117"/>
+      <c r="J75" s="117"/>
+      <c r="K75" s="118"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5523,19 +5489,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="114" t="s">
+      <c r="A83" s="116" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="115"/>
-      <c r="C83" s="115"/>
-      <c r="D83" s="115"/>
-      <c r="E83" s="115"/>
-      <c r="F83" s="115"/>
-      <c r="G83" s="115"/>
-      <c r="H83" s="115"/>
-      <c r="I83" s="115"/>
-      <c r="J83" s="115"/>
-      <c r="K83" s="116"/>
+      <c r="B83" s="117"/>
+      <c r="C83" s="117"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="117"/>
+      <c r="F83" s="117"/>
+      <c r="G83" s="117"/>
+      <c r="H83" s="117"/>
+      <c r="I83" s="117"/>
+      <c r="J83" s="117"/>
+      <c r="K83" s="118"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5647,19 +5613,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="114" t="s">
+      <c r="A91" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="115"/>
-      <c r="C91" s="115"/>
-      <c r="D91" s="115"/>
-      <c r="E91" s="115"/>
-      <c r="F91" s="115"/>
-      <c r="G91" s="115"/>
-      <c r="H91" s="115"/>
-      <c r="I91" s="115"/>
-      <c r="J91" s="115"/>
-      <c r="K91" s="116"/>
+      <c r="B91" s="117"/>
+      <c r="C91" s="117"/>
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="117"/>
+      <c r="G91" s="117"/>
+      <c r="H91" s="117"/>
+      <c r="I91" s="117"/>
+      <c r="J91" s="117"/>
+      <c r="K91" s="118"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5773,19 +5739,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="114" t="s">
+      <c r="A99" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="115"/>
-      <c r="C99" s="115"/>
-      <c r="D99" s="115"/>
-      <c r="E99" s="115"/>
-      <c r="F99" s="115"/>
-      <c r="G99" s="115"/>
-      <c r="H99" s="115"/>
-      <c r="I99" s="115"/>
-      <c r="J99" s="115"/>
-      <c r="K99" s="116"/>
+      <c r="B99" s="117"/>
+      <c r="C99" s="117"/>
+      <c r="D99" s="117"/>
+      <c r="E99" s="117"/>
+      <c r="F99" s="117"/>
+      <c r="G99" s="117"/>
+      <c r="H99" s="117"/>
+      <c r="I99" s="117"/>
+      <c r="J99" s="117"/>
+      <c r="K99" s="118"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -5889,19 +5855,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="114" t="s">
+      <c r="A107" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="115"/>
-      <c r="C107" s="115"/>
-      <c r="D107" s="115"/>
-      <c r="E107" s="115"/>
-      <c r="F107" s="115"/>
-      <c r="G107" s="115"/>
-      <c r="H107" s="115"/>
-      <c r="I107" s="115"/>
-      <c r="J107" s="115"/>
-      <c r="K107" s="116"/>
+      <c r="B107" s="117"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="117"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="117"/>
+      <c r="J107" s="117"/>
+      <c r="K107" s="118"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -6023,7 +5989,7 @@
     <mergeCell ref="A99:K99"/>
     <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6238,7 +6204,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6265,10 +6231,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="122"/>
+      <c r="C1" s="124"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6279,7 +6245,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="125" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6293,7 +6259,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6305,7 +6271,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6314,7 +6280,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6326,7 +6292,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6338,7 +6304,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6347,7 +6313,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="125"/>
+      <c r="A9" s="127"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6362,7 +6328,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="125" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6376,7 +6342,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6388,7 +6354,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6397,7 +6363,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6409,7 +6375,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6421,7 +6387,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="124"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6430,7 +6396,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="125"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6445,7 +6411,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="123" t="s">
+      <c r="A19" s="125" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6454,7 +6420,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="124"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6464,14 +6430,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="124"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="124"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6481,7 +6447,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="124"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6491,14 +6457,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="124"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="125"/>
+      <c r="A25" s="127"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6511,7 +6477,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6533,147 +6499,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="136"/>
+      <c r="B1" s="138"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="133"/>
+      <c r="B2" s="135"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="134" t="s">
+      <c r="A3" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="133"/>
+      <c r="B3" s="135"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+      <c r="A4" s="141"/>
+      <c r="B4" s="142"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="138"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="143" t="s">
+      <c r="A7" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="144"/>
+      <c r="B7" s="146"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="141" t="s">
+      <c r="A9" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="142"/>
+      <c r="B9" s="144"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="128"/>
-      <c r="B10" s="129"/>
+      <c r="A10" s="130"/>
+      <c r="B10" s="131"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="130" t="s">
+      <c r="A11" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="131"/>
+      <c r="B11" s="133"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="130" t="s">
+      <c r="A12" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="131"/>
+      <c r="B12" s="133"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="130" t="s">
+      <c r="A13" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="131"/>
+      <c r="B13" s="133"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="130" t="s">
+      <c r="A14" s="132" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="131"/>
+      <c r="B14" s="133"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="130" t="s">
+      <c r="A15" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="131"/>
+      <c r="B15" s="133"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="132" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="131"/>
+      <c r="B16" s="133"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="127"/>
+      <c r="B17" s="129"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="144"/>
+      <c r="B19" s="146"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="141" t="s">
+      <c r="A21" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="142"/>
+      <c r="B21" s="144"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="128"/>
-      <c r="B22" s="129"/>
+      <c r="A22" s="130"/>
+      <c r="B22" s="131"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="130" t="s">
+      <c r="A23" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="131"/>
+      <c r="B23" s="133"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="130"/>
-      <c r="B24" s="131"/>
+      <c r="A24" s="132"/>
+      <c r="B24" s="133"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="131"/>
+      <c r="B25" s="133"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="130" t="s">
+      <c r="A26" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="131"/>
+      <c r="B26" s="133"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="126"/>
-      <c r="B27" s="127"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Terminator - More of level 7 done
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="154">
   <si>
     <t>Notes</t>
   </si>
@@ -591,6 +591,18 @@
   <si>
     <t>X = 4394, Y = 131</t>
   </si>
+  <si>
+    <t>X = 1287</t>
+  </si>
+  <si>
+    <t>X = 726</t>
+  </si>
+  <si>
+    <t>X = 872/870</t>
+  </si>
+  <si>
+    <t>X = 896</t>
+  </si>
 </sst>
 </file>
 
@@ -600,10 +612,24 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1313,14 +1339,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1328,7 +1354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1336,75 +1362,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1414,10 +1440,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1438,69 +1464,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1510,66 +1542,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1577,47 +1612,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Färg1" xfId="2" builtinId="29"/>
-    <cellStyle name="Hyperlänk" xfId="3" builtinId="8"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Summa" xfId="1" builtinId="25"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1632,7 +1664,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1918,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1933,16 +1965,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="110"/>
-      <c r="D1" s="111" t="s">
+      <c r="C1" s="113"/>
+      <c r="D1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="112"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="115"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
         <f>SUM(H1:H65518)</f>
@@ -2020,10 +2052,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="113"/>
+      <c r="E5" s="116"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2060,7 +2092,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="117" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2080,7 +2112,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="115"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2090,7 +2122,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="115"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2101,7 +2133,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="115"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2112,7 +2144,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="115"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2123,7 +2155,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="115"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2134,7 +2166,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="115"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2145,7 +2177,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="115"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2156,7 +2188,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="115"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2199,7 +2231,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="111" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2234,7 +2266,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="109"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2267,7 +2299,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="109"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2300,7 +2332,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="109"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2333,7 +2365,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="109"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2366,7 +2398,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="109"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2402,7 +2434,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="109"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2435,7 +2467,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="109"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2468,7 +2500,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="109"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2501,7 +2533,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="109"/>
+      <c r="B28" s="112"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2534,7 +2566,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="109"/>
+      <c r="B29" s="112"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2560,7 +2592,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="109" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2595,7 +2627,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="107"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2624,7 +2656,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="107"/>
+      <c r="B33" s="110"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2653,7 +2685,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="107"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2683,7 +2715,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="107"/>
+      <c r="B35" s="110"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2703,7 +2735,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="107"/>
+      <c r="B36" s="110"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2723,7 +2755,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="107"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2746,7 +2778,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="107"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2769,7 +2801,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="107"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2837,7 +2869,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="111" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2857,7 +2889,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="109"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2874,7 +2906,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="109"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2891,7 +2923,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="109"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2909,7 +2941,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="109"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -2926,7 +2958,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="109"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -2943,7 +2975,7 @@
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:13" ht="15">
-      <c r="B49" s="109"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -2960,7 +2992,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:13" ht="15">
-      <c r="B50" s="109"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
@@ -2977,7 +3009,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:13" ht="15">
-      <c r="B51" s="109"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
@@ -2994,7 +3026,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:13" ht="15">
-      <c r="B52" s="109"/>
+      <c r="B52" s="112"/>
       <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
@@ -3011,7 +3043,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:13" ht="15">
-      <c r="B53" s="109"/>
+      <c r="B53" s="112"/>
       <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
@@ -3028,7 +3060,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:13" ht="15">
-      <c r="B54" s="109"/>
+      <c r="B54" s="112"/>
       <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
@@ -3045,7 +3077,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:13" ht="15">
-      <c r="B55" s="109"/>
+      <c r="B55" s="112"/>
       <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
@@ -3062,7 +3094,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:13" ht="15">
-      <c r="B56" s="109"/>
+      <c r="B56" s="112"/>
       <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
@@ -3079,7 +3111,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:13" ht="15">
-      <c r="B57" s="109"/>
+      <c r="B57" s="112"/>
       <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
@@ -3096,7 +3128,7 @@
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="2:13" ht="15">
-      <c r="B58" s="109"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
@@ -3116,7 +3148,7 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="15">
-      <c r="B59" s="109"/>
+      <c r="B59" s="112"/>
       <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
@@ -3133,7 +3165,7 @@
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:13" ht="15">
-      <c r="B60" s="109"/>
+      <c r="B60" s="112"/>
       <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
@@ -3150,7 +3182,7 @@
       <c r="G60" s="34"/>
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B61" s="109"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3189,7 +3221,7 @@
     </row>
     <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
     <row r="64" spans="2:13" ht="15">
-      <c r="B64" s="106" t="s">
+      <c r="B64" s="109" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3209,7 +3241,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="107"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3229,7 +3261,7 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="107"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
@@ -3246,7 +3278,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="107"/>
+      <c r="B67" s="110"/>
       <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
@@ -3260,7 +3292,7 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="107"/>
+      <c r="B68" s="110"/>
       <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
@@ -3277,7 +3309,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="107"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
@@ -3294,7 +3326,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="107"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
@@ -3314,7 +3346,7 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="107"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
@@ -3331,7 +3363,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="107"/>
+      <c r="B72" s="110"/>
       <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
@@ -3348,7 +3380,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="107"/>
+      <c r="B73" s="110"/>
       <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
@@ -3365,7 +3397,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="107"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
@@ -3382,7 +3414,7 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="107"/>
+      <c r="B75" s="110"/>
       <c r="C75" s="105" t="s">
         <v>139</v>
       </c>
@@ -3399,7 +3431,7 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="107"/>
+      <c r="B76" s="110"/>
       <c r="C76" s="105" t="s">
         <v>140</v>
       </c>
@@ -3416,7 +3448,7 @@
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="107"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3427,7 +3459,7 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="107"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
@@ -3466,7 +3498,7 @@
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="81" spans="2:9" ht="15" customHeight="1">
-      <c r="B81" s="108" t="s">
+      <c r="B81" s="111" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3486,7 +3518,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B82" s="109"/>
+      <c r="B82" s="112"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
@@ -3503,8 +3535,8 @@
       <c r="G82" s="33"/>
     </row>
     <row r="83" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B83" s="109"/>
-      <c r="C83" s="147" t="s">
+      <c r="B83" s="112"/>
+      <c r="C83" s="106" t="s">
         <v>141</v>
       </c>
       <c r="D83" s="30">
@@ -3520,8 +3552,8 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:9" ht="15">
-      <c r="B84" s="109"/>
-      <c r="C84" s="147" t="s">
+      <c r="B84" s="112"/>
+      <c r="C84" s="106" t="s">
         <v>142</v>
       </c>
       <c r="D84" s="30"/>
@@ -3536,8 +3568,8 @@
       <c r="H84" s="41"/>
     </row>
     <row r="85" spans="2:9" ht="15">
-      <c r="B85" s="109"/>
-      <c r="C85" s="147" t="s">
+      <c r="B85" s="112"/>
+      <c r="C85" s="106" t="s">
         <v>143</v>
       </c>
       <c r="D85" s="30">
@@ -3553,8 +3585,8 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:9" ht="15" customHeight="1">
-      <c r="B86" s="109"/>
-      <c r="C86" s="147" t="s">
+      <c r="B86" s="112"/>
+      <c r="C86" s="106" t="s">
         <v>144</v>
       </c>
       <c r="D86" s="30">
@@ -3570,8 +3602,8 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="109"/>
-      <c r="C87" s="147" t="s">
+      <c r="B87" s="112"/>
+      <c r="C87" s="106" t="s">
         <v>145</v>
       </c>
       <c r="D87" s="30">
@@ -3587,7 +3619,7 @@
       <c r="G87" s="34"/>
     </row>
     <row r="88" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B88" s="148"/>
+      <c r="B88" s="107"/>
       <c r="C88" s="27" t="s">
         <v>32</v>
       </c>
@@ -3629,7 +3661,7 @@
     </row>
     <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="91" spans="2:9" ht="15" customHeight="1">
-      <c r="B91" s="106" t="s">
+      <c r="B91" s="109" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="42" t="s">
@@ -3649,7 +3681,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B92" s="107"/>
+      <c r="B92" s="110"/>
       <c r="C92" s="27" t="s">
         <v>29</v>
       </c>
@@ -3666,8 +3698,8 @@
       <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B93" s="107"/>
-      <c r="C93" s="147" t="s">
+      <c r="B93" s="110"/>
+      <c r="C93" s="106" t="s">
         <v>147</v>
       </c>
       <c r="D93" s="30">
@@ -3683,8 +3715,8 @@
       <c r="G93" s="34"/>
     </row>
     <row r="94" spans="2:9" ht="15">
-      <c r="B94" s="107"/>
-      <c r="C94" s="147" t="s">
+      <c r="B94" s="110"/>
+      <c r="C94" s="106" t="s">
         <v>148</v>
       </c>
       <c r="D94" s="30">
@@ -3701,8 +3733,8 @@
       <c r="H94" s="41"/>
     </row>
     <row r="95" spans="2:9" ht="15">
-      <c r="B95" s="107"/>
-      <c r="C95" s="147" t="s">
+      <c r="B95" s="110"/>
+      <c r="C95" s="106" t="s">
         <v>149</v>
       </c>
       <c r="D95" s="30"/>
@@ -3755,7 +3787,7 @@
     </row>
     <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="108" t="s">
+      <c r="B99" s="111" t="s">
         <v>19</v>
       </c>
       <c r="C99" s="38" t="s">
@@ -3775,7 +3807,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="109"/>
+      <c r="B100" s="112"/>
       <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
@@ -3792,107 +3824,161 @@
       <c r="G100" s="33"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="109"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="30"/>
+      <c r="B101" s="112"/>
+      <c r="C101" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" s="30">
+        <v>27529</v>
+      </c>
+      <c r="E101" s="30">
+        <v>31313</v>
+      </c>
       <c r="F101" s="53">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3784</v>
       </c>
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="109"/>
-      <c r="C102" s="29"/>
-      <c r="D102" s="30"/>
-      <c r="E102" s="30"/>
+      <c r="B102" s="112"/>
+      <c r="C102" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="D102" s="30">
+        <v>27661</v>
+      </c>
+      <c r="E102" s="30">
+        <v>31445</v>
+      </c>
       <c r="F102" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3784</v>
       </c>
       <c r="G102" s="34"/>
       <c r="H102" s="41"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="109"/>
-      <c r="C103" s="29"/>
-      <c r="D103" s="30"/>
-      <c r="E103" s="30"/>
+      <c r="B103" s="112"/>
+      <c r="C103" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="D103" s="30">
+        <v>27854</v>
+      </c>
+      <c r="E103" s="30">
+        <v>31693</v>
+      </c>
       <c r="F103" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3839</v>
       </c>
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="109"/>
-      <c r="C104" s="29"/>
-      <c r="D104" s="30"/>
-      <c r="E104" s="30"/>
+      <c r="B104" s="112"/>
+      <c r="C104" s="150" t="s">
+        <v>152</v>
+      </c>
+      <c r="D104" s="30">
+        <v>28190</v>
+      </c>
+      <c r="E104" s="30">
+        <v>32042</v>
+      </c>
       <c r="F104" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3852</v>
       </c>
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="109"/>
-      <c r="C105" s="29"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
+      <c r="B105" s="112"/>
+      <c r="C105" s="150" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105" s="30">
+        <v>28344</v>
+      </c>
+      <c r="E105" s="30">
+        <v>32200</v>
+      </c>
       <c r="F105" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3856</v>
       </c>
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="109"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="30"/>
+      <c r="B106" s="112"/>
+      <c r="C106" s="150" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106" s="30">
+        <v>28456</v>
+      </c>
+      <c r="E106" s="30">
+        <v>32315</v>
+      </c>
       <c r="F106" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3859</v>
       </c>
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="109"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="30"/>
+      <c r="B107" s="112"/>
+      <c r="C107" s="150" t="s">
+        <v>121</v>
+      </c>
+      <c r="D107" s="30">
+        <v>28576</v>
+      </c>
+      <c r="E107" s="30">
+        <v>32436</v>
+      </c>
       <c r="F107" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3860</v>
       </c>
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="109"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="30"/>
+      <c r="B108" s="112"/>
+      <c r="C108" s="150" t="s">
+        <v>121</v>
+      </c>
+      <c r="D108" s="30">
+        <v>28712</v>
+      </c>
+      <c r="E108" s="30">
+        <v>32573</v>
+      </c>
       <c r="F108" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3861</v>
       </c>
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="109"/>
-      <c r="C109" s="29"/>
-      <c r="D109" s="30"/>
-      <c r="E109" s="30"/>
+      <c r="B109" s="112"/>
+      <c r="C109" s="150" t="s">
+        <v>153</v>
+      </c>
+      <c r="D109" s="30">
+        <v>28970</v>
+      </c>
+      <c r="E109" s="30">
+        <v>32861</v>
+      </c>
       <c r="F109" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3891</v>
       </c>
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="109"/>
+      <c r="B110" s="112"/>
       <c r="C110" s="29"/>
       <c r="D110" s="30"/>
       <c r="E110" s="30"/>
@@ -3903,7 +3989,7 @@
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="109"/>
+      <c r="B111" s="112"/>
       <c r="C111" s="29"/>
       <c r="D111" s="30"/>
       <c r="E111" s="30"/>
@@ -3914,7 +4000,7 @@
       <c r="G111" s="34"/>
     </row>
     <row r="112" spans="2:8" ht="15">
-      <c r="B112" s="109"/>
+      <c r="B112" s="112"/>
       <c r="C112" s="29"/>
       <c r="D112" s="30"/>
       <c r="E112" s="30"/>
@@ -3925,7 +4011,7 @@
       <c r="G112" s="34"/>
     </row>
     <row r="113" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B113" s="109"/>
+      <c r="B113" s="112"/>
       <c r="C113" s="27" t="s">
         <v>32</v>
       </c>
@@ -3960,7 +4046,7 @@
     </row>
     <row r="115" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="116" spans="2:8" ht="15">
-      <c r="B116" s="106" t="s">
+      <c r="B116" s="109" t="s">
         <v>20</v>
       </c>
       <c r="C116" s="42" t="s">
@@ -3980,7 +4066,7 @@
       </c>
     </row>
     <row r="117" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B117" s="107"/>
+      <c r="B117" s="110"/>
       <c r="C117" s="27" t="s">
         <v>29</v>
       </c>
@@ -3993,7 +4079,7 @@
       <c r="G117" s="33"/>
     </row>
     <row r="118" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B118" s="107"/>
+      <c r="B118" s="110"/>
       <c r="C118" s="29"/>
       <c r="D118" s="30"/>
       <c r="E118" s="30"/>
@@ -4004,7 +4090,7 @@
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:8" ht="15">
-      <c r="B119" s="107"/>
+      <c r="B119" s="110"/>
       <c r="C119" s="29"/>
       <c r="D119" s="30"/>
       <c r="E119" s="30"/>
@@ -4016,7 +4102,7 @@
       <c r="H119" s="41"/>
     </row>
     <row r="120" spans="2:8" ht="15">
-      <c r="B120" s="107"/>
+      <c r="B120" s="110"/>
       <c r="C120" s="29"/>
       <c r="D120" s="30"/>
       <c r="E120" s="30"/>
@@ -4027,7 +4113,7 @@
       <c r="G120" s="34"/>
     </row>
     <row r="121" spans="2:8" ht="15" customHeight="1">
-      <c r="B121" s="107"/>
+      <c r="B121" s="110"/>
       <c r="C121" s="29"/>
       <c r="D121" s="30"/>
       <c r="E121" s="30"/>
@@ -4038,7 +4124,7 @@
       <c r="G121" s="34"/>
     </row>
     <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="107"/>
+      <c r="B122" s="110"/>
       <c r="C122" s="29"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30"/>
@@ -4049,7 +4135,7 @@
       <c r="G122" s="34"/>
     </row>
     <row r="123" spans="2:8" ht="15">
-      <c r="B123" s="107"/>
+      <c r="B123" s="110"/>
       <c r="C123" s="29"/>
       <c r="D123" s="30"/>
       <c r="E123" s="30"/>
@@ -4060,7 +4146,7 @@
       <c r="G123" s="34"/>
     </row>
     <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="107"/>
+      <c r="B124" s="110"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
@@ -4071,7 +4157,7 @@
       <c r="G124" s="34"/>
     </row>
     <row r="125" spans="2:8" ht="15">
-      <c r="B125" s="107"/>
+      <c r="B125" s="110"/>
       <c r="C125" s="29"/>
       <c r="D125" s="30"/>
       <c r="E125" s="30"/>
@@ -4082,7 +4168,7 @@
       <c r="G125" s="34"/>
     </row>
     <row r="126" spans="2:8" ht="15">
-      <c r="B126" s="107"/>
+      <c r="B126" s="110"/>
       <c r="C126" s="29"/>
       <c r="D126" s="30"/>
       <c r="E126" s="30"/>
@@ -4093,7 +4179,7 @@
       <c r="G126" s="34"/>
     </row>
     <row r="127" spans="2:8" ht="15">
-      <c r="B127" s="107"/>
+      <c r="B127" s="110"/>
       <c r="C127" s="29"/>
       <c r="D127" s="30"/>
       <c r="E127" s="30"/>
@@ -4104,7 +4190,7 @@
       <c r="G127" s="34"/>
     </row>
     <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="107"/>
+      <c r="B128" s="110"/>
       <c r="C128" s="29"/>
       <c r="D128" s="30"/>
       <c r="E128" s="30"/>
@@ -4115,7 +4201,7 @@
       <c r="G128" s="34"/>
     </row>
     <row r="129" spans="2:8" ht="15">
-      <c r="B129" s="107"/>
+      <c r="B129" s="110"/>
       <c r="C129" s="29"/>
       <c r="D129" s="30"/>
       <c r="E129" s="30"/>
@@ -4126,7 +4212,7 @@
       <c r="G129" s="34"/>
     </row>
     <row r="130" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B130" s="107"/>
+      <c r="B130" s="110"/>
       <c r="C130" s="27" t="s">
         <v>32</v>
       </c>
@@ -4164,7 +4250,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
@@ -4176,6 +4261,7 @@
     <mergeCell ref="B19:B29"/>
     <mergeCell ref="B43:B61"/>
     <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4201,51 +4287,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="121"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="124"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="118"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="121"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4359,19 +4445,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="117"/>
-      <c r="C11" s="117"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="118"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="121"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4485,19 +4571,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="117"/>
-      <c r="J19" s="117"/>
-      <c r="K19" s="118"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="121"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4611,19 +4697,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
-      <c r="G27" s="117"/>
-      <c r="H27" s="117"/>
-      <c r="I27" s="117"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="118"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="121"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4737,19 +4823,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="116" t="s">
+      <c r="A35" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="117"/>
-      <c r="C35" s="117"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="117"/>
-      <c r="H35" s="117"/>
-      <c r="I35" s="117"/>
-      <c r="J35" s="117"/>
-      <c r="K35" s="118"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="121"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -4861,19 +4947,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="117"/>
-      <c r="C43" s="117"/>
-      <c r="D43" s="117"/>
-      <c r="E43" s="117"/>
-      <c r="F43" s="117"/>
-      <c r="G43" s="117"/>
-      <c r="H43" s="117"/>
-      <c r="I43" s="117"/>
-      <c r="J43" s="117"/>
-      <c r="K43" s="118"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120"/>
+      <c r="G43" s="120"/>
+      <c r="H43" s="120"/>
+      <c r="I43" s="120"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="121"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -4987,19 +5073,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="116" t="s">
+      <c r="A51" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="117"/>
-      <c r="C51" s="117"/>
-      <c r="D51" s="117"/>
-      <c r="E51" s="117"/>
-      <c r="F51" s="117"/>
-      <c r="G51" s="117"/>
-      <c r="H51" s="117"/>
-      <c r="I51" s="117"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="118"/>
+      <c r="B51" s="120"/>
+      <c r="C51" s="120"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="120"/>
+      <c r="F51" s="120"/>
+      <c r="G51" s="120"/>
+      <c r="H51" s="120"/>
+      <c r="I51" s="120"/>
+      <c r="J51" s="120"/>
+      <c r="K51" s="121"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -5119,19 +5205,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="116" t="s">
+      <c r="A59" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="117"/>
-      <c r="C59" s="117"/>
-      <c r="D59" s="117"/>
-      <c r="E59" s="117"/>
-      <c r="F59" s="117"/>
-      <c r="G59" s="117"/>
-      <c r="H59" s="117"/>
-      <c r="I59" s="117"/>
-      <c r="J59" s="117"/>
-      <c r="K59" s="118"/>
+      <c r="B59" s="120"/>
+      <c r="C59" s="120"/>
+      <c r="D59" s="120"/>
+      <c r="E59" s="120"/>
+      <c r="F59" s="120"/>
+      <c r="G59" s="120"/>
+      <c r="H59" s="120"/>
+      <c r="I59" s="120"/>
+      <c r="J59" s="120"/>
+      <c r="K59" s="121"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -5241,19 +5327,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="116" t="s">
+      <c r="A67" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="117"/>
-      <c r="C67" s="117"/>
-      <c r="D67" s="117"/>
-      <c r="E67" s="117"/>
-      <c r="F67" s="117"/>
-      <c r="G67" s="117"/>
-      <c r="H67" s="117"/>
-      <c r="I67" s="117"/>
-      <c r="J67" s="117"/>
-      <c r="K67" s="118"/>
+      <c r="B67" s="120"/>
+      <c r="C67" s="120"/>
+      <c r="D67" s="120"/>
+      <c r="E67" s="120"/>
+      <c r="F67" s="120"/>
+      <c r="G67" s="120"/>
+      <c r="H67" s="120"/>
+      <c r="I67" s="120"/>
+      <c r="J67" s="120"/>
+      <c r="K67" s="121"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5361,19 +5447,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="116" t="s">
+      <c r="A75" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="117"/>
-      <c r="C75" s="117"/>
-      <c r="D75" s="117"/>
-      <c r="E75" s="117"/>
-      <c r="F75" s="117"/>
-      <c r="G75" s="117"/>
-      <c r="H75" s="117"/>
-      <c r="I75" s="117"/>
-      <c r="J75" s="117"/>
-      <c r="K75" s="118"/>
+      <c r="B75" s="120"/>
+      <c r="C75" s="120"/>
+      <c r="D75" s="120"/>
+      <c r="E75" s="120"/>
+      <c r="F75" s="120"/>
+      <c r="G75" s="120"/>
+      <c r="H75" s="120"/>
+      <c r="I75" s="120"/>
+      <c r="J75" s="120"/>
+      <c r="K75" s="121"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5489,19 +5575,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="116" t="s">
+      <c r="A83" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="117"/>
-      <c r="C83" s="117"/>
-      <c r="D83" s="117"/>
-      <c r="E83" s="117"/>
-      <c r="F83" s="117"/>
-      <c r="G83" s="117"/>
-      <c r="H83" s="117"/>
-      <c r="I83" s="117"/>
-      <c r="J83" s="117"/>
-      <c r="K83" s="118"/>
+      <c r="B83" s="120"/>
+      <c r="C83" s="120"/>
+      <c r="D83" s="120"/>
+      <c r="E83" s="120"/>
+      <c r="F83" s="120"/>
+      <c r="G83" s="120"/>
+      <c r="H83" s="120"/>
+      <c r="I83" s="120"/>
+      <c r="J83" s="120"/>
+      <c r="K83" s="121"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5613,19 +5699,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="116" t="s">
+      <c r="A91" s="119" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="117"/>
-      <c r="C91" s="117"/>
-      <c r="D91" s="117"/>
-      <c r="E91" s="117"/>
-      <c r="F91" s="117"/>
-      <c r="G91" s="117"/>
-      <c r="H91" s="117"/>
-      <c r="I91" s="117"/>
-      <c r="J91" s="117"/>
-      <c r="K91" s="118"/>
+      <c r="B91" s="120"/>
+      <c r="C91" s="120"/>
+      <c r="D91" s="120"/>
+      <c r="E91" s="120"/>
+      <c r="F91" s="120"/>
+      <c r="G91" s="120"/>
+      <c r="H91" s="120"/>
+      <c r="I91" s="120"/>
+      <c r="J91" s="120"/>
+      <c r="K91" s="121"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5739,19 +5825,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="116" t="s">
+      <c r="A99" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="117"/>
-      <c r="C99" s="117"/>
-      <c r="D99" s="117"/>
-      <c r="E99" s="117"/>
-      <c r="F99" s="117"/>
-      <c r="G99" s="117"/>
-      <c r="H99" s="117"/>
-      <c r="I99" s="117"/>
-      <c r="J99" s="117"/>
-      <c r="K99" s="118"/>
+      <c r="B99" s="120"/>
+      <c r="C99" s="120"/>
+      <c r="D99" s="120"/>
+      <c r="E99" s="120"/>
+      <c r="F99" s="120"/>
+      <c r="G99" s="120"/>
+      <c r="H99" s="120"/>
+      <c r="I99" s="120"/>
+      <c r="J99" s="120"/>
+      <c r="K99" s="121"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -5855,19 +5941,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="116" t="s">
+      <c r="A107" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="117"/>
-      <c r="C107" s="117"/>
-      <c r="D107" s="117"/>
-      <c r="E107" s="117"/>
-      <c r="F107" s="117"/>
-      <c r="G107" s="117"/>
-      <c r="H107" s="117"/>
-      <c r="I107" s="117"/>
-      <c r="J107" s="117"/>
-      <c r="K107" s="118"/>
+      <c r="B107" s="120"/>
+      <c r="C107" s="120"/>
+      <c r="D107" s="120"/>
+      <c r="E107" s="120"/>
+      <c r="F107" s="120"/>
+      <c r="G107" s="120"/>
+      <c r="H107" s="120"/>
+      <c r="I107" s="120"/>
+      <c r="J107" s="120"/>
+      <c r="K107" s="121"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -5989,7 +6075,7 @@
     <mergeCell ref="A99:K99"/>
     <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6204,7 +6290,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6231,10 +6317,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="124"/>
+      <c r="C1" s="127"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6245,7 +6331,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="128" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6259,7 +6345,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="126"/>
+      <c r="A4" s="129"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6271,7 +6357,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="126"/>
+      <c r="A5" s="129"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6280,7 +6366,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="126"/>
+      <c r="A6" s="129"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6292,7 +6378,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="126"/>
+      <c r="A7" s="129"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6304,7 +6390,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="126"/>
+      <c r="A8" s="129"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6313,7 +6399,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="127"/>
+      <c r="A9" s="130"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6328,7 +6414,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="125" t="s">
+      <c r="A11" s="128" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6342,7 +6428,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="126"/>
+      <c r="A12" s="129"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6354,7 +6440,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="126"/>
+      <c r="A13" s="129"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6363,7 +6449,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="126"/>
+      <c r="A14" s="129"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6375,7 +6461,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="126"/>
+      <c r="A15" s="129"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6387,7 +6473,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="126"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6396,7 +6482,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="127"/>
+      <c r="A17" s="130"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6411,7 +6497,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="125" t="s">
+      <c r="A19" s="128" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6420,7 +6506,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="126"/>
+      <c r="A20" s="129"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6430,14 +6516,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="126"/>
+      <c r="A21" s="129"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="126"/>
+      <c r="A22" s="129"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6447,7 +6533,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="126"/>
+      <c r="A23" s="129"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6457,14 +6543,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="126"/>
+      <c r="A24" s="129"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="127"/>
+      <c r="A25" s="130"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6477,7 +6563,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6499,147 +6585,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="138"/>
+      <c r="B1" s="141"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="135"/>
+      <c r="B2" s="138"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="135"/>
+      <c r="B3" s="138"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="141"/>
-      <c r="B4" s="142"/>
+      <c r="A4" s="144"/>
+      <c r="B4" s="145"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="140"/>
+      <c r="B5" s="143"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="145" t="s">
+      <c r="A7" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="146"/>
+      <c r="B7" s="149"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="143" t="s">
+      <c r="A9" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="144"/>
+      <c r="B9" s="147"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="130"/>
-      <c r="B10" s="131"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="134"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="132" t="s">
+      <c r="A11" s="135" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="133"/>
+      <c r="B11" s="136"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="133"/>
+      <c r="B12" s="136"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="136"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="132" t="s">
+      <c r="A14" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="133"/>
+      <c r="B14" s="136"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="132" t="s">
+      <c r="A15" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="133"/>
+      <c r="B15" s="136"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="135" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="133"/>
+      <c r="B16" s="136"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="128" t="s">
+      <c r="A17" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="129"/>
+      <c r="B17" s="132"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="145" t="s">
+      <c r="A19" s="148" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="146"/>
+      <c r="B19" s="149"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="144"/>
+      <c r="B21" s="147"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="130"/>
-      <c r="B22" s="131"/>
+      <c r="A22" s="133"/>
+      <c r="B22" s="134"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="132" t="s">
+      <c r="A23" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="136"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="132"/>
-      <c r="B24" s="133"/>
+      <c r="A24" s="135"/>
+      <c r="B24" s="136"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="133"/>
+      <c r="B25" s="136"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="132" t="s">
+      <c r="A26" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="133"/>
+      <c r="B26" s="136"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="128"/>
-      <c r="B27" s="129"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Terminator - Level 7 done
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="162">
   <si>
     <t>Notes</t>
   </si>
@@ -615,6 +615,18 @@
   <si>
     <t>X = 399</t>
   </si>
+  <si>
+    <t>X = 150</t>
+  </si>
+  <si>
+    <t>X =1320</t>
+  </si>
+  <si>
+    <t>Black screen</t>
+  </si>
+  <si>
+    <t>End Level bonus</t>
+  </si>
 </sst>
 </file>
 
@@ -624,10 +636,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1358,14 +1377,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1373,7 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1381,75 +1400,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1459,10 +1478,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1483,69 +1502,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1558,111 +1580,111 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1970,10 +1992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O141"/>
+  <dimension ref="B1:O142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1987,19 +2009,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="110" t="s">
+      <c r="C1" s="115"/>
+      <c r="D1" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="111"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="117"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
-        <f>SUM(H1:H65523)</f>
+        <f>SUM(H1:H65524)</f>
         <v>225</v>
       </c>
       <c r="J1" s="71" t="s">
@@ -2074,10 +2096,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2114,7 +2136,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="119" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2134,7 +2156,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="114"/>
+      <c r="B9" s="120"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2144,7 +2166,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="114"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2155,7 +2177,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="114"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2166,7 +2188,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="114"/>
+      <c r="B12" s="120"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2177,7 +2199,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="114"/>
+      <c r="B13" s="120"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2188,7 +2210,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="114"/>
+      <c r="B14" s="120"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2199,7 +2221,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="114"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2210,7 +2232,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="114"/>
+      <c r="B16" s="120"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2253,7 +2275,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="113" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2288,7 +2310,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="116"/>
+      <c r="B20" s="114"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2321,7 +2343,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="116"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2354,7 +2376,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="116"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2387,7 +2409,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="116"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2420,7 +2442,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="116"/>
+      <c r="B24" s="114"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2456,7 +2478,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="116"/>
+      <c r="B25" s="114"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2489,7 +2511,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="116"/>
+      <c r="B26" s="114"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2522,7 +2544,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="116"/>
+      <c r="B27" s="114"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2555,7 +2577,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="116"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2588,7 +2610,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="116"/>
+      <c r="B29" s="114"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2614,7 +2636,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="111" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2649,7 +2671,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="118"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2678,7 +2700,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="118"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2707,7 +2729,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="118"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2737,7 +2759,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="118"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2757,7 +2779,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="118"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2777,7 +2799,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="118"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2800,7 +2822,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="118"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2823,7 +2845,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="118"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2891,7 +2913,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="113" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2911,7 +2933,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="116"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2928,7 +2950,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="116"/>
+      <c r="B45" s="114"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2945,7 +2967,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="116"/>
+      <c r="B46" s="114"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2963,7 +2985,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="116"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -2980,7 +3002,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="116"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -2997,7 +3019,7 @@
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:13" ht="15">
-      <c r="B49" s="116"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -3014,7 +3036,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:13" ht="15">
-      <c r="B50" s="116"/>
+      <c r="B50" s="114"/>
       <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
@@ -3031,7 +3053,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:13" ht="15">
-      <c r="B51" s="116"/>
+      <c r="B51" s="114"/>
       <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
@@ -3048,7 +3070,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:13" ht="15">
-      <c r="B52" s="116"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
@@ -3065,7 +3087,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:13" ht="15">
-      <c r="B53" s="116"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
@@ -3082,7 +3104,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:13" ht="15">
-      <c r="B54" s="116"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
@@ -3099,7 +3121,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:13" ht="15">
-      <c r="B55" s="116"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
@@ -3116,7 +3138,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:13" ht="15">
-      <c r="B56" s="116"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
@@ -3133,7 +3155,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:13" ht="15">
-      <c r="B57" s="116"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
@@ -3150,7 +3172,7 @@
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="2:13" ht="15">
-      <c r="B58" s="116"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
@@ -3170,7 +3192,7 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="15">
-      <c r="B59" s="116"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
@@ -3187,7 +3209,7 @@
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:13" ht="15">
-      <c r="B60" s="116"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
@@ -3204,7 +3226,7 @@
       <c r="G60" s="34"/>
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B61" s="116"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3243,7 +3265,7 @@
     </row>
     <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
     <row r="64" spans="2:13" ht="15">
-      <c r="B64" s="117" t="s">
+      <c r="B64" s="111" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3263,7 +3285,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="118"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3283,7 +3305,7 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="118"/>
+      <c r="B66" s="112"/>
       <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
@@ -3300,7 +3322,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="118"/>
+      <c r="B67" s="112"/>
       <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
@@ -3314,7 +3336,7 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="118"/>
+      <c r="B68" s="112"/>
       <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
@@ -3331,7 +3353,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="118"/>
+      <c r="B69" s="112"/>
       <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
@@ -3348,7 +3370,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="118"/>
+      <c r="B70" s="112"/>
       <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
@@ -3368,7 +3390,7 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="118"/>
+      <c r="B71" s="112"/>
       <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
@@ -3385,7 +3407,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="118"/>
+      <c r="B72" s="112"/>
       <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
@@ -3402,7 +3424,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="118"/>
+      <c r="B73" s="112"/>
       <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
@@ -3419,7 +3441,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="118"/>
+      <c r="B74" s="112"/>
       <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
@@ -3436,7 +3458,7 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="118"/>
+      <c r="B75" s="112"/>
       <c r="C75" s="105" t="s">
         <v>139</v>
       </c>
@@ -3453,7 +3475,7 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="118"/>
+      <c r="B76" s="112"/>
       <c r="C76" s="105" t="s">
         <v>140</v>
       </c>
@@ -3470,7 +3492,7 @@
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="118"/>
+      <c r="B77" s="112"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3481,7 +3503,7 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="118"/>
+      <c r="B78" s="112"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
@@ -3520,7 +3542,7 @@
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="81" spans="2:9" ht="15" customHeight="1">
-      <c r="B81" s="115" t="s">
+      <c r="B81" s="113" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3540,7 +3562,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B82" s="116"/>
+      <c r="B82" s="114"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
@@ -3557,7 +3579,7 @@
       <c r="G82" s="33"/>
     </row>
     <row r="83" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B83" s="116"/>
+      <c r="B83" s="114"/>
       <c r="C83" s="106" t="s">
         <v>141</v>
       </c>
@@ -3574,7 +3596,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:9" ht="15">
-      <c r="B84" s="116"/>
+      <c r="B84" s="114"/>
       <c r="C84" s="106" t="s">
         <v>142</v>
       </c>
@@ -3590,7 +3612,7 @@
       <c r="H84" s="41"/>
     </row>
     <row r="85" spans="2:9" ht="15">
-      <c r="B85" s="116"/>
+      <c r="B85" s="114"/>
       <c r="C85" s="106" t="s">
         <v>143</v>
       </c>
@@ -3607,7 +3629,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:9" ht="15" customHeight="1">
-      <c r="B86" s="116"/>
+      <c r="B86" s="114"/>
       <c r="C86" s="106" t="s">
         <v>144</v>
       </c>
@@ -3624,7 +3646,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="116"/>
+      <c r="B87" s="114"/>
       <c r="C87" s="106" t="s">
         <v>145</v>
       </c>
@@ -3683,7 +3705,7 @@
     </row>
     <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="91" spans="2:9" ht="15" customHeight="1">
-      <c r="B91" s="117" t="s">
+      <c r="B91" s="111" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="42" t="s">
@@ -3703,7 +3725,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B92" s="118"/>
+      <c r="B92" s="112"/>
       <c r="C92" s="27" t="s">
         <v>29</v>
       </c>
@@ -3720,7 +3742,7 @@
       <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B93" s="118"/>
+      <c r="B93" s="112"/>
       <c r="C93" s="106" t="s">
         <v>147</v>
       </c>
@@ -3737,7 +3759,7 @@
       <c r="G93" s="34"/>
     </row>
     <row r="94" spans="2:9" ht="15">
-      <c r="B94" s="118"/>
+      <c r="B94" s="112"/>
       <c r="C94" s="106" t="s">
         <v>148</v>
       </c>
@@ -3755,7 +3777,7 @@
       <c r="H94" s="41"/>
     </row>
     <row r="95" spans="2:9" ht="15">
-      <c r="B95" s="118"/>
+      <c r="B95" s="112"/>
       <c r="C95" s="106" t="s">
         <v>149</v>
       </c>
@@ -3809,7 +3831,7 @@
     </row>
     <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="115" t="s">
+      <c r="B99" s="113" t="s">
         <v>19</v>
       </c>
       <c r="C99" s="38" t="s">
@@ -3829,7 +3851,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="116"/>
+      <c r="B100" s="114"/>
       <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
@@ -3840,13 +3862,13 @@
         <v>31052</v>
       </c>
       <c r="F100" s="52">
-        <f t="shared" ref="F100:F118" si="8">IF(AND(D100&gt;0,E100&gt;0), E100-D100, 0)</f>
+        <f t="shared" ref="F100:F119" si="8">IF(AND(D100&gt;0,E100&gt;0), E100-D100, 0)</f>
         <v>3779</v>
       </c>
       <c r="G100" s="33"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="116"/>
+      <c r="B101" s="114"/>
       <c r="C101" s="108" t="s">
         <v>121</v>
       </c>
@@ -3863,7 +3885,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="116"/>
+      <c r="B102" s="114"/>
       <c r="C102" s="108" t="s">
         <v>150</v>
       </c>
@@ -3881,7 +3903,7 @@
       <c r="H102" s="41"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="116"/>
+      <c r="B103" s="114"/>
       <c r="C103" s="108" t="s">
         <v>151</v>
       </c>
@@ -3898,7 +3920,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="116"/>
+      <c r="B104" s="114"/>
       <c r="C104" s="109" t="s">
         <v>152</v>
       </c>
@@ -3915,7 +3937,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="116"/>
+      <c r="B105" s="114"/>
       <c r="C105" s="109" t="s">
         <v>121</v>
       </c>
@@ -3932,7 +3954,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="116"/>
+      <c r="B106" s="114"/>
       <c r="C106" s="109" t="s">
         <v>121</v>
       </c>
@@ -3949,7 +3971,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="116"/>
+      <c r="B107" s="114"/>
       <c r="C107" s="109" t="s">
         <v>121</v>
       </c>
@@ -3966,7 +3988,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="116"/>
+      <c r="B108" s="114"/>
       <c r="C108" s="109" t="s">
         <v>121</v>
       </c>
@@ -3983,7 +4005,7 @@
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="116"/>
+      <c r="B109" s="114"/>
       <c r="C109" s="109" t="s">
         <v>153</v>
       </c>
@@ -4000,8 +4022,8 @@
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="116"/>
-      <c r="C110" s="151" t="s">
+      <c r="B110" s="114"/>
+      <c r="C110" s="110" t="s">
         <v>154</v>
       </c>
       <c r="D110" s="30">
@@ -4017,8 +4039,8 @@
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="116"/>
-      <c r="C111" s="151" t="s">
+      <c r="B111" s="114"/>
+      <c r="C111" s="110" t="s">
         <v>155</v>
       </c>
       <c r="D111" s="30">
@@ -4034,8 +4056,8 @@
       <c r="G111" s="34"/>
     </row>
     <row r="112" spans="2:8" ht="15">
-      <c r="B112" s="116"/>
-      <c r="C112" s="151" t="s">
+      <c r="B112" s="114"/>
+      <c r="C112" s="110" t="s">
         <v>156</v>
       </c>
       <c r="D112" s="30">
@@ -4051,8 +4073,8 @@
       <c r="G112" s="34"/>
     </row>
     <row r="113" spans="2:8" ht="15">
-      <c r="B113" s="116"/>
-      <c r="C113" s="151" t="s">
+      <c r="B113" s="114"/>
+      <c r="C113" s="110" t="s">
         <v>121</v>
       </c>
       <c r="D113" s="30">
@@ -4068,8 +4090,8 @@
       <c r="G113" s="34"/>
     </row>
     <row r="114" spans="2:8" ht="15">
-      <c r="B114" s="116"/>
-      <c r="C114" s="151" t="s">
+      <c r="B114" s="114"/>
+      <c r="C114" s="110" t="s">
         <v>157</v>
       </c>
       <c r="D114" s="30">
@@ -4085,125 +4107,162 @@
       <c r="G114" s="34"/>
     </row>
     <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="116"/>
-      <c r="C115" s="151"/>
-      <c r="D115" s="30"/>
-      <c r="E115" s="30"/>
-      <c r="F115" s="52"/>
+      <c r="B115" s="114"/>
+      <c r="C115" s="152" t="s">
+        <v>158</v>
+      </c>
+      <c r="D115" s="30">
+        <v>30115</v>
+      </c>
+      <c r="E115" s="30">
+        <v>34189</v>
+      </c>
+      <c r="F115" s="52">
+        <f t="shared" si="8"/>
+        <v>4074</v>
+      </c>
       <c r="G115" s="34"/>
     </row>
     <row r="116" spans="2:8" ht="15">
-      <c r="B116" s="116"/>
-      <c r="C116" s="151"/>
-      <c r="D116" s="30"/>
-      <c r="E116" s="30"/>
-      <c r="F116" s="52"/>
+      <c r="B116" s="114"/>
+      <c r="C116" s="152" t="s">
+        <v>159</v>
+      </c>
+      <c r="D116" s="30">
+        <v>30530</v>
+      </c>
+      <c r="E116" s="30">
+        <v>34615</v>
+      </c>
+      <c r="F116" s="52">
+        <f t="shared" si="8"/>
+        <v>4085</v>
+      </c>
       <c r="G116" s="34"/>
     </row>
     <row r="117" spans="2:8" ht="15">
-      <c r="B117" s="116"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
+      <c r="B117" s="114"/>
+      <c r="C117" s="152" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117" s="30">
+        <v>31299</v>
+      </c>
+      <c r="E117" s="30">
+        <v>35555</v>
+      </c>
       <c r="F117" s="52">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4256</v>
       </c>
       <c r="G117" s="34"/>
     </row>
-    <row r="118" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B118" s="116"/>
-      <c r="C118" s="27" t="s">
+    <row r="118" spans="2:8" ht="15">
+      <c r="B118" s="114"/>
+      <c r="C118" s="152" t="s">
+        <v>161</v>
+      </c>
+      <c r="D118" s="30">
+        <v>31582</v>
+      </c>
+      <c r="E118" s="30">
+        <v>35843</v>
+      </c>
+      <c r="F118" s="52">
+        <f t="shared" si="8"/>
+        <v>4261</v>
+      </c>
+      <c r="G118" s="34"/>
+    </row>
+    <row r="119" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B119" s="114"/>
+      <c r="C119" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D118" s="28"/>
-      <c r="E118" s="28"/>
-      <c r="F118" s="54">
+      <c r="D119" s="28">
+        <v>32154</v>
+      </c>
+      <c r="E119" s="28">
+        <v>36262</v>
+      </c>
+      <c r="F119" s="54">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G118" s="33"/>
-    </row>
-    <row r="119" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B119" s="46">
+        <v>4108</v>
+      </c>
+      <c r="G119" s="33"/>
+    </row>
+    <row r="120" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B120" s="46">
         <v>7</v>
       </c>
-      <c r="C119" s="31" t="s">
+      <c r="C120" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D119" s="32">
-        <f>D118-D100</f>
-        <v>-27273</v>
-      </c>
-      <c r="E119" s="32">
-        <f>E118-E100</f>
-        <v>-31052</v>
-      </c>
-      <c r="F119" s="32">
-        <f>F118-F100</f>
-        <v>-3779</v>
-      </c>
-      <c r="G119" s="37"/>
-    </row>
-    <row r="120" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="121" spans="2:8" ht="15">
-      <c r="B121" s="117" t="s">
+      <c r="D120" s="32">
+        <f>D119-D100</f>
+        <v>4881</v>
+      </c>
+      <c r="E120" s="32">
+        <f>E119-E100</f>
+        <v>5210</v>
+      </c>
+      <c r="F120" s="32">
+        <f>F119-F100</f>
+        <v>329</v>
+      </c>
+      <c r="G120" s="37"/>
+    </row>
+    <row r="121" spans="2:8" ht="13.5" thickBot="1"/>
+    <row r="122" spans="2:8" ht="15">
+      <c r="B122" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="42" t="s">
+      <c r="C122" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D121" s="43" t="s">
+      <c r="D122" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E121" s="43" t="s">
+      <c r="E122" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F121" s="43" t="s">
+      <c r="F122" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G121" s="44" t="s">
+      <c r="G122" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B122" s="118"/>
-      <c r="C122" s="27" t="s">
+    <row r="123" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B123" s="112"/>
+      <c r="C123" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D122" s="28"/>
-      <c r="E122" s="28"/>
-      <c r="F122" s="52">
-        <f t="shared" ref="F122:F135" si="9">IF(AND(D122&gt;0,E122&gt;0), E122-D122, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G122" s="33"/>
-    </row>
-    <row r="123" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B123" s="118"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="30"/>
-      <c r="F123" s="53">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G123" s="34"/>
-    </row>
-    <row r="124" spans="2:8" ht="15">
-      <c r="B124" s="118"/>
+      <c r="D123" s="28">
+        <v>32154</v>
+      </c>
+      <c r="E123" s="28">
+        <v>36262</v>
+      </c>
+      <c r="F123" s="52">
+        <f t="shared" ref="F123:F136" si="9">IF(AND(D123&gt;0,E123&gt;0), E123-D123, 0)</f>
+        <v>4108</v>
+      </c>
+      <c r="G123" s="33"/>
+    </row>
+    <row r="124" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B124" s="112"/>
       <c r="C124" s="29"/>
       <c r="D124" s="30"/>
       <c r="E124" s="30"/>
-      <c r="F124" s="52">
+      <c r="F124" s="53">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G124" s="34"/>
-      <c r="H124" s="41"/>
     </row>
     <row r="125" spans="2:8" ht="15">
-      <c r="B125" s="118"/>
+      <c r="B125" s="112"/>
       <c r="C125" s="29"/>
       <c r="D125" s="30"/>
       <c r="E125" s="30"/>
@@ -4212,9 +4271,10 @@
         <v>0</v>
       </c>
       <c r="G125" s="34"/>
-    </row>
-    <row r="126" spans="2:8" ht="15" customHeight="1">
-      <c r="B126" s="118"/>
+      <c r="H125" s="41"/>
+    </row>
+    <row r="126" spans="2:8" ht="15">
+      <c r="B126" s="112"/>
       <c r="C126" s="29"/>
       <c r="D126" s="30"/>
       <c r="E126" s="30"/>
@@ -4224,8 +4284,8 @@
       </c>
       <c r="G126" s="34"/>
     </row>
-    <row r="127" spans="2:8" ht="15">
-      <c r="B127" s="118"/>
+    <row r="127" spans="2:8" ht="15" customHeight="1">
+      <c r="B127" s="112"/>
       <c r="C127" s="29"/>
       <c r="D127" s="30"/>
       <c r="E127" s="30"/>
@@ -4236,7 +4296,7 @@
       <c r="G127" s="34"/>
     </row>
     <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="118"/>
+      <c r="B128" s="112"/>
       <c r="C128" s="29"/>
       <c r="D128" s="30"/>
       <c r="E128" s="30"/>
@@ -4247,7 +4307,7 @@
       <c r="G128" s="34"/>
     </row>
     <row r="129" spans="2:8" ht="15">
-      <c r="B129" s="118"/>
+      <c r="B129" s="112"/>
       <c r="C129" s="29"/>
       <c r="D129" s="30"/>
       <c r="E129" s="30"/>
@@ -4258,7 +4318,7 @@
       <c r="G129" s="34"/>
     </row>
     <row r="130" spans="2:8" ht="15">
-      <c r="B130" s="118"/>
+      <c r="B130" s="112"/>
       <c r="C130" s="29"/>
       <c r="D130" s="30"/>
       <c r="E130" s="30"/>
@@ -4269,7 +4329,7 @@
       <c r="G130" s="34"/>
     </row>
     <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="118"/>
+      <c r="B131" s="112"/>
       <c r="C131" s="29"/>
       <c r="D131" s="30"/>
       <c r="E131" s="30"/>
@@ -4280,7 +4340,7 @@
       <c r="G131" s="34"/>
     </row>
     <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="118"/>
+      <c r="B132" s="112"/>
       <c r="C132" s="29"/>
       <c r="D132" s="30"/>
       <c r="E132" s="30"/>
@@ -4291,7 +4351,7 @@
       <c r="G132" s="34"/>
     </row>
     <row r="133" spans="2:8" ht="15">
-      <c r="B133" s="118"/>
+      <c r="B133" s="112"/>
       <c r="C133" s="29"/>
       <c r="D133" s="30"/>
       <c r="E133" s="30"/>
@@ -4302,7 +4362,7 @@
       <c r="G133" s="34"/>
     </row>
     <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="118"/>
+      <c r="B134" s="112"/>
       <c r="C134" s="29"/>
       <c r="D134" s="30"/>
       <c r="E134" s="30"/>
@@ -4312,57 +4372,68 @@
       </c>
       <c r="G134" s="34"/>
     </row>
-    <row r="135" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B135" s="118"/>
-      <c r="C135" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D135" s="28"/>
-      <c r="E135" s="28"/>
-      <c r="F135" s="54">
+    <row r="135" spans="2:8" ht="15">
+      <c r="B135" s="112"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="30"/>
+      <c r="E135" s="30"/>
+      <c r="F135" s="52">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G135" s="33"/>
-    </row>
-    <row r="136" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B136" s="45">
+      <c r="G135" s="34"/>
+    </row>
+    <row r="136" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B136" s="112"/>
+      <c r="C136" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G136" s="33"/>
+    </row>
+    <row r="137" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B137" s="45">
         <v>8</v>
       </c>
-      <c r="C136" s="31" t="s">
+      <c r="C137" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D136" s="32">
-        <f>D135-D122</f>
-        <v>0</v>
-      </c>
-      <c r="E136" s="32">
-        <f>E135-E122</f>
-        <v>0</v>
-      </c>
-      <c r="F136" s="32">
-        <f>F135-F122</f>
-        <v>0</v>
-      </c>
-      <c r="G136" s="36"/>
-    </row>
-    <row r="141" spans="2:8">
-      <c r="H141" s="41"/>
+      <c r="D137" s="32">
+        <f>D136-D123</f>
+        <v>-32154</v>
+      </c>
+      <c r="E137" s="32">
+        <f>E136-E123</f>
+        <v>-36262</v>
+      </c>
+      <c r="F137" s="32">
+        <f>F136-F123</f>
+        <v>-4108</v>
+      </c>
+      <c r="G137" s="36"/>
+    </row>
+    <row r="142" spans="2:8">
+      <c r="H142" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B121:B135"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B8:B16"/>
+    <mergeCell ref="B99:B119"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="B81:B87"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B122:B136"/>
     <mergeCell ref="B19:B29"/>
     <mergeCell ref="B43:B61"/>
     <mergeCell ref="B64:B78"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B99:B118"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B81:B87"/>
-    <mergeCell ref="B91:B95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4388,51 +4459,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="125"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="126"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="122"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="123"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4546,19 +4617,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="121"/>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="121"/>
-      <c r="H11" s="121"/>
-      <c r="I11" s="121"/>
-      <c r="J11" s="121"/>
-      <c r="K11" s="122"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="123"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4672,19 +4743,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="120" t="s">
+      <c r="A19" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="121"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="121"/>
-      <c r="K19" s="122"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="122"/>
+      <c r="I19" s="122"/>
+      <c r="J19" s="122"/>
+      <c r="K19" s="123"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4798,19 +4869,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="121"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="121"/>
-      <c r="K27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="123"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4924,19 +4995,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="121"/>
-      <c r="C35" s="121"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="121"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="121"/>
-      <c r="K35" s="122"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="122"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="122"/>
+      <c r="J35" s="122"/>
+      <c r="K35" s="123"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -5048,19 +5119,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="120" t="s">
+      <c r="A43" s="121" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="121"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
-      <c r="F43" s="121"/>
-      <c r="G43" s="121"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="121"/>
-      <c r="J43" s="121"/>
-      <c r="K43" s="122"/>
+      <c r="B43" s="122"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122"/>
+      <c r="G43" s="122"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="123"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -5174,19 +5245,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="120" t="s">
+      <c r="A51" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="121"/>
-      <c r="C51" s="121"/>
-      <c r="D51" s="121"/>
-      <c r="E51" s="121"/>
-      <c r="F51" s="121"/>
-      <c r="G51" s="121"/>
-      <c r="H51" s="121"/>
-      <c r="I51" s="121"/>
-      <c r="J51" s="121"/>
-      <c r="K51" s="122"/>
+      <c r="B51" s="122"/>
+      <c r="C51" s="122"/>
+      <c r="D51" s="122"/>
+      <c r="E51" s="122"/>
+      <c r="F51" s="122"/>
+      <c r="G51" s="122"/>
+      <c r="H51" s="122"/>
+      <c r="I51" s="122"/>
+      <c r="J51" s="122"/>
+      <c r="K51" s="123"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -5306,19 +5377,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="120" t="s">
+      <c r="A59" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="121"/>
-      <c r="C59" s="121"/>
-      <c r="D59" s="121"/>
-      <c r="E59" s="121"/>
-      <c r="F59" s="121"/>
-      <c r="G59" s="121"/>
-      <c r="H59" s="121"/>
-      <c r="I59" s="121"/>
-      <c r="J59" s="121"/>
-      <c r="K59" s="122"/>
+      <c r="B59" s="122"/>
+      <c r="C59" s="122"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="122"/>
+      <c r="F59" s="122"/>
+      <c r="G59" s="122"/>
+      <c r="H59" s="122"/>
+      <c r="I59" s="122"/>
+      <c r="J59" s="122"/>
+      <c r="K59" s="123"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -5428,19 +5499,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="120" t="s">
+      <c r="A67" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="121"/>
-      <c r="C67" s="121"/>
-      <c r="D67" s="121"/>
-      <c r="E67" s="121"/>
-      <c r="F67" s="121"/>
-      <c r="G67" s="121"/>
-      <c r="H67" s="121"/>
-      <c r="I67" s="121"/>
-      <c r="J67" s="121"/>
-      <c r="K67" s="122"/>
+      <c r="B67" s="122"/>
+      <c r="C67" s="122"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="122"/>
+      <c r="F67" s="122"/>
+      <c r="G67" s="122"/>
+      <c r="H67" s="122"/>
+      <c r="I67" s="122"/>
+      <c r="J67" s="122"/>
+      <c r="K67" s="123"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5548,19 +5619,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="120" t="s">
+      <c r="A75" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="121"/>
-      <c r="C75" s="121"/>
-      <c r="D75" s="121"/>
-      <c r="E75" s="121"/>
-      <c r="F75" s="121"/>
-      <c r="G75" s="121"/>
-      <c r="H75" s="121"/>
-      <c r="I75" s="121"/>
-      <c r="J75" s="121"/>
-      <c r="K75" s="122"/>
+      <c r="B75" s="122"/>
+      <c r="C75" s="122"/>
+      <c r="D75" s="122"/>
+      <c r="E75" s="122"/>
+      <c r="F75" s="122"/>
+      <c r="G75" s="122"/>
+      <c r="H75" s="122"/>
+      <c r="I75" s="122"/>
+      <c r="J75" s="122"/>
+      <c r="K75" s="123"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5676,19 +5747,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="120" t="s">
+      <c r="A83" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="121"/>
-      <c r="C83" s="121"/>
-      <c r="D83" s="121"/>
-      <c r="E83" s="121"/>
-      <c r="F83" s="121"/>
-      <c r="G83" s="121"/>
-      <c r="H83" s="121"/>
-      <c r="I83" s="121"/>
-      <c r="J83" s="121"/>
-      <c r="K83" s="122"/>
+      <c r="B83" s="122"/>
+      <c r="C83" s="122"/>
+      <c r="D83" s="122"/>
+      <c r="E83" s="122"/>
+      <c r="F83" s="122"/>
+      <c r="G83" s="122"/>
+      <c r="H83" s="122"/>
+      <c r="I83" s="122"/>
+      <c r="J83" s="122"/>
+      <c r="K83" s="123"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5800,19 +5871,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="120" t="s">
+      <c r="A91" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="121"/>
-      <c r="C91" s="121"/>
-      <c r="D91" s="121"/>
-      <c r="E91" s="121"/>
-      <c r="F91" s="121"/>
-      <c r="G91" s="121"/>
-      <c r="H91" s="121"/>
-      <c r="I91" s="121"/>
-      <c r="J91" s="121"/>
-      <c r="K91" s="122"/>
+      <c r="B91" s="122"/>
+      <c r="C91" s="122"/>
+      <c r="D91" s="122"/>
+      <c r="E91" s="122"/>
+      <c r="F91" s="122"/>
+      <c r="G91" s="122"/>
+      <c r="H91" s="122"/>
+      <c r="I91" s="122"/>
+      <c r="J91" s="122"/>
+      <c r="K91" s="123"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5926,19 +5997,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="120" t="s">
+      <c r="A99" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="121"/>
-      <c r="C99" s="121"/>
-      <c r="D99" s="121"/>
-      <c r="E99" s="121"/>
-      <c r="F99" s="121"/>
-      <c r="G99" s="121"/>
-      <c r="H99" s="121"/>
-      <c r="I99" s="121"/>
-      <c r="J99" s="121"/>
-      <c r="K99" s="122"/>
+      <c r="B99" s="122"/>
+      <c r="C99" s="122"/>
+      <c r="D99" s="122"/>
+      <c r="E99" s="122"/>
+      <c r="F99" s="122"/>
+      <c r="G99" s="122"/>
+      <c r="H99" s="122"/>
+      <c r="I99" s="122"/>
+      <c r="J99" s="122"/>
+      <c r="K99" s="123"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -6042,19 +6113,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="120" t="s">
+      <c r="A107" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="121"/>
-      <c r="C107" s="121"/>
-      <c r="D107" s="121"/>
-      <c r="E107" s="121"/>
-      <c r="F107" s="121"/>
-      <c r="G107" s="121"/>
-      <c r="H107" s="121"/>
-      <c r="I107" s="121"/>
-      <c r="J107" s="121"/>
-      <c r="K107" s="122"/>
+      <c r="B107" s="122"/>
+      <c r="C107" s="122"/>
+      <c r="D107" s="122"/>
+      <c r="E107" s="122"/>
+      <c r="F107" s="122"/>
+      <c r="G107" s="122"/>
+      <c r="H107" s="122"/>
+      <c r="I107" s="122"/>
+      <c r="J107" s="122"/>
+      <c r="K107" s="123"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -6159,24 +6230,24 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6391,7 +6462,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6418,10 +6489,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="128"/>
+      <c r="C1" s="129"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6432,7 +6503,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="130" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6446,7 +6517,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="130"/>
+      <c r="A4" s="131"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6458,7 +6529,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="130"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6467,7 +6538,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="130"/>
+      <c r="A6" s="131"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6479,7 +6550,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="130"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6491,7 +6562,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="130"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6500,7 +6571,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="131"/>
+      <c r="A9" s="132"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6515,7 +6586,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="130" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6529,7 +6600,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="130"/>
+      <c r="A12" s="131"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6541,7 +6612,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="130"/>
+      <c r="A13" s="131"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6550,7 +6621,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="130"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6562,7 +6633,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="130"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6574,7 +6645,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="130"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6583,7 +6654,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="131"/>
+      <c r="A17" s="132"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6598,7 +6669,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="130" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6607,7 +6678,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="130"/>
+      <c r="A20" s="131"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6617,14 +6688,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="130"/>
+      <c r="A21" s="131"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="130"/>
+      <c r="A22" s="131"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6634,7 +6705,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="130"/>
+      <c r="A23" s="131"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6644,14 +6715,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="130"/>
+      <c r="A24" s="131"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="131"/>
+      <c r="A25" s="132"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6664,7 +6735,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6695,17 +6766,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="149"/>
+      <c r="B2" s="140"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="150" t="s">
+      <c r="A3" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="149"/>
+      <c r="B3" s="140"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
@@ -6721,115 +6792,128 @@
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="137"/>
+      <c r="B7" s="151"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="138" t="s">
+      <c r="A9" s="148" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="139"/>
+      <c r="B9" s="149"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="140"/>
-      <c r="B10" s="141"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="136"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="132" t="s">
+      <c r="A11" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="133"/>
+      <c r="B11" s="138"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="133"/>
+      <c r="B12" s="138"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="138"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="132" t="s">
+      <c r="A14" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="133"/>
+      <c r="B14" s="138"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="132" t="s">
+      <c r="A15" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="133"/>
+      <c r="B15" s="138"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="133"/>
+      <c r="B16" s="138"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="134" t="s">
+      <c r="A17" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="135"/>
+      <c r="B17" s="134"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="136" t="s">
+      <c r="A19" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="137"/>
+      <c r="B19" s="151"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="138" t="s">
+      <c r="A21" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="139"/>
+      <c r="B21" s="149"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="140"/>
-      <c r="B22" s="141"/>
+      <c r="A22" s="135"/>
+      <c r="B22" s="136"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="132" t="s">
+      <c r="A23" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="138"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="132"/>
-      <c r="B24" s="133"/>
+      <c r="A24" s="137"/>
+      <c r="B24" s="138"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="133"/>
+      <c r="B25" s="138"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="132" t="s">
+      <c r="A26" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="133"/>
+      <c r="B26" s="138"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="134"/>
-      <c r="B27" s="135"/>
+      <c r="A27" s="133"/>
+      <c r="B27" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -6840,19 +6924,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - done!  Last 2 levels completed by Cardboard
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -95,12 +95,62 @@
         </r>
       </text>
     </comment>
+    <comment ref="C141" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anders:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+On the boxes
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C150" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anders:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Conveyor belt
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="184">
   <si>
     <t>Notes</t>
   </si>
@@ -627,6 +677,72 @@
   <si>
     <t>End Level bonus</t>
   </si>
+  <si>
+    <t>First Kyle-sprite seen</t>
+  </si>
+  <si>
+    <t>X = 941 going left</t>
+  </si>
+  <si>
+    <t>X = 988 going right</t>
+  </si>
+  <si>
+    <t>X = 925 going right</t>
+  </si>
+  <si>
+    <t>X = 2042</t>
+  </si>
+  <si>
+    <t>X = 1440 going right</t>
+  </si>
+  <si>
+    <t>X = 2248 going left</t>
+  </si>
+  <si>
+    <t>Press S at bonus</t>
+  </si>
+  <si>
+    <t>Level 9</t>
+  </si>
+  <si>
+    <t>X = 500 going left</t>
+  </si>
+  <si>
+    <t>X = 700 going right</t>
+  </si>
+  <si>
+    <t>Weap. Upgrade get</t>
+  </si>
+  <si>
+    <t>X = 2349 going left</t>
+  </si>
+  <si>
+    <t>X = 2502 going right</t>
+  </si>
+  <si>
+    <t>X = 3329 going right</t>
+  </si>
+  <si>
+    <t>X = 4306 going right</t>
+  </si>
+  <si>
+    <t>Level 10</t>
+  </si>
+  <si>
+    <t>X = 504 going right</t>
+  </si>
+  <si>
+    <t>X = 540 going right</t>
+  </si>
+  <si>
+    <t>X = 1194 going left</t>
+  </si>
+  <si>
+    <t>X = 1855 going right</t>
+  </si>
+  <si>
+    <t>X = 2387 going right</t>
+  </si>
 </sst>
 </file>
 
@@ -636,10 +752,31 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -925,6 +1062,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1377,14 +1527,14 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1392,7 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1400,75 +1550,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="10" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1478,10 +1628,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1502,75 +1652,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="14" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1580,9 +1742,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1592,108 +1751,108 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Färg1" xfId="2" builtinId="29"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Total" xfId="1" builtinId="25"/>
+    <cellStyle name="Summa" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1708,7 +1867,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1992,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O142"/>
+  <dimension ref="B1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2009,20 +2168,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="115"/>
-      <c r="D1" s="116" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="117"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="116"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
-        <f>SUM(H1:H65524)</f>
-        <v>225</v>
+        <f>SUM(H1:H65514)</f>
+        <v>106314</v>
       </c>
       <c r="J1" s="71" t="s">
         <v>51</v>
@@ -2044,19 +2203,19 @@
       <c r="H2" s="70"/>
       <c r="I2" s="74">
         <f>IF(I1&lt;3600,I1/60,QUOTIENT(I1, 3600))</f>
-        <v>3.75</v>
+        <v>29</v>
       </c>
       <c r="J2" s="71" t="str">
         <f>IF(I1&lt;3600,"Seconds","Minutes")</f>
-        <v>Seconds</v>
-      </c>
-      <c r="K2" s="74" t="str">
+        <v>Minutes</v>
+      </c>
+      <c r="K2" s="74">
         <f>IF(I1&lt;3600,"",(MOD(I1,3600)/60))</f>
-        <v/>
+        <v>31.9</v>
       </c>
       <c r="L2" s="71" t="str">
         <f>IF(I1&lt;3600, "", "Seconds")</f>
-        <v/>
+        <v>Seconds</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15">
@@ -2096,10 +2255,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="118" t="s">
+      <c r="D5" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="118"/>
+      <c r="E5" s="117"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2136,7 +2295,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="118" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2156,7 +2315,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2166,7 +2325,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="120"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2177,7 +2336,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="120"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2188,7 +2347,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="120"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2199,7 +2358,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="120"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2210,7 +2369,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="120"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2221,7 +2380,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="120"/>
+      <c r="B15" s="119"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2232,7 +2391,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="120"/>
+      <c r="B16" s="119"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2275,7 +2434,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="120" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2310,7 +2469,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="114"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2343,7 +2502,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="114"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2376,7 +2535,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="114"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2568,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="114"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2442,7 +2601,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="114"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2478,7 +2637,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="114"/>
+      <c r="B25" s="121"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2511,7 +2670,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="114"/>
+      <c r="B26" s="121"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2544,7 +2703,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="114"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2577,7 +2736,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="114"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2610,7 +2769,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="114"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2636,7 +2795,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="111" t="s">
+      <c r="B31" s="122" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2671,7 +2830,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="112"/>
+      <c r="B32" s="123"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2700,7 +2859,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="112"/>
+      <c r="B33" s="123"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2729,7 +2888,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="112"/>
+      <c r="B34" s="123"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2759,7 +2918,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="112"/>
+      <c r="B35" s="123"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2779,7 +2938,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="112"/>
+      <c r="B36" s="123"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2799,7 +2958,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="112"/>
+      <c r="B37" s="123"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2822,7 +2981,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="112"/>
+      <c r="B38" s="123"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -2845,7 +3004,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="112"/>
+      <c r="B39" s="123"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -2913,7 +3072,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="120" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2933,7 +3092,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="114"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -2950,7 +3109,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="114"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -2967,7 +3126,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="114"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -2985,7 +3144,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="114"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -3002,7 +3161,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="114"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -3019,7 +3178,7 @@
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:13" ht="15">
-      <c r="B49" s="114"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -3036,7 +3195,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:13" ht="15">
-      <c r="B50" s="114"/>
+      <c r="B50" s="121"/>
       <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
@@ -3053,7 +3212,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:13" ht="15">
-      <c r="B51" s="114"/>
+      <c r="B51" s="121"/>
       <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
@@ -3070,7 +3229,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:13" ht="15">
-      <c r="B52" s="114"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
@@ -3087,7 +3246,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:13" ht="15">
-      <c r="B53" s="114"/>
+      <c r="B53" s="121"/>
       <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
@@ -3104,7 +3263,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:13" ht="15">
-      <c r="B54" s="114"/>
+      <c r="B54" s="121"/>
       <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
@@ -3121,7 +3280,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:13" ht="15">
-      <c r="B55" s="114"/>
+      <c r="B55" s="121"/>
       <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
@@ -3138,7 +3297,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:13" ht="15">
-      <c r="B56" s="114"/>
+      <c r="B56" s="121"/>
       <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
@@ -3155,7 +3314,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:13" ht="15">
-      <c r="B57" s="114"/>
+      <c r="B57" s="121"/>
       <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
@@ -3172,7 +3331,7 @@
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="2:13" ht="15">
-      <c r="B58" s="114"/>
+      <c r="B58" s="121"/>
       <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
@@ -3192,7 +3351,7 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="15">
-      <c r="B59" s="114"/>
+      <c r="B59" s="121"/>
       <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
@@ -3209,7 +3368,7 @@
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:13" ht="15">
-      <c r="B60" s="114"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
@@ -3226,7 +3385,7 @@
       <c r="G60" s="34"/>
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B61" s="114"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3265,7 +3424,7 @@
     </row>
     <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
     <row r="64" spans="2:13" ht="15">
-      <c r="B64" s="111" t="s">
+      <c r="B64" s="122" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3285,7 +3444,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="112"/>
+      <c r="B65" s="123"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3305,7 +3464,7 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="112"/>
+      <c r="B66" s="123"/>
       <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
@@ -3322,7 +3481,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="112"/>
+      <c r="B67" s="123"/>
       <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
@@ -3336,7 +3495,7 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="112"/>
+      <c r="B68" s="123"/>
       <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
@@ -3353,7 +3512,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="112"/>
+      <c r="B69" s="123"/>
       <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
@@ -3370,7 +3529,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="112"/>
+      <c r="B70" s="123"/>
       <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
@@ -3390,7 +3549,7 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="112"/>
+      <c r="B71" s="123"/>
       <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
@@ -3407,7 +3566,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="112"/>
+      <c r="B72" s="123"/>
       <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
@@ -3424,7 +3583,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="112"/>
+      <c r="B73" s="123"/>
       <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
@@ -3441,7 +3600,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="112"/>
+      <c r="B74" s="123"/>
       <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
@@ -3458,7 +3617,7 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="112"/>
+      <c r="B75" s="123"/>
       <c r="C75" s="105" t="s">
         <v>139</v>
       </c>
@@ -3475,7 +3634,7 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="112"/>
+      <c r="B76" s="123"/>
       <c r="C76" s="105" t="s">
         <v>140</v>
       </c>
@@ -3492,7 +3651,7 @@
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="112"/>
+      <c r="B77" s="123"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3503,7 +3662,7 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="112"/>
+      <c r="B78" s="123"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
@@ -3542,7 +3701,7 @@
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="81" spans="2:9" ht="15" customHeight="1">
-      <c r="B81" s="113" t="s">
+      <c r="B81" s="120" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3562,7 +3721,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B82" s="114"/>
+      <c r="B82" s="121"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
@@ -3579,7 +3738,7 @@
       <c r="G82" s="33"/>
     </row>
     <row r="83" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B83" s="114"/>
+      <c r="B83" s="121"/>
       <c r="C83" s="106" t="s">
         <v>141</v>
       </c>
@@ -3596,7 +3755,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:9" ht="15">
-      <c r="B84" s="114"/>
+      <c r="B84" s="121"/>
       <c r="C84" s="106" t="s">
         <v>142</v>
       </c>
@@ -3612,7 +3771,7 @@
       <c r="H84" s="41"/>
     </row>
     <row r="85" spans="2:9" ht="15">
-      <c r="B85" s="114"/>
+      <c r="B85" s="121"/>
       <c r="C85" s="106" t="s">
         <v>143</v>
       </c>
@@ -3629,7 +3788,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:9" ht="15" customHeight="1">
-      <c r="B86" s="114"/>
+      <c r="B86" s="121"/>
       <c r="C86" s="106" t="s">
         <v>144</v>
       </c>
@@ -3646,7 +3805,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="114"/>
+      <c r="B87" s="121"/>
       <c r="C87" s="106" t="s">
         <v>145</v>
       </c>
@@ -3705,7 +3864,7 @@
     </row>
     <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="91" spans="2:9" ht="15" customHeight="1">
-      <c r="B91" s="111" t="s">
+      <c r="B91" s="122" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="42" t="s">
@@ -3725,7 +3884,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B92" s="112"/>
+      <c r="B92" s="123"/>
       <c r="C92" s="27" t="s">
         <v>29</v>
       </c>
@@ -3742,7 +3901,7 @@
       <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B93" s="112"/>
+      <c r="B93" s="123"/>
       <c r="C93" s="106" t="s">
         <v>147</v>
       </c>
@@ -3759,7 +3918,7 @@
       <c r="G93" s="34"/>
     </row>
     <row r="94" spans="2:9" ht="15">
-      <c r="B94" s="112"/>
+      <c r="B94" s="123"/>
       <c r="C94" s="106" t="s">
         <v>148</v>
       </c>
@@ -3777,7 +3936,7 @@
       <c r="H94" s="41"/>
     </row>
     <row r="95" spans="2:9" ht="15">
-      <c r="B95" s="112"/>
+      <c r="B95" s="123"/>
       <c r="C95" s="106" t="s">
         <v>149</v>
       </c>
@@ -3831,7 +3990,7 @@
     </row>
     <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="113" t="s">
+      <c r="B99" s="120" t="s">
         <v>19</v>
       </c>
       <c r="C99" s="38" t="s">
@@ -3851,7 +4010,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="114"/>
+      <c r="B100" s="121"/>
       <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
@@ -3868,7 +4027,7 @@
       <c r="G100" s="33"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="114"/>
+      <c r="B101" s="121"/>
       <c r="C101" s="108" t="s">
         <v>121</v>
       </c>
@@ -3885,7 +4044,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="114"/>
+      <c r="B102" s="121"/>
       <c r="C102" s="108" t="s">
         <v>150</v>
       </c>
@@ -3903,7 +4062,7 @@
       <c r="H102" s="41"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="114"/>
+      <c r="B103" s="121"/>
       <c r="C103" s="108" t="s">
         <v>151</v>
       </c>
@@ -3920,7 +4079,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="114"/>
+      <c r="B104" s="121"/>
       <c r="C104" s="109" t="s">
         <v>152</v>
       </c>
@@ -3937,7 +4096,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="114"/>
+      <c r="B105" s="121"/>
       <c r="C105" s="109" t="s">
         <v>121</v>
       </c>
@@ -3954,7 +4113,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="114"/>
+      <c r="B106" s="121"/>
       <c r="C106" s="109" t="s">
         <v>121</v>
       </c>
@@ -3971,7 +4130,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="114"/>
+      <c r="B107" s="121"/>
       <c r="C107" s="109" t="s">
         <v>121</v>
       </c>
@@ -3988,7 +4147,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="114"/>
+      <c r="B108" s="121"/>
       <c r="C108" s="109" t="s">
         <v>121</v>
       </c>
@@ -4005,7 +4164,7 @@
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="114"/>
+      <c r="B109" s="121"/>
       <c r="C109" s="109" t="s">
         <v>153</v>
       </c>
@@ -4022,7 +4181,7 @@
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="114"/>
+      <c r="B110" s="121"/>
       <c r="C110" s="110" t="s">
         <v>154</v>
       </c>
@@ -4039,7 +4198,7 @@
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="114"/>
+      <c r="B111" s="121"/>
       <c r="C111" s="110" t="s">
         <v>155</v>
       </c>
@@ -4056,7 +4215,7 @@
       <c r="G111" s="34"/>
     </row>
     <row r="112" spans="2:8" ht="15">
-      <c r="B112" s="114"/>
+      <c r="B112" s="121"/>
       <c r="C112" s="110" t="s">
         <v>156</v>
       </c>
@@ -4072,8 +4231,8 @@
       </c>
       <c r="G112" s="34"/>
     </row>
-    <row r="113" spans="2:8" ht="15">
-      <c r="B113" s="114"/>
+    <row r="113" spans="2:9" ht="15">
+      <c r="B113" s="121"/>
       <c r="C113" s="110" t="s">
         <v>121</v>
       </c>
@@ -4089,8 +4248,8 @@
       </c>
       <c r="G113" s="34"/>
     </row>
-    <row r="114" spans="2:8" ht="15">
-      <c r="B114" s="114"/>
+    <row r="114" spans="2:9" ht="15">
+      <c r="B114" s="121"/>
       <c r="C114" s="110" t="s">
         <v>157</v>
       </c>
@@ -4106,9 +4265,9 @@
       </c>
       <c r="G114" s="34"/>
     </row>
-    <row r="115" spans="2:8" ht="15">
-      <c r="B115" s="114"/>
-      <c r="C115" s="152" t="s">
+    <row r="115" spans="2:9" ht="15">
+      <c r="B115" s="121"/>
+      <c r="C115" s="111" t="s">
         <v>158</v>
       </c>
       <c r="D115" s="30">
@@ -4123,9 +4282,9 @@
       </c>
       <c r="G115" s="34"/>
     </row>
-    <row r="116" spans="2:8" ht="15">
-      <c r="B116" s="114"/>
-      <c r="C116" s="152" t="s">
+    <row r="116" spans="2:9" ht="15">
+      <c r="B116" s="121"/>
+      <c r="C116" s="111" t="s">
         <v>159</v>
       </c>
       <c r="D116" s="30">
@@ -4140,9 +4299,9 @@
       </c>
       <c r="G116" s="34"/>
     </row>
-    <row r="117" spans="2:8" ht="15">
-      <c r="B117" s="114"/>
-      <c r="C117" s="152" t="s">
+    <row r="117" spans="2:9" ht="15">
+      <c r="B117" s="121"/>
+      <c r="C117" s="111" t="s">
         <v>160</v>
       </c>
       <c r="D117" s="30">
@@ -4157,25 +4316,25 @@
       </c>
       <c r="G117" s="34"/>
     </row>
-    <row r="118" spans="2:8" ht="15">
-      <c r="B118" s="114"/>
-      <c r="C118" s="152" t="s">
+    <row r="118" spans="2:9" ht="15">
+      <c r="B118" s="121"/>
+      <c r="C118" s="111" t="s">
         <v>161</v>
       </c>
       <c r="D118" s="30">
-        <v>31582</v>
+        <v>31342</v>
       </c>
       <c r="E118" s="30">
         <v>35843</v>
       </c>
       <c r="F118" s="52">
         <f t="shared" si="8"/>
-        <v>4261</v>
+        <v>4501</v>
       </c>
       <c r="G118" s="34"/>
     </row>
-    <row r="119" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B119" s="114"/>
+    <row r="119" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B119" s="121"/>
       <c r="C119" s="27" t="s">
         <v>32</v>
       </c>
@@ -4191,7 +4350,7 @@
       </c>
       <c r="G119" s="33"/>
     </row>
-    <row r="120" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
+    <row r="120" spans="2:9" ht="17.25" thickTop="1" thickBot="1">
       <c r="B120" s="46">
         <v>7</v>
       </c>
@@ -4212,9 +4371,9 @@
       </c>
       <c r="G120" s="37"/>
     </row>
-    <row r="121" spans="2:8" ht="13.5" thickBot="1"/>
-    <row r="122" spans="2:8" ht="15">
-      <c r="B122" s="111" t="s">
+    <row r="121" spans="2:9" ht="13.5" thickBot="1"/>
+    <row r="122" spans="2:9" ht="15" customHeight="1">
+      <c r="B122" s="122" t="s">
         <v>20</v>
       </c>
       <c r="C122" s="42" t="s">
@@ -4233,8 +4392,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B123" s="112"/>
+    <row r="123" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B123" s="123"/>
       <c r="C123" s="27" t="s">
         <v>29</v>
       </c>
@@ -4245,183 +4404,554 @@
         <v>36262</v>
       </c>
       <c r="F123" s="52">
-        <f t="shared" ref="F123:F136" si="9">IF(AND(D123&gt;0,E123&gt;0), E123-D123, 0)</f>
+        <f t="shared" ref="F123:F132" si="9">IF(AND(D123&gt;0,E123&gt;0), E123-D123, 0)</f>
         <v>4108</v>
       </c>
       <c r="G123" s="33"/>
     </row>
-    <row r="124" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B124" s="112"/>
-      <c r="C124" s="29"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
+    <row r="124" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B124" s="123"/>
+      <c r="C124" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="D124" s="30">
+        <v>31840</v>
+      </c>
+      <c r="E124" s="30">
+        <v>36277</v>
+      </c>
       <c r="F124" s="53">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4437</v>
       </c>
       <c r="G124" s="34"/>
     </row>
-    <row r="125" spans="2:8" ht="15">
-      <c r="B125" s="112"/>
-      <c r="C125" s="29"/>
-      <c r="D125" s="30"/>
-      <c r="E125" s="30"/>
+    <row r="125" spans="2:9" ht="15">
+      <c r="B125" s="123"/>
+      <c r="C125" s="112" t="s">
+        <v>163</v>
+      </c>
+      <c r="D125" s="30">
+        <v>32244</v>
+      </c>
+      <c r="E125" s="30">
+        <v>36692</v>
+      </c>
       <c r="F125" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4448</v>
       </c>
       <c r="G125" s="34"/>
       <c r="H125" s="41"/>
     </row>
-    <row r="126" spans="2:8" ht="15">
-      <c r="B126" s="112"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="30"/>
+    <row r="126" spans="2:9" ht="15">
+      <c r="B126" s="123"/>
+      <c r="C126" s="112" t="s">
+        <v>164</v>
+      </c>
+      <c r="D126" s="30">
+        <v>32911</v>
+      </c>
+      <c r="E126" s="30">
+        <v>37424</v>
+      </c>
       <c r="F126" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4513</v>
       </c>
       <c r="G126" s="34"/>
     </row>
-    <row r="127" spans="2:8" ht="15" customHeight="1">
-      <c r="B127" s="112"/>
-      <c r="C127" s="29"/>
+    <row r="127" spans="2:9" ht="15" customHeight="1">
+      <c r="B127" s="123"/>
+      <c r="C127" s="112" t="s">
+        <v>165</v>
+      </c>
       <c r="D127" s="30"/>
-      <c r="E127" s="30"/>
+      <c r="E127" s="30">
+        <v>38564</v>
+      </c>
       <c r="F127" s="52">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G127" s="34"/>
     </row>
-    <row r="128" spans="2:8" ht="15">
-      <c r="B128" s="112"/>
-      <c r="C128" s="29"/>
-      <c r="D128" s="30"/>
-      <c r="E128" s="30"/>
+    <row r="128" spans="2:9" ht="15">
+      <c r="B128" s="123"/>
+      <c r="C128" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="D128" s="30">
+        <v>35005</v>
+      </c>
+      <c r="E128" s="30">
+        <v>39739</v>
+      </c>
       <c r="F128" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4734</v>
       </c>
       <c r="G128" s="34"/>
-    </row>
-    <row r="129" spans="2:8" ht="15">
-      <c r="B129" s="112"/>
-      <c r="C129" s="29"/>
-      <c r="D129" s="30"/>
-      <c r="E129" s="30"/>
+      <c r="H128">
+        <v>34862</v>
+      </c>
+      <c r="I128" s="41">
+        <f>D128-H128</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" ht="15">
+      <c r="B129" s="123"/>
+      <c r="C129" s="112" t="s">
+        <v>167</v>
+      </c>
+      <c r="D129" s="30">
+        <v>35588</v>
+      </c>
+      <c r="E129" s="30">
+        <v>40341</v>
+      </c>
       <c r="F129" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4753</v>
       </c>
       <c r="G129" s="34"/>
-    </row>
-    <row r="130" spans="2:8" ht="15">
-      <c r="B130" s="112"/>
-      <c r="C130" s="29"/>
-      <c r="D130" s="30"/>
-      <c r="E130" s="30"/>
+      <c r="H129">
+        <v>35445</v>
+      </c>
+      <c r="I129" s="41">
+        <f>D129-H129</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9" ht="15">
+      <c r="B130" s="123"/>
+      <c r="C130" s="112" t="s">
+        <v>168</v>
+      </c>
+      <c r="D130" s="30">
+        <v>35922</v>
+      </c>
+      <c r="E130" s="30">
+        <v>40945</v>
+      </c>
       <c r="F130" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5023</v>
       </c>
       <c r="G130" s="34"/>
-    </row>
-    <row r="131" spans="2:8" ht="15">
-      <c r="B131" s="112"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="30"/>
-      <c r="E131" s="30"/>
+      <c r="H130">
+        <v>35782</v>
+      </c>
+      <c r="I130" s="41">
+        <f>D130-H130</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" ht="15">
+      <c r="B131" s="123"/>
+      <c r="C131" s="112" t="s">
+        <v>169</v>
+      </c>
+      <c r="D131" s="30">
+        <v>37112</v>
+      </c>
+      <c r="E131" s="30">
+        <v>42279</v>
+      </c>
       <c r="F131" s="52">
         <f t="shared" si="9"/>
+        <v>5167</v>
+      </c>
+      <c r="G131" s="34"/>
+    </row>
+    <row r="132" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B132" s="123"/>
+      <c r="C132" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132" s="28">
+        <v>37112</v>
+      </c>
+      <c r="E132" s="28">
+        <v>42279</v>
+      </c>
+      <c r="F132" s="54">
+        <f t="shared" si="9"/>
+        <v>5167</v>
+      </c>
+      <c r="G132" s="33"/>
+    </row>
+    <row r="133" spans="2:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B133" s="45">
+        <v>8</v>
+      </c>
+      <c r="C133" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="32">
+        <f>D132-D123</f>
+        <v>4958</v>
+      </c>
+      <c r="E133" s="32">
+        <f>E132-E123</f>
+        <v>6017</v>
+      </c>
+      <c r="F133" s="32">
+        <f>F132-F123</f>
+        <v>1059</v>
+      </c>
+      <c r="G133" s="36"/>
+    </row>
+    <row r="134" spans="2:9" ht="13.5" thickBot="1"/>
+    <row r="135" spans="2:9" ht="15" customHeight="1">
+      <c r="B135" s="122" t="s">
+        <v>170</v>
+      </c>
+      <c r="C135" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D135" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E135" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G135" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B136" s="123"/>
+      <c r="C136" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D136" s="28">
+        <v>37562</v>
+      </c>
+      <c r="E136" s="28">
+        <v>42696</v>
+      </c>
+      <c r="F136" s="52">
+        <f t="shared" ref="F136:F143" si="10">IF(AND(D136&gt;0,E136&gt;0), E136-D136, 0)</f>
+        <v>5134</v>
+      </c>
+      <c r="G136" s="33"/>
+    </row>
+    <row r="137" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B137" s="123"/>
+      <c r="C137" s="113" t="s">
+        <v>171</v>
+      </c>
+      <c r="D137" s="30">
+        <v>38103</v>
+      </c>
+      <c r="E137" s="30">
+        <v>43270</v>
+      </c>
+      <c r="F137" s="53">
+        <f t="shared" si="10"/>
+        <v>5167</v>
+      </c>
+      <c r="G137" s="34"/>
+    </row>
+    <row r="138" spans="2:9" ht="15">
+      <c r="B138" s="123"/>
+      <c r="C138" s="113" t="s">
+        <v>172</v>
+      </c>
+      <c r="D138" s="30">
+        <v>38637</v>
+      </c>
+      <c r="E138" s="30">
+        <v>43858</v>
+      </c>
+      <c r="F138" s="52">
+        <f t="shared" si="10"/>
+        <v>5221</v>
+      </c>
+      <c r="G138" s="34"/>
+      <c r="H138" s="41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" ht="15">
+      <c r="B139" s="123"/>
+      <c r="C139" s="113" t="s">
+        <v>174</v>
+      </c>
+      <c r="D139" s="30"/>
+      <c r="E139" s="30">
+        <v>44803</v>
+      </c>
+      <c r="F139" s="52">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G131" s="34"/>
-    </row>
-    <row r="132" spans="2:8" ht="15">
-      <c r="B132" s="112"/>
-      <c r="C132" s="29"/>
-      <c r="D132" s="30"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G132" s="34"/>
-    </row>
-    <row r="133" spans="2:8" ht="15">
-      <c r="B133" s="112"/>
-      <c r="C133" s="29"/>
-      <c r="D133" s="30"/>
-      <c r="E133" s="30"/>
-      <c r="F133" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G133" s="34"/>
-    </row>
-    <row r="134" spans="2:8" ht="15">
-      <c r="B134" s="112"/>
-      <c r="C134" s="29"/>
-      <c r="D134" s="30"/>
-      <c r="E134" s="30"/>
-      <c r="F134" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G134" s="34"/>
-    </row>
-    <row r="135" spans="2:8" ht="15">
-      <c r="B135" s="112"/>
-      <c r="C135" s="29"/>
-      <c r="D135" s="30"/>
-      <c r="E135" s="30"/>
-      <c r="F135" s="52">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G135" s="34"/>
-    </row>
-    <row r="136" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B136" s="112"/>
-      <c r="C136" s="27" t="s">
+      <c r="G139" s="34"/>
+    </row>
+    <row r="140" spans="2:9" ht="15">
+      <c r="B140" s="123"/>
+      <c r="C140" s="113" t="s">
+        <v>175</v>
+      </c>
+      <c r="D140" s="30">
+        <v>39967</v>
+      </c>
+      <c r="E140" s="30">
+        <v>45440</v>
+      </c>
+      <c r="F140" s="52">
+        <f t="shared" si="10"/>
+        <v>5473</v>
+      </c>
+      <c r="G140" s="34"/>
+    </row>
+    <row r="141" spans="2:9" ht="15">
+      <c r="B141" s="123"/>
+      <c r="C141" s="113" t="s">
+        <v>176</v>
+      </c>
+      <c r="D141" s="30">
+        <v>40700</v>
+      </c>
+      <c r="E141" s="30">
+        <v>46265</v>
+      </c>
+      <c r="F141" s="52">
+        <f t="shared" si="10"/>
+        <v>5565</v>
+      </c>
+      <c r="G141" s="34"/>
+    </row>
+    <row r="142" spans="2:9" ht="15">
+      <c r="B142" s="123"/>
+      <c r="C142" s="113" t="s">
+        <v>177</v>
+      </c>
+      <c r="D142" s="30">
+        <v>41201</v>
+      </c>
+      <c r="E142" s="30">
+        <v>46825</v>
+      </c>
+      <c r="F142" s="52">
+        <f t="shared" si="10"/>
+        <v>5624</v>
+      </c>
+      <c r="G142" s="34"/>
+    </row>
+    <row r="143" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B143" s="101"/>
+      <c r="C143" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D136" s="28"/>
-      <c r="E136" s="28"/>
-      <c r="F136" s="54">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G136" s="33"/>
-    </row>
-    <row r="137" spans="2:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="B137" s="45">
-        <v>8</v>
-      </c>
-      <c r="C137" s="31" t="s">
+      <c r="D143" s="28">
+        <v>42297</v>
+      </c>
+      <c r="E143" s="28">
+        <v>48178</v>
+      </c>
+      <c r="F143" s="54">
+        <f t="shared" si="10"/>
+        <v>5881</v>
+      </c>
+      <c r="G143" s="33"/>
+    </row>
+    <row r="144" spans="2:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B144" s="45">
+        <v>9</v>
+      </c>
+      <c r="C144" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D137" s="32">
-        <f>D136-D123</f>
-        <v>-32154</v>
-      </c>
-      <c r="E137" s="32">
-        <f>E136-E123</f>
-        <v>-36262</v>
-      </c>
-      <c r="F137" s="32">
-        <f>F136-F123</f>
-        <v>-4108</v>
-      </c>
-      <c r="G137" s="36"/>
-    </row>
-    <row r="142" spans="2:8">
-      <c r="H142" s="41"/>
+      <c r="D144" s="32">
+        <f>D143-D136</f>
+        <v>4735</v>
+      </c>
+      <c r="E144" s="32">
+        <f>E143-E136</f>
+        <v>5482</v>
+      </c>
+      <c r="F144" s="32">
+        <f>F143-F136</f>
+        <v>747</v>
+      </c>
+      <c r="G144" s="36"/>
+    </row>
+    <row r="145" spans="2:7" ht="13.5" thickBot="1"/>
+    <row r="146" spans="2:7" ht="15" customHeight="1">
+      <c r="B146" s="120" t="s">
+        <v>178</v>
+      </c>
+      <c r="C146" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D146" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E146" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F146" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G146" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B147" s="121"/>
+      <c r="C147" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D147" s="28">
+        <v>42715</v>
+      </c>
+      <c r="E147" s="28">
+        <v>48596</v>
+      </c>
+      <c r="F147" s="52">
+        <f t="shared" ref="F147:F153" si="11">IF(AND(D147&gt;0,E147&gt;0), E147-D147, 0)</f>
+        <v>5881</v>
+      </c>
+      <c r="G147" s="33"/>
+    </row>
+    <row r="148" spans="2:7" ht="15.75" thickTop="1">
+      <c r="B148" s="121"/>
+      <c r="C148" s="155" t="s">
+        <v>180</v>
+      </c>
+      <c r="D148" s="30">
+        <v>43163</v>
+      </c>
+      <c r="E148" s="30">
+        <v>49128</v>
+      </c>
+      <c r="F148" s="53">
+        <f t="shared" si="11"/>
+        <v>5965</v>
+      </c>
+      <c r="G148" s="34"/>
+    </row>
+    <row r="149" spans="2:7" ht="15">
+      <c r="B149" s="121"/>
+      <c r="C149" s="155" t="s">
+        <v>181</v>
+      </c>
+      <c r="D149" s="30">
+        <v>43666</v>
+      </c>
+      <c r="E149" s="30">
+        <v>49728</v>
+      </c>
+      <c r="F149" s="52">
+        <f t="shared" si="11"/>
+        <v>6062</v>
+      </c>
+      <c r="G149" s="34"/>
+    </row>
+    <row r="150" spans="2:7" ht="15">
+      <c r="B150" s="121"/>
+      <c r="C150" s="155" t="s">
+        <v>179</v>
+      </c>
+      <c r="D150" s="30">
+        <v>44266</v>
+      </c>
+      <c r="E150" s="30">
+        <v>50464</v>
+      </c>
+      <c r="F150" s="52">
+        <f t="shared" si="11"/>
+        <v>6198</v>
+      </c>
+      <c r="G150" s="34"/>
+    </row>
+    <row r="151" spans="2:7" ht="15">
+      <c r="B151" s="121"/>
+      <c r="C151" s="155" t="s">
+        <v>182</v>
+      </c>
+      <c r="D151" s="30">
+        <v>45549</v>
+      </c>
+      <c r="E151" s="30">
+        <v>51768</v>
+      </c>
+      <c r="F151" s="52">
+        <f t="shared" si="11"/>
+        <v>6219</v>
+      </c>
+      <c r="G151" s="34"/>
+    </row>
+    <row r="152" spans="2:7" ht="15">
+      <c r="B152" s="121"/>
+      <c r="C152" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D152" s="30">
+        <v>46519</v>
+      </c>
+      <c r="E152" s="30">
+        <v>52929</v>
+      </c>
+      <c r="F152" s="52">
+        <f t="shared" si="11"/>
+        <v>6410</v>
+      </c>
+      <c r="G152" s="34"/>
+    </row>
+    <row r="153" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B153" s="121"/>
+      <c r="C153" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D153" s="28">
+        <v>48431</v>
+      </c>
+      <c r="E153" s="28">
+        <v>54956</v>
+      </c>
+      <c r="F153" s="54">
+        <f t="shared" si="11"/>
+        <v>6525</v>
+      </c>
+      <c r="G153" s="33"/>
+    </row>
+    <row r="154" spans="2:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="B154" s="46">
+        <v>10</v>
+      </c>
+      <c r="C154" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D154" s="32">
+        <f>D153-D147</f>
+        <v>5716</v>
+      </c>
+      <c r="E154" s="32">
+        <f>E153-E147</f>
+        <v>6360</v>
+      </c>
+      <c r="F154" s="32">
+        <f>F153-F147</f>
+        <v>644</v>
+      </c>
+      <c r="G154" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="B122:B132"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B43:B61"/>
+    <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B135:B142"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B8:B16"/>
@@ -4429,11 +4959,6 @@
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="B81:B87"/>
     <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B122:B136"/>
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B43:B61"/>
-    <mergeCell ref="B64:B78"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4459,51 +4984,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="126"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="129"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="123"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="126"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -4617,19 +5142,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
-      <c r="J11" s="122"/>
-      <c r="K11" s="123"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="126"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -4743,19 +5268,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
-      <c r="G19" s="122"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122"/>
-      <c r="K19" s="123"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="126"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -4869,19 +5394,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="122"/>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
-      <c r="K27" s="123"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="125"/>
+      <c r="G27" s="125"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="126"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -4995,19 +5520,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="121" t="s">
+      <c r="A35" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="122"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="122"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="123"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="126"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -5119,19 +5644,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="121" t="s">
+      <c r="A43" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="122"/>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="122"/>
-      <c r="H43" s="122"/>
-      <c r="I43" s="122"/>
-      <c r="J43" s="122"/>
-      <c r="K43" s="123"/>
+      <c r="B43" s="125"/>
+      <c r="C43" s="125"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="125"/>
+      <c r="F43" s="125"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="125"/>
+      <c r="I43" s="125"/>
+      <c r="J43" s="125"/>
+      <c r="K43" s="126"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -5245,19 +5770,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="121" t="s">
+      <c r="A51" s="124" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="122"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
-      <c r="G51" s="122"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="122"/>
-      <c r="J51" s="122"/>
-      <c r="K51" s="123"/>
+      <c r="B51" s="125"/>
+      <c r="C51" s="125"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="125"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="125"/>
+      <c r="K51" s="126"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -5377,19 +5902,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="121" t="s">
+      <c r="A59" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="122"/>
-      <c r="C59" s="122"/>
-      <c r="D59" s="122"/>
-      <c r="E59" s="122"/>
-      <c r="F59" s="122"/>
-      <c r="G59" s="122"/>
-      <c r="H59" s="122"/>
-      <c r="I59" s="122"/>
-      <c r="J59" s="122"/>
-      <c r="K59" s="123"/>
+      <c r="B59" s="125"/>
+      <c r="C59" s="125"/>
+      <c r="D59" s="125"/>
+      <c r="E59" s="125"/>
+      <c r="F59" s="125"/>
+      <c r="G59" s="125"/>
+      <c r="H59" s="125"/>
+      <c r="I59" s="125"/>
+      <c r="J59" s="125"/>
+      <c r="K59" s="126"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -5499,19 +6024,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="121" t="s">
+      <c r="A67" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="122"/>
-      <c r="C67" s="122"/>
-      <c r="D67" s="122"/>
-      <c r="E67" s="122"/>
-      <c r="F67" s="122"/>
-      <c r="G67" s="122"/>
-      <c r="H67" s="122"/>
-      <c r="I67" s="122"/>
-      <c r="J67" s="122"/>
-      <c r="K67" s="123"/>
+      <c r="B67" s="125"/>
+      <c r="C67" s="125"/>
+      <c r="D67" s="125"/>
+      <c r="E67" s="125"/>
+      <c r="F67" s="125"/>
+      <c r="G67" s="125"/>
+      <c r="H67" s="125"/>
+      <c r="I67" s="125"/>
+      <c r="J67" s="125"/>
+      <c r="K67" s="126"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -5619,19 +6144,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="121" t="s">
+      <c r="A75" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="122"/>
-      <c r="C75" s="122"/>
-      <c r="D75" s="122"/>
-      <c r="E75" s="122"/>
-      <c r="F75" s="122"/>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122"/>
-      <c r="I75" s="122"/>
-      <c r="J75" s="122"/>
-      <c r="K75" s="123"/>
+      <c r="B75" s="125"/>
+      <c r="C75" s="125"/>
+      <c r="D75" s="125"/>
+      <c r="E75" s="125"/>
+      <c r="F75" s="125"/>
+      <c r="G75" s="125"/>
+      <c r="H75" s="125"/>
+      <c r="I75" s="125"/>
+      <c r="J75" s="125"/>
+      <c r="K75" s="126"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -5747,19 +6272,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="121" t="s">
+      <c r="A83" s="124" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="122"/>
-      <c r="C83" s="122"/>
-      <c r="D83" s="122"/>
-      <c r="E83" s="122"/>
-      <c r="F83" s="122"/>
-      <c r="G83" s="122"/>
-      <c r="H83" s="122"/>
-      <c r="I83" s="122"/>
-      <c r="J83" s="122"/>
-      <c r="K83" s="123"/>
+      <c r="B83" s="125"/>
+      <c r="C83" s="125"/>
+      <c r="D83" s="125"/>
+      <c r="E83" s="125"/>
+      <c r="F83" s="125"/>
+      <c r="G83" s="125"/>
+      <c r="H83" s="125"/>
+      <c r="I83" s="125"/>
+      <c r="J83" s="125"/>
+      <c r="K83" s="126"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -5871,19 +6396,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="121" t="s">
+      <c r="A91" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="122"/>
-      <c r="C91" s="122"/>
-      <c r="D91" s="122"/>
-      <c r="E91" s="122"/>
-      <c r="F91" s="122"/>
-      <c r="G91" s="122"/>
-      <c r="H91" s="122"/>
-      <c r="I91" s="122"/>
-      <c r="J91" s="122"/>
-      <c r="K91" s="123"/>
+      <c r="B91" s="125"/>
+      <c r="C91" s="125"/>
+      <c r="D91" s="125"/>
+      <c r="E91" s="125"/>
+      <c r="F91" s="125"/>
+      <c r="G91" s="125"/>
+      <c r="H91" s="125"/>
+      <c r="I91" s="125"/>
+      <c r="J91" s="125"/>
+      <c r="K91" s="126"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -5997,19 +6522,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="121" t="s">
+      <c r="A99" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="122"/>
-      <c r="C99" s="122"/>
-      <c r="D99" s="122"/>
-      <c r="E99" s="122"/>
-      <c r="F99" s="122"/>
-      <c r="G99" s="122"/>
-      <c r="H99" s="122"/>
-      <c r="I99" s="122"/>
-      <c r="J99" s="122"/>
-      <c r="K99" s="123"/>
+      <c r="B99" s="125"/>
+      <c r="C99" s="125"/>
+      <c r="D99" s="125"/>
+      <c r="E99" s="125"/>
+      <c r="F99" s="125"/>
+      <c r="G99" s="125"/>
+      <c r="H99" s="125"/>
+      <c r="I99" s="125"/>
+      <c r="J99" s="125"/>
+      <c r="K99" s="126"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -6113,19 +6638,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="121" t="s">
+      <c r="A107" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="122"/>
-      <c r="C107" s="122"/>
-      <c r="D107" s="122"/>
-      <c r="E107" s="122"/>
-      <c r="F107" s="122"/>
-      <c r="G107" s="122"/>
-      <c r="H107" s="122"/>
-      <c r="I107" s="122"/>
-      <c r="J107" s="122"/>
-      <c r="K107" s="123"/>
+      <c r="B107" s="125"/>
+      <c r="C107" s="125"/>
+      <c r="D107" s="125"/>
+      <c r="E107" s="125"/>
+      <c r="F107" s="125"/>
+      <c r="G107" s="125"/>
+      <c r="H107" s="125"/>
+      <c r="I107" s="125"/>
+      <c r="J107" s="125"/>
+      <c r="K107" s="126"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -6230,24 +6755,24 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6462,7 +6987,7 @@
       <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6489,10 +7014,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="128" t="s">
+      <c r="B1" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="129"/>
+      <c r="C1" s="132"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -6503,7 +7028,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="133" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -6517,7 +7042,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="131"/>
+      <c r="A4" s="134"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -6529,7 +7054,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="131"/>
+      <c r="A5" s="134"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -6538,7 +7063,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="131"/>
+      <c r="A6" s="134"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -6550,7 +7075,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="131"/>
+      <c r="A7" s="134"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -6562,7 +7087,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="131"/>
+      <c r="A8" s="134"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -6571,7 +7096,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="132"/>
+      <c r="A9" s="135"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -6586,7 +7111,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="130" t="s">
+      <c r="A11" s="133" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -6600,7 +7125,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="131"/>
+      <c r="A12" s="134"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -6612,7 +7137,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="131"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -6621,7 +7146,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="131"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -6633,7 +7158,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="131"/>
+      <c r="A15" s="134"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -6645,7 +7170,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="131"/>
+      <c r="A16" s="134"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -6654,7 +7179,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="132"/>
+      <c r="A17" s="135"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -6669,7 +7194,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="130" t="s">
+      <c r="A19" s="133" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -6678,7 +7203,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="131"/>
+      <c r="A20" s="134"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -6688,14 +7213,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="131"/>
+      <c r="A21" s="134"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="131"/>
+      <c r="A22" s="134"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -6705,7 +7230,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="131"/>
+      <c r="A23" s="134"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -6715,14 +7240,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="131"/>
+      <c r="A24" s="134"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="132"/>
+      <c r="A25" s="135"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -6735,7 +7260,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -6757,163 +7282,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="146" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="143"/>
+      <c r="B1" s="147"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="152" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="140"/>
+      <c r="B2" s="153"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="140"/>
+      <c r="B3" s="153"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="146"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="150"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="145"/>
+      <c r="B5" s="149"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="150" t="s">
+      <c r="A7" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="151"/>
+      <c r="B7" s="141"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="148" t="s">
+      <c r="A9" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="149"/>
+      <c r="B9" s="143"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="135"/>
-      <c r="B10" s="136"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="145"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="138"/>
+      <c r="B11" s="137"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="138"/>
+      <c r="B12" s="137"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="138"/>
+      <c r="B13" s="137"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="138"/>
+      <c r="B14" s="137"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="137" t="s">
+      <c r="A15" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="138"/>
+      <c r="B15" s="137"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="137" t="s">
+      <c r="A16" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="138"/>
+      <c r="B16" s="137"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="133" t="s">
+      <c r="A17" s="138" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="134"/>
+      <c r="B17" s="139"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="151"/>
+      <c r="B19" s="141"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="148" t="s">
+      <c r="A21" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="149"/>
+      <c r="B21" s="143"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="135"/>
-      <c r="B22" s="136"/>
+      <c r="A22" s="144"/>
+      <c r="B22" s="145"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="137" t="s">
+      <c r="A23" s="136" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="138"/>
+      <c r="B23" s="137"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="137"/>
-      <c r="B24" s="138"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="137"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="137" t="s">
+      <c r="A25" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="138"/>
+      <c r="B25" s="137"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="137" t="s">
+      <c r="A26" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="138"/>
+      <c r="B26" s="137"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="133"/>
-      <c r="B27" s="134"/>
+      <c r="A27" s="138"/>
+      <c r="B27" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -6924,6 +7436,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - improved final boss by cardboard
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1751,6 +1751,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1763,18 +1778,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1807,46 +1810,43 @@
     <xf numFmtId="0" fontId="42" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Färg1" xfId="2" builtinId="29"/>
@@ -2168,16 +2168,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="115" t="s">
+      <c r="C1" s="119"/>
+      <c r="D1" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="116"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
         <f>SUM(H1:H65514)</f>
@@ -2255,10 +2255,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="117"/>
+      <c r="E5" s="122"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2295,7 +2295,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="123" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2315,7 +2315,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="119"/>
+      <c r="B9" s="124"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="119"/>
+      <c r="B10" s="124"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2336,7 +2336,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="119"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2347,7 +2347,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="119"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2358,7 +2358,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="119"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2369,7 +2369,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="119"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2380,7 +2380,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="119"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2391,7 +2391,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="119"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2434,7 +2434,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="115" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="121"/>
+      <c r="B20" s="116"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2502,7 +2502,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="121"/>
+      <c r="B21" s="116"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="121"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2568,7 +2568,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="121"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2601,7 +2601,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="121"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2637,7 +2637,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="121"/>
+      <c r="B25" s="116"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2670,7 +2670,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="121"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2703,7 +2703,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="121"/>
+      <c r="B27" s="116"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2736,7 +2736,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="121"/>
+      <c r="B28" s="116"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="121"/>
+      <c r="B29" s="116"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="122" t="s">
+      <c r="B31" s="117" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="123"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="123"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2888,7 +2888,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="123"/>
+      <c r="B34" s="118"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2918,7 +2918,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="123"/>
+      <c r="B35" s="118"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2938,7 +2938,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="123"/>
+      <c r="B36" s="118"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="123"/>
+      <c r="B37" s="118"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2981,7 +2981,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="123"/>
+      <c r="B38" s="118"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="123"/>
+      <c r="B39" s="118"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="120" t="s">
+      <c r="B43" s="115" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -3092,7 +3092,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="121"/>
+      <c r="B44" s="116"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -3109,7 +3109,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="121"/>
+      <c r="B45" s="116"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="121"/>
+      <c r="B46" s="116"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="121"/>
+      <c r="B47" s="116"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -3161,7 +3161,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="121"/>
+      <c r="B48" s="116"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:13" ht="15">
-      <c r="B49" s="121"/>
+      <c r="B49" s="116"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:13" ht="15">
-      <c r="B50" s="121"/>
+      <c r="B50" s="116"/>
       <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:13" ht="15">
-      <c r="B51" s="121"/>
+      <c r="B51" s="116"/>
       <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
@@ -3229,7 +3229,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:13" ht="15">
-      <c r="B52" s="121"/>
+      <c r="B52" s="116"/>
       <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
@@ -3246,7 +3246,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:13" ht="15">
-      <c r="B53" s="121"/>
+      <c r="B53" s="116"/>
       <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:13" ht="15">
-      <c r="B54" s="121"/>
+      <c r="B54" s="116"/>
       <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
@@ -3280,7 +3280,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:13" ht="15">
-      <c r="B55" s="121"/>
+      <c r="B55" s="116"/>
       <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:13" ht="15">
-      <c r="B56" s="121"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:13" ht="15">
-      <c r="B57" s="121"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="2:13" ht="15">
-      <c r="B58" s="121"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="15">
-      <c r="B59" s="121"/>
+      <c r="B59" s="116"/>
       <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:13" ht="15">
-      <c r="B60" s="121"/>
+      <c r="B60" s="116"/>
       <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="G60" s="34"/>
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B61" s="121"/>
+      <c r="B61" s="116"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
     <row r="64" spans="2:13" ht="15">
-      <c r="B64" s="122" t="s">
+      <c r="B64" s="117" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3444,7 +3444,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="123"/>
+      <c r="B65" s="118"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3464,7 +3464,7 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="123"/>
+      <c r="B66" s="118"/>
       <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="123"/>
+      <c r="B67" s="118"/>
       <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
@@ -3495,7 +3495,7 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="123"/>
+      <c r="B68" s="118"/>
       <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="123"/>
+      <c r="B69" s="118"/>
       <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="123"/>
+      <c r="B70" s="118"/>
       <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
@@ -3549,7 +3549,7 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="123"/>
+      <c r="B71" s="118"/>
       <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
@@ -3566,7 +3566,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="123"/>
+      <c r="B72" s="118"/>
       <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
@@ -3583,7 +3583,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="123"/>
+      <c r="B73" s="118"/>
       <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="123"/>
+      <c r="B74" s="118"/>
       <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
@@ -3617,7 +3617,7 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="123"/>
+      <c r="B75" s="118"/>
       <c r="C75" s="105" t="s">
         <v>139</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="123"/>
+      <c r="B76" s="118"/>
       <c r="C76" s="105" t="s">
         <v>140</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="123"/>
+      <c r="B77" s="118"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3662,7 +3662,7 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="123"/>
+      <c r="B78" s="118"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="81" spans="2:9" ht="15" customHeight="1">
-      <c r="B81" s="120" t="s">
+      <c r="B81" s="115" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3721,7 +3721,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B82" s="121"/>
+      <c r="B82" s="116"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="G82" s="33"/>
     </row>
     <row r="83" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B83" s="121"/>
+      <c r="B83" s="116"/>
       <c r="C83" s="106" t="s">
         <v>141</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:9" ht="15">
-      <c r="B84" s="121"/>
+      <c r="B84" s="116"/>
       <c r="C84" s="106" t="s">
         <v>142</v>
       </c>
@@ -3771,7 +3771,7 @@
       <c r="H84" s="41"/>
     </row>
     <row r="85" spans="2:9" ht="15">
-      <c r="B85" s="121"/>
+      <c r="B85" s="116"/>
       <c r="C85" s="106" t="s">
         <v>143</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:9" ht="15" customHeight="1">
-      <c r="B86" s="121"/>
+      <c r="B86" s="116"/>
       <c r="C86" s="106" t="s">
         <v>144</v>
       </c>
@@ -3805,7 +3805,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="121"/>
+      <c r="B87" s="116"/>
       <c r="C87" s="106" t="s">
         <v>145</v>
       </c>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="91" spans="2:9" ht="15" customHeight="1">
-      <c r="B91" s="122" t="s">
+      <c r="B91" s="117" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="42" t="s">
@@ -3884,7 +3884,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B92" s="123"/>
+      <c r="B92" s="118"/>
       <c r="C92" s="27" t="s">
         <v>29</v>
       </c>
@@ -3901,7 +3901,7 @@
       <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B93" s="123"/>
+      <c r="B93" s="118"/>
       <c r="C93" s="106" t="s">
         <v>147</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="G93" s="34"/>
     </row>
     <row r="94" spans="2:9" ht="15">
-      <c r="B94" s="123"/>
+      <c r="B94" s="118"/>
       <c r="C94" s="106" t="s">
         <v>148</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="H94" s="41"/>
     </row>
     <row r="95" spans="2:9" ht="15">
-      <c r="B95" s="123"/>
+      <c r="B95" s="118"/>
       <c r="C95" s="106" t="s">
         <v>149</v>
       </c>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="120" t="s">
+      <c r="B99" s="115" t="s">
         <v>19</v>
       </c>
       <c r="C99" s="38" t="s">
@@ -4010,7 +4010,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="121"/>
+      <c r="B100" s="116"/>
       <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="G100" s="33"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="121"/>
+      <c r="B101" s="116"/>
       <c r="C101" s="108" t="s">
         <v>121</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="121"/>
+      <c r="B102" s="116"/>
       <c r="C102" s="108" t="s">
         <v>150</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="H102" s="41"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="121"/>
+      <c r="B103" s="116"/>
       <c r="C103" s="108" t="s">
         <v>151</v>
       </c>
@@ -4079,7 +4079,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="121"/>
+      <c r="B104" s="116"/>
       <c r="C104" s="109" t="s">
         <v>152</v>
       </c>
@@ -4096,7 +4096,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="121"/>
+      <c r="B105" s="116"/>
       <c r="C105" s="109" t="s">
         <v>121</v>
       </c>
@@ -4113,7 +4113,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="121"/>
+      <c r="B106" s="116"/>
       <c r="C106" s="109" t="s">
         <v>121</v>
       </c>
@@ -4130,7 +4130,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="121"/>
+      <c r="B107" s="116"/>
       <c r="C107" s="109" t="s">
         <v>121</v>
       </c>
@@ -4147,7 +4147,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="121"/>
+      <c r="B108" s="116"/>
       <c r="C108" s="109" t="s">
         <v>121</v>
       </c>
@@ -4164,7 +4164,7 @@
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="121"/>
+      <c r="B109" s="116"/>
       <c r="C109" s="109" t="s">
         <v>153</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="121"/>
+      <c r="B110" s="116"/>
       <c r="C110" s="110" t="s">
         <v>154</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="121"/>
+      <c r="B111" s="116"/>
       <c r="C111" s="110" t="s">
         <v>155</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="G111" s="34"/>
     </row>
     <row r="112" spans="2:8" ht="15">
-      <c r="B112" s="121"/>
+      <c r="B112" s="116"/>
       <c r="C112" s="110" t="s">
         <v>156</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="G112" s="34"/>
     </row>
     <row r="113" spans="2:9" ht="15">
-      <c r="B113" s="121"/>
+      <c r="B113" s="116"/>
       <c r="C113" s="110" t="s">
         <v>121</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="G113" s="34"/>
     </row>
     <row r="114" spans="2:9" ht="15">
-      <c r="B114" s="121"/>
+      <c r="B114" s="116"/>
       <c r="C114" s="110" t="s">
         <v>157</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="G114" s="34"/>
     </row>
     <row r="115" spans="2:9" ht="15">
-      <c r="B115" s="121"/>
+      <c r="B115" s="116"/>
       <c r="C115" s="111" t="s">
         <v>158</v>
       </c>
@@ -4283,7 +4283,7 @@
       <c r="G115" s="34"/>
     </row>
     <row r="116" spans="2:9" ht="15">
-      <c r="B116" s="121"/>
+      <c r="B116" s="116"/>
       <c r="C116" s="111" t="s">
         <v>159</v>
       </c>
@@ -4300,7 +4300,7 @@
       <c r="G116" s="34"/>
     </row>
     <row r="117" spans="2:9" ht="15">
-      <c r="B117" s="121"/>
+      <c r="B117" s="116"/>
       <c r="C117" s="111" t="s">
         <v>160</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="G117" s="34"/>
     </row>
     <row r="118" spans="2:9" ht="15">
-      <c r="B118" s="121"/>
+      <c r="B118" s="116"/>
       <c r="C118" s="111" t="s">
         <v>161</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B119" s="121"/>
+      <c r="B119" s="116"/>
       <c r="C119" s="27" t="s">
         <v>32</v>
       </c>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="121" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="122" spans="2:9" ht="15" customHeight="1">
-      <c r="B122" s="122" t="s">
+      <c r="B122" s="117" t="s">
         <v>20</v>
       </c>
       <c r="C122" s="42" t="s">
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="123" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B123" s="123"/>
+      <c r="B123" s="118"/>
       <c r="C123" s="27" t="s">
         <v>29</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="G123" s="33"/>
     </row>
     <row r="124" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B124" s="123"/>
+      <c r="B124" s="118"/>
       <c r="C124" s="112" t="s">
         <v>162</v>
       </c>
@@ -4427,7 +4427,7 @@
       <c r="G124" s="34"/>
     </row>
     <row r="125" spans="2:9" ht="15">
-      <c r="B125" s="123"/>
+      <c r="B125" s="118"/>
       <c r="C125" s="112" t="s">
         <v>163</v>
       </c>
@@ -4445,7 +4445,7 @@
       <c r="H125" s="41"/>
     </row>
     <row r="126" spans="2:9" ht="15">
-      <c r="B126" s="123"/>
+      <c r="B126" s="118"/>
       <c r="C126" s="112" t="s">
         <v>164</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="G126" s="34"/>
     </row>
     <row r="127" spans="2:9" ht="15" customHeight="1">
-      <c r="B127" s="123"/>
+      <c r="B127" s="118"/>
       <c r="C127" s="112" t="s">
         <v>165</v>
       </c>
@@ -4477,7 +4477,7 @@
       <c r="G127" s="34"/>
     </row>
     <row r="128" spans="2:9" ht="15">
-      <c r="B128" s="123"/>
+      <c r="B128" s="118"/>
       <c r="C128" s="112" t="s">
         <v>166</v>
       </c>
@@ -4501,7 +4501,7 @@
       </c>
     </row>
     <row r="129" spans="2:9" ht="15">
-      <c r="B129" s="123"/>
+      <c r="B129" s="118"/>
       <c r="C129" s="112" t="s">
         <v>167</v>
       </c>
@@ -4525,7 +4525,7 @@
       </c>
     </row>
     <row r="130" spans="2:9" ht="15">
-      <c r="B130" s="123"/>
+      <c r="B130" s="118"/>
       <c r="C130" s="112" t="s">
         <v>168</v>
       </c>
@@ -4549,7 +4549,7 @@
       </c>
     </row>
     <row r="131" spans="2:9" ht="15">
-      <c r="B131" s="123"/>
+      <c r="B131" s="118"/>
       <c r="C131" s="112" t="s">
         <v>169</v>
       </c>
@@ -4566,7 +4566,7 @@
       <c r="G131" s="34"/>
     </row>
     <row r="132" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B132" s="123"/>
+      <c r="B132" s="118"/>
       <c r="C132" s="27" t="s">
         <v>32</v>
       </c>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="134" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="135" spans="2:9" ht="15" customHeight="1">
-      <c r="B135" s="122" t="s">
+      <c r="B135" s="117" t="s">
         <v>170</v>
       </c>
       <c r="C135" s="42" t="s">
@@ -4625,7 +4625,7 @@
       </c>
     </row>
     <row r="136" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B136" s="123"/>
+      <c r="B136" s="118"/>
       <c r="C136" s="27" t="s">
         <v>29</v>
       </c>
@@ -4642,7 +4642,7 @@
       <c r="G136" s="33"/>
     </row>
     <row r="137" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B137" s="123"/>
+      <c r="B137" s="118"/>
       <c r="C137" s="113" t="s">
         <v>171</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="G137" s="34"/>
     </row>
     <row r="138" spans="2:9" ht="15">
-      <c r="B138" s="123"/>
+      <c r="B138" s="118"/>
       <c r="C138" s="113" t="s">
         <v>172</v>
       </c>
@@ -4679,7 +4679,7 @@
       </c>
     </row>
     <row r="139" spans="2:9" ht="15">
-      <c r="B139" s="123"/>
+      <c r="B139" s="118"/>
       <c r="C139" s="113" t="s">
         <v>174</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:9" ht="15">
-      <c r="B140" s="123"/>
+      <c r="B140" s="118"/>
       <c r="C140" s="113" t="s">
         <v>175</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:9" ht="15">
-      <c r="B141" s="123"/>
+      <c r="B141" s="118"/>
       <c r="C141" s="113" t="s">
         <v>176</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="G141" s="34"/>
     </row>
     <row r="142" spans="2:9" ht="15">
-      <c r="B142" s="123"/>
+      <c r="B142" s="118"/>
       <c r="C142" s="113" t="s">
         <v>177</v>
       </c>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="145" spans="2:7" ht="13.5" thickBot="1"/>
     <row r="146" spans="2:7" ht="15" customHeight="1">
-      <c r="B146" s="120" t="s">
+      <c r="B146" s="115" t="s">
         <v>178</v>
       </c>
       <c r="C146" s="38" t="s">
@@ -4804,7 +4804,7 @@
       </c>
     </row>
     <row r="147" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B147" s="121"/>
+      <c r="B147" s="116"/>
       <c r="C147" s="27" t="s">
         <v>29</v>
       </c>
@@ -4821,8 +4821,8 @@
       <c r="G147" s="33"/>
     </row>
     <row r="148" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B148" s="121"/>
-      <c r="C148" s="155" t="s">
+      <c r="B148" s="116"/>
+      <c r="C148" s="114" t="s">
         <v>180</v>
       </c>
       <c r="D148" s="30">
@@ -4838,8 +4838,8 @@
       <c r="G148" s="34"/>
     </row>
     <row r="149" spans="2:7" ht="15">
-      <c r="B149" s="121"/>
-      <c r="C149" s="155" t="s">
+      <c r="B149" s="116"/>
+      <c r="C149" s="114" t="s">
         <v>181</v>
       </c>
       <c r="D149" s="30">
@@ -4855,8 +4855,8 @@
       <c r="G149" s="34"/>
     </row>
     <row r="150" spans="2:7" ht="15">
-      <c r="B150" s="121"/>
-      <c r="C150" s="155" t="s">
+      <c r="B150" s="116"/>
+      <c r="C150" s="114" t="s">
         <v>179</v>
       </c>
       <c r="D150" s="30">
@@ -4872,8 +4872,8 @@
       <c r="G150" s="34"/>
     </row>
     <row r="151" spans="2:7" ht="15">
-      <c r="B151" s="121"/>
-      <c r="C151" s="155" t="s">
+      <c r="B151" s="116"/>
+      <c r="C151" s="114" t="s">
         <v>182</v>
       </c>
       <c r="D151" s="30">
@@ -4889,8 +4889,8 @@
       <c r="G151" s="34"/>
     </row>
     <row r="152" spans="2:7" ht="15">
-      <c r="B152" s="121"/>
-      <c r="C152" s="155" t="s">
+      <c r="B152" s="116"/>
+      <c r="C152" s="114" t="s">
         <v>183</v>
       </c>
       <c r="D152" s="30">
@@ -4906,19 +4906,19 @@
       <c r="G152" s="34"/>
     </row>
     <row r="153" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B153" s="121"/>
+      <c r="B153" s="116"/>
       <c r="C153" s="27" t="s">
         <v>32</v>
       </c>
       <c r="D153" s="28">
-        <v>48431</v>
+        <v>48395</v>
       </c>
       <c r="E153" s="28">
         <v>54956</v>
       </c>
       <c r="F153" s="54">
         <f t="shared" si="11"/>
-        <v>6525</v>
+        <v>6561</v>
       </c>
       <c r="G153" s="33"/>
     </row>
@@ -4931,7 +4931,7 @@
       </c>
       <c r="D154" s="32">
         <f>D153-D147</f>
-        <v>5716</v>
+        <v>5680</v>
       </c>
       <c r="E154" s="32">
         <f>E153-E147</f>
@@ -4939,18 +4939,12 @@
       </c>
       <c r="F154" s="32">
         <f>F153-F147</f>
-        <v>644</v>
+        <v>680</v>
       </c>
       <c r="G154" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B146:B153"/>
-    <mergeCell ref="B122:B132"/>
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B43:B61"/>
-    <mergeCell ref="B64:B78"/>
-    <mergeCell ref="B135:B142"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
@@ -4959,6 +4953,12 @@
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="B81:B87"/>
     <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="B122:B132"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B43:B61"/>
+    <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B135:B142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4984,51 +4984,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="129"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="130"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="126"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="127"/>
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1">
       <c r="A4" s="16" t="s">
@@ -5142,19 +5142,19 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="125"/>
-      <c r="J11" s="125"/>
-      <c r="K11" s="126"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="127"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
@@ -5268,19 +5268,19 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="125"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="126"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="126"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="126"/>
+      <c r="K19" s="127"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="16" t="s">
@@ -5394,19 +5394,19 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A27" s="124" t="s">
+      <c r="A27" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="125"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="125"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="125"/>
-      <c r="K27" s="126"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="126"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="126"/>
+      <c r="K27" s="127"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="82" t="s">
@@ -5520,19 +5520,19 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A35" s="124" t="s">
+      <c r="A35" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="125"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="126"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="126"/>
+      <c r="H35" s="126"/>
+      <c r="I35" s="126"/>
+      <c r="J35" s="126"/>
+      <c r="K35" s="127"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="82" t="s">
@@ -5644,19 +5644,19 @@
       <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A43" s="124" t="s">
+      <c r="A43" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="125"/>
-      <c r="C43" s="125"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="125"/>
-      <c r="I43" s="125"/>
-      <c r="J43" s="125"/>
-      <c r="K43" s="126"/>
+      <c r="B43" s="126"/>
+      <c r="C43" s="126"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="126"/>
+      <c r="G43" s="126"/>
+      <c r="H43" s="126"/>
+      <c r="I43" s="126"/>
+      <c r="J43" s="126"/>
+      <c r="K43" s="127"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="82" t="s">
@@ -5770,19 +5770,19 @@
       <c r="K50" s="87"/>
     </row>
     <row r="51" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A51" s="124" t="s">
+      <c r="A51" s="125" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="125"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="125"/>
-      <c r="I51" s="125"/>
-      <c r="J51" s="125"/>
-      <c r="K51" s="126"/>
+      <c r="B51" s="126"/>
+      <c r="C51" s="126"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="126"/>
+      <c r="F51" s="126"/>
+      <c r="G51" s="126"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="126"/>
+      <c r="K51" s="127"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="82" t="s">
@@ -5902,19 +5902,19 @@
       <c r="K58" s="87"/>
     </row>
     <row r="59" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A59" s="124" t="s">
+      <c r="A59" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="125"/>
-      <c r="C59" s="125"/>
-      <c r="D59" s="125"/>
-      <c r="E59" s="125"/>
-      <c r="F59" s="125"/>
-      <c r="G59" s="125"/>
-      <c r="H59" s="125"/>
-      <c r="I59" s="125"/>
-      <c r="J59" s="125"/>
-      <c r="K59" s="126"/>
+      <c r="B59" s="126"/>
+      <c r="C59" s="126"/>
+      <c r="D59" s="126"/>
+      <c r="E59" s="126"/>
+      <c r="F59" s="126"/>
+      <c r="G59" s="126"/>
+      <c r="H59" s="126"/>
+      <c r="I59" s="126"/>
+      <c r="J59" s="126"/>
+      <c r="K59" s="127"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="82" t="s">
@@ -6024,19 +6024,19 @@
       <c r="K66" s="87"/>
     </row>
     <row r="67" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A67" s="124" t="s">
+      <c r="A67" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="125"/>
-      <c r="C67" s="125"/>
-      <c r="D67" s="125"/>
-      <c r="E67" s="125"/>
-      <c r="F67" s="125"/>
-      <c r="G67" s="125"/>
-      <c r="H67" s="125"/>
-      <c r="I67" s="125"/>
-      <c r="J67" s="125"/>
-      <c r="K67" s="126"/>
+      <c r="B67" s="126"/>
+      <c r="C67" s="126"/>
+      <c r="D67" s="126"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="126"/>
+      <c r="G67" s="126"/>
+      <c r="H67" s="126"/>
+      <c r="I67" s="126"/>
+      <c r="J67" s="126"/>
+      <c r="K67" s="127"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="82" t="s">
@@ -6144,19 +6144,19 @@
       <c r="K74" s="87"/>
     </row>
     <row r="75" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A75" s="124" t="s">
+      <c r="A75" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="125"/>
-      <c r="C75" s="125"/>
-      <c r="D75" s="125"/>
-      <c r="E75" s="125"/>
-      <c r="F75" s="125"/>
-      <c r="G75" s="125"/>
-      <c r="H75" s="125"/>
-      <c r="I75" s="125"/>
-      <c r="J75" s="125"/>
-      <c r="K75" s="126"/>
+      <c r="B75" s="126"/>
+      <c r="C75" s="126"/>
+      <c r="D75" s="126"/>
+      <c r="E75" s="126"/>
+      <c r="F75" s="126"/>
+      <c r="G75" s="126"/>
+      <c r="H75" s="126"/>
+      <c r="I75" s="126"/>
+      <c r="J75" s="126"/>
+      <c r="K75" s="127"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="82" t="s">
@@ -6272,19 +6272,19 @@
       <c r="K82" s="87"/>
     </row>
     <row r="83" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A83" s="124" t="s">
+      <c r="A83" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="125"/>
-      <c r="C83" s="125"/>
-      <c r="D83" s="125"/>
-      <c r="E83" s="125"/>
-      <c r="F83" s="125"/>
-      <c r="G83" s="125"/>
-      <c r="H83" s="125"/>
-      <c r="I83" s="125"/>
-      <c r="J83" s="125"/>
-      <c r="K83" s="126"/>
+      <c r="B83" s="126"/>
+      <c r="C83" s="126"/>
+      <c r="D83" s="126"/>
+      <c r="E83" s="126"/>
+      <c r="F83" s="126"/>
+      <c r="G83" s="126"/>
+      <c r="H83" s="126"/>
+      <c r="I83" s="126"/>
+      <c r="J83" s="126"/>
+      <c r="K83" s="127"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="82" t="s">
@@ -6396,19 +6396,19 @@
       <c r="K90" s="87"/>
     </row>
     <row r="91" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A91" s="124" t="s">
+      <c r="A91" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="125"/>
-      <c r="C91" s="125"/>
-      <c r="D91" s="125"/>
-      <c r="E91" s="125"/>
-      <c r="F91" s="125"/>
-      <c r="G91" s="125"/>
-      <c r="H91" s="125"/>
-      <c r="I91" s="125"/>
-      <c r="J91" s="125"/>
-      <c r="K91" s="126"/>
+      <c r="B91" s="126"/>
+      <c r="C91" s="126"/>
+      <c r="D91" s="126"/>
+      <c r="E91" s="126"/>
+      <c r="F91" s="126"/>
+      <c r="G91" s="126"/>
+      <c r="H91" s="126"/>
+      <c r="I91" s="126"/>
+      <c r="J91" s="126"/>
+      <c r="K91" s="127"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="82" t="s">
@@ -6522,19 +6522,19 @@
       <c r="K98" s="87"/>
     </row>
     <row r="99" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A99" s="124" t="s">
+      <c r="A99" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="125"/>
-      <c r="C99" s="125"/>
-      <c r="D99" s="125"/>
-      <c r="E99" s="125"/>
-      <c r="F99" s="125"/>
-      <c r="G99" s="125"/>
-      <c r="H99" s="125"/>
-      <c r="I99" s="125"/>
-      <c r="J99" s="125"/>
-      <c r="K99" s="126"/>
+      <c r="B99" s="126"/>
+      <c r="C99" s="126"/>
+      <c r="D99" s="126"/>
+      <c r="E99" s="126"/>
+      <c r="F99" s="126"/>
+      <c r="G99" s="126"/>
+      <c r="H99" s="126"/>
+      <c r="I99" s="126"/>
+      <c r="J99" s="126"/>
+      <c r="K99" s="127"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="82" t="s">
@@ -6638,19 +6638,19 @@
       <c r="K106" s="87"/>
     </row>
     <row r="107" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A107" s="124" t="s">
+      <c r="A107" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="125"/>
-      <c r="C107" s="125"/>
-      <c r="D107" s="125"/>
-      <c r="E107" s="125"/>
-      <c r="F107" s="125"/>
-      <c r="G107" s="125"/>
-      <c r="H107" s="125"/>
-      <c r="I107" s="125"/>
-      <c r="J107" s="125"/>
-      <c r="K107" s="126"/>
+      <c r="B107" s="126"/>
+      <c r="C107" s="126"/>
+      <c r="D107" s="126"/>
+      <c r="E107" s="126"/>
+      <c r="F107" s="126"/>
+      <c r="G107" s="126"/>
+      <c r="H107" s="126"/>
+      <c r="I107" s="126"/>
+      <c r="J107" s="126"/>
+      <c r="K107" s="127"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="82" t="s">
@@ -6755,22 +6755,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7014,10 +7014,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="132"/>
+      <c r="C1" s="133"/>
       <c r="D1" s="21"/>
       <c r="E1" s="20"/>
     </row>
@@ -7028,7 +7028,7 @@
       <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="134" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -7042,7 +7042,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="134"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="57" t="s">
         <v>8</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="134"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="57" t="s">
         <v>9</v>
       </c>
@@ -7063,7 +7063,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="134"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="68" t="s">
         <v>59</v>
       </c>
@@ -7075,7 +7075,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="134"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="57" t="s">
         <v>22</v>
       </c>
@@ -7087,7 +7087,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="134"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="57" t="s">
         <v>23</v>
       </c>
@@ -7096,7 +7096,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="135"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="65" t="s">
         <v>10</v>
       </c>
@@ -7111,7 +7111,7 @@
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="134" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="60" t="s">
@@ -7125,7 +7125,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="134"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
@@ -7137,7 +7137,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="134"/>
+      <c r="A13" s="135"/>
       <c r="B13" s="57" t="s">
         <v>9</v>
       </c>
@@ -7146,7 +7146,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="134"/>
+      <c r="A14" s="135"/>
       <c r="B14" s="68" t="s">
         <v>59</v>
       </c>
@@ -7158,7 +7158,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="134"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="57" t="s">
         <v>22</v>
       </c>
@@ -7170,7 +7170,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="134"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="57" t="s">
         <v>23</v>
       </c>
@@ -7179,7 +7179,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="135"/>
+      <c r="A17" s="136"/>
       <c r="B17" s="65" t="s">
         <v>10</v>
       </c>
@@ -7194,7 +7194,7 @@
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="133" t="s">
+      <c r="A19" s="134" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="60" t="s">
@@ -7203,7 +7203,7 @@
       <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="134"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="57" t="s">
         <v>8</v>
       </c>
@@ -7213,14 +7213,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="134"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="57" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="62"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="134"/>
+      <c r="A22" s="135"/>
       <c r="B22" s="68" t="s">
         <v>59</v>
       </c>
@@ -7230,7 +7230,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="134"/>
+      <c r="A23" s="135"/>
       <c r="B23" s="57" t="s">
         <v>22</v>
       </c>
@@ -7240,14 +7240,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="134"/>
+      <c r="A24" s="135"/>
       <c r="B24" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="61"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="135"/>
+      <c r="A25" s="136"/>
       <c r="B25" s="65" t="s">
         <v>10</v>
       </c>
@@ -7291,17 +7291,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="153"/>
+      <c r="B2" s="144"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="145" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="153"/>
+      <c r="B3" s="144"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
@@ -7317,115 +7317,128 @@
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="140" t="s">
+      <c r="A7" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="155"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="142" t="s">
+      <c r="A9" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="143"/>
+      <c r="B9" s="153"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="144"/>
-      <c r="B10" s="145"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="140"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="137"/>
+      <c r="B11" s="142"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="136" t="s">
+      <c r="A12" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="137"/>
+      <c r="B12" s="142"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="137"/>
+      <c r="B13" s="142"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="141" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="137"/>
+      <c r="B14" s="142"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="136" t="s">
+      <c r="A15" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="137"/>
+      <c r="B15" s="142"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="136" t="s">
+      <c r="A16" s="141" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="137"/>
+      <c r="B16" s="142"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="138" t="s">
+      <c r="A17" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="139"/>
+      <c r="B17" s="138"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="140" t="s">
+      <c r="A19" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="155"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="142" t="s">
+      <c r="A21" s="152" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="143"/>
+      <c r="B21" s="153"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="144"/>
-      <c r="B22" s="145"/>
+      <c r="A22" s="139"/>
+      <c r="B22" s="140"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="136" t="s">
+      <c r="A23" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="137"/>
+      <c r="B23" s="142"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="136"/>
-      <c r="B24" s="137"/>
+      <c r="A24" s="141"/>
+      <c r="B24" s="142"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="136" t="s">
+      <c r="A25" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="137"/>
+      <c r="B25" s="142"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="136" t="s">
+      <c r="A26" s="141" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="137"/>
+      <c r="B26" s="142"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="138"/>
-      <c r="B27" s="139"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -7436,19 +7449,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminator - more release prep
</commit_message>
<xml_diff>
--- a/Terminator/TerminatorSegaCD.xlsx
+++ b/Terminator/TerminatorSegaCD.xlsx
@@ -1754,18 +1754,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1778,6 +1766,18 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1810,43 +1810,43 @@
     <xf numFmtId="0" fontId="42" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Färg1" xfId="2" builtinId="29"/>
@@ -2153,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2168,16 +2168,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="33">
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="120" t="s">
+      <c r="C1" s="115"/>
+      <c r="D1" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="121"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="117"/>
       <c r="H1" s="70"/>
       <c r="I1" s="71">
         <f>SUM(H1:H65514)</f>
@@ -2255,10 +2255,10 @@
       <c r="C5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="122" t="s">
+      <c r="D5" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="122"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="77"/>
       <c r="G5" s="73"/>
       <c r="H5" s="70"/>
@@ -2295,7 +2295,7 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1">
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="119" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2315,7 +2315,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B9" s="124"/>
+      <c r="B9" s="120"/>
       <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickTop="1">
-      <c r="B10" s="124"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -2336,7 +2336,7 @@
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:12" ht="15">
-      <c r="B11" s="124"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2347,7 +2347,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:12" ht="15">
-      <c r="B12" s="124"/>
+      <c r="B12" s="120"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2358,7 +2358,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:12" ht="15">
-      <c r="B13" s="124"/>
+      <c r="B13" s="120"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2369,7 +2369,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:12" ht="15">
-      <c r="B14" s="124"/>
+      <c r="B14" s="120"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -2380,7 +2380,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="124"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="29"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -2391,7 +2391,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B16" s="124"/>
+      <c r="B16" s="120"/>
       <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
@@ -2434,7 +2434,7 @@
     </row>
     <row r="18" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="19" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="121" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B20" s="116"/>
+      <c r="B20" s="122"/>
       <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
@@ -2502,7 +2502,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B21" s="116"/>
+      <c r="B21" s="122"/>
       <c r="C21" s="92" t="s">
         <v>99</v>
       </c>
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" ht="15">
-      <c r="B22" s="116"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="92" t="s">
         <v>100</v>
       </c>
@@ -2568,7 +2568,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15">
-      <c r="B23" s="116"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="92" t="s">
         <v>103</v>
       </c>
@@ -2601,7 +2601,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15">
-      <c r="B24" s="116"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="92" t="s">
         <v>104</v>
       </c>
@@ -2637,7 +2637,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" ht="15">
-      <c r="B25" s="116"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="92" t="s">
         <v>105</v>
       </c>
@@ -2670,7 +2670,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="15">
-      <c r="B26" s="116"/>
+      <c r="B26" s="122"/>
       <c r="C26" s="92" t="s">
         <v>106</v>
       </c>
@@ -2703,7 +2703,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="15">
-      <c r="B27" s="116"/>
+      <c r="B27" s="122"/>
       <c r="C27" s="92" t="s">
         <v>107</v>
       </c>
@@ -2736,7 +2736,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B28" s="116"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="27" t="s">
         <v>32</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B29" s="116"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="31" t="s">
         <v>24</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="B30" s="93"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="123" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2830,7 +2830,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B32" s="118"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B33" s="118"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="100" t="s">
         <v>111</v>
       </c>
@@ -2888,7 +2888,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15">
-      <c r="B34" s="118"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="100" t="s">
         <v>112</v>
       </c>
@@ -2918,7 +2918,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15">
-      <c r="B35" s="118"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="100" t="s">
         <v>113</v>
       </c>
@@ -2938,7 +2938,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1">
-      <c r="B36" s="118"/>
+      <c r="B36" s="124"/>
       <c r="C36" s="100" t="s">
         <v>114</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" ht="15">
-      <c r="B37" s="118"/>
+      <c r="B37" s="124"/>
       <c r="C37" s="100" t="s">
         <v>115</v>
       </c>
@@ -2981,7 +2981,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="15">
-      <c r="B38" s="118"/>
+      <c r="B38" s="124"/>
       <c r="C38" s="100" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15">
-      <c r="B39" s="118"/>
+      <c r="B39" s="124"/>
       <c r="C39" s="100" t="s">
         <v>117</v>
       </c>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="42" spans="2:15" ht="13.5" thickBot="1"/>
     <row r="43" spans="2:15" ht="15">
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="121" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -3092,7 +3092,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B44" s="116"/>
+      <c r="B44" s="122"/>
       <c r="C44" s="27" t="s">
         <v>29</v>
       </c>
@@ -3109,7 +3109,7 @@
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickTop="1">
-      <c r="B45" s="116"/>
+      <c r="B45" s="122"/>
       <c r="C45" s="102" t="s">
         <v>118</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="2:15" ht="15">
-      <c r="B46" s="116"/>
+      <c r="B46" s="122"/>
       <c r="C46" s="102" t="s">
         <v>119</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="H46" s="41"/>
     </row>
     <row r="47" spans="2:15" ht="15">
-      <c r="B47" s="116"/>
+      <c r="B47" s="122"/>
       <c r="C47" s="103" t="s">
         <v>120</v>
       </c>
@@ -3161,7 +3161,7 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:15" ht="15" customHeight="1">
-      <c r="B48" s="116"/>
+      <c r="B48" s="122"/>
       <c r="C48" s="103" t="s">
         <v>121</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:13" ht="15">
-      <c r="B49" s="116"/>
+      <c r="B49" s="122"/>
       <c r="C49" s="103" t="s">
         <v>122</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="2:13" ht="15">
-      <c r="B50" s="116"/>
+      <c r="B50" s="122"/>
       <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:13" ht="15">
-      <c r="B51" s="116"/>
+      <c r="B51" s="122"/>
       <c r="C51" s="104" t="s">
         <v>124</v>
       </c>
@@ -3229,7 +3229,7 @@
       <c r="G51" s="34"/>
     </row>
     <row r="52" spans="2:13" ht="15">
-      <c r="B52" s="116"/>
+      <c r="B52" s="122"/>
       <c r="C52" s="104" t="s">
         <v>125</v>
       </c>
@@ -3246,7 +3246,7 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:13" ht="15">
-      <c r="B53" s="116"/>
+      <c r="B53" s="122"/>
       <c r="C53" s="104" t="s">
         <v>126</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:13" ht="15">
-      <c r="B54" s="116"/>
+      <c r="B54" s="122"/>
       <c r="C54" s="104" t="s">
         <v>127</v>
       </c>
@@ -3280,7 +3280,7 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="2:13" ht="15">
-      <c r="B55" s="116"/>
+      <c r="B55" s="122"/>
       <c r="C55" s="104" t="s">
         <v>120</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="G55" s="34"/>
     </row>
     <row r="56" spans="2:13" ht="15">
-      <c r="B56" s="116"/>
+      <c r="B56" s="122"/>
       <c r="C56" s="104" t="s">
         <v>120</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:13" ht="15">
-      <c r="B57" s="116"/>
+      <c r="B57" s="122"/>
       <c r="C57" s="104" t="s">
         <v>128</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="G57" s="34"/>
     </row>
     <row r="58" spans="2:13" ht="15">
-      <c r="B58" s="116"/>
+      <c r="B58" s="122"/>
       <c r="C58" s="104" t="s">
         <v>129</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
     </row>
     <row r="59" spans="2:13" ht="15">
-      <c r="B59" s="116"/>
+      <c r="B59" s="122"/>
       <c r="C59" s="104" t="s">
         <v>130</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:13" ht="15">
-      <c r="B60" s="116"/>
+      <c r="B60" s="122"/>
       <c r="C60" s="104" t="s">
         <v>131</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="G60" s="34"/>
     </row>
     <row r="61" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B61" s="116"/>
+      <c r="B61" s="122"/>
       <c r="C61" s="27" t="s">
         <v>32</v>
       </c>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="63" spans="2:13" ht="13.5" thickBot="1"/>
     <row r="64" spans="2:13" ht="15">
-      <c r="B64" s="117" t="s">
+      <c r="B64" s="123" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="42" t="s">
@@ -3444,7 +3444,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B65" s="118"/>
+      <c r="B65" s="124"/>
       <c r="C65" s="27" t="s">
         <v>29</v>
       </c>
@@ -3464,7 +3464,7 @@
       </c>
     </row>
     <row r="66" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B66" s="118"/>
+      <c r="B66" s="124"/>
       <c r="C66" s="104" t="s">
         <v>121</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="G66" s="34"/>
     </row>
     <row r="67" spans="2:8" ht="15">
-      <c r="B67" s="118"/>
+      <c r="B67" s="124"/>
       <c r="C67" s="104" t="s">
         <v>121</v>
       </c>
@@ -3495,7 +3495,7 @@
       <c r="H67" s="41"/>
     </row>
     <row r="68" spans="2:8" ht="15">
-      <c r="B68" s="118"/>
+      <c r="B68" s="124"/>
       <c r="C68" s="104" t="s">
         <v>133</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1">
-      <c r="B69" s="118"/>
+      <c r="B69" s="124"/>
       <c r="C69" s="104" t="s">
         <v>121</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="2:8" ht="15">
-      <c r="B70" s="118"/>
+      <c r="B70" s="124"/>
       <c r="C70" s="104" t="s">
         <v>134</v>
       </c>
@@ -3549,7 +3549,7 @@
       </c>
     </row>
     <row r="71" spans="2:8" ht="15">
-      <c r="B71" s="118"/>
+      <c r="B71" s="124"/>
       <c r="C71" s="104" t="s">
         <v>136</v>
       </c>
@@ -3566,7 +3566,7 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="15">
-      <c r="B72" s="118"/>
+      <c r="B72" s="124"/>
       <c r="C72" s="104" t="s">
         <v>121</v>
       </c>
@@ -3583,7 +3583,7 @@
       <c r="G72" s="34"/>
     </row>
     <row r="73" spans="2:8" ht="15">
-      <c r="B73" s="118"/>
+      <c r="B73" s="124"/>
       <c r="C73" s="104" t="s">
         <v>137</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="G73" s="34"/>
     </row>
     <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="118"/>
+      <c r="B74" s="124"/>
       <c r="C74" s="104" t="s">
         <v>138</v>
       </c>
@@ -3617,7 +3617,7 @@
       <c r="G74" s="34"/>
     </row>
     <row r="75" spans="2:8" ht="15">
-      <c r="B75" s="118"/>
+      <c r="B75" s="124"/>
       <c r="C75" s="105" t="s">
         <v>139</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="G75" s="34"/>
     </row>
     <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="118"/>
+      <c r="B76" s="124"/>
       <c r="C76" s="105" t="s">
         <v>140</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="G76" s="34"/>
     </row>
     <row r="77" spans="2:8" ht="15">
-      <c r="B77" s="118"/>
+      <c r="B77" s="124"/>
       <c r="C77" s="29"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3662,7 +3662,7 @@
       <c r="G77" s="34"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B78" s="118"/>
+      <c r="B78" s="124"/>
       <c r="C78" s="27" t="s">
         <v>32</v>
       </c>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="80" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="81" spans="2:9" ht="15" customHeight="1">
-      <c r="B81" s="115" t="s">
+      <c r="B81" s="121" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="38" t="s">
@@ -3721,7 +3721,7 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B82" s="116"/>
+      <c r="B82" s="122"/>
       <c r="C82" s="27" t="s">
         <v>29</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="G82" s="33"/>
     </row>
     <row r="83" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B83" s="116"/>
+      <c r="B83" s="122"/>
       <c r="C83" s="106" t="s">
         <v>141</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="G83" s="34"/>
     </row>
     <row r="84" spans="2:9" ht="15">
-      <c r="B84" s="116"/>
+      <c r="B84" s="122"/>
       <c r="C84" s="106" t="s">
         <v>142</v>
       </c>
@@ -3771,7 +3771,7 @@
       <c r="H84" s="41"/>
     </row>
     <row r="85" spans="2:9" ht="15">
-      <c r="B85" s="116"/>
+      <c r="B85" s="122"/>
       <c r="C85" s="106" t="s">
         <v>143</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="2:9" ht="15" customHeight="1">
-      <c r="B86" s="116"/>
+      <c r="B86" s="122"/>
       <c r="C86" s="106" t="s">
         <v>144</v>
       </c>
@@ -3805,7 +3805,7 @@
       <c r="G86" s="34"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="116"/>
+      <c r="B87" s="122"/>
       <c r="C87" s="106" t="s">
         <v>145</v>
       </c>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="90" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="91" spans="2:9" ht="15" customHeight="1">
-      <c r="B91" s="117" t="s">
+      <c r="B91" s="123" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="42" t="s">
@@ -3884,7 +3884,7 @@
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B92" s="118"/>
+      <c r="B92" s="124"/>
       <c r="C92" s="27" t="s">
         <v>29</v>
       </c>
@@ -3901,7 +3901,7 @@
       <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B93" s="118"/>
+      <c r="B93" s="124"/>
       <c r="C93" s="106" t="s">
         <v>147</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="G93" s="34"/>
     </row>
     <row r="94" spans="2:9" ht="15">
-      <c r="B94" s="118"/>
+      <c r="B94" s="124"/>
       <c r="C94" s="106" t="s">
         <v>148</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="H94" s="41"/>
     </row>
     <row r="95" spans="2:9" ht="15">
-      <c r="B95" s="118"/>
+      <c r="B95" s="124"/>
       <c r="C95" s="106" t="s">
         <v>149</v>
       </c>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="98" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="2:8" ht="15">
-      <c r="B99" s="115" t="s">
+      <c r="B99" s="121" t="s">
         <v>19</v>
       </c>
       <c r="C99" s="38" t="s">
@@ -4010,7 +4010,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B100" s="116"/>
+      <c r="B100" s="122"/>
       <c r="C100" s="27" t="s">
         <v>29</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="G100" s="33"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B101" s="116"/>
+      <c r="B101" s="122"/>
       <c r="C101" s="108" t="s">
         <v>121</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="2:8" ht="15">
-      <c r="B102" s="116"/>
+      <c r="B102" s="122"/>
       <c r="C102" s="108" t="s">
         <v>150</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="H102" s="41"/>
     </row>
     <row r="103" spans="2:8" ht="15">
-      <c r="B103" s="116"/>
+      <c r="B103" s="122"/>
       <c r="C103" s="108" t="s">
         <v>151</v>
       </c>
@@ -4079,7 +4079,7 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1">
-      <c r="B104" s="116"/>
+      <c r="B104" s="122"/>
       <c r="C104" s="109" t="s">
         <v>152</v>
       </c>
@@ -4096,7 +4096,7 @@
       <c r="G104" s="34"/>
     </row>
     <row r="105" spans="2:8" ht="15">
-      <c r="B105" s="116"/>
+      <c r="B105" s="122"/>
       <c r="C105" s="109" t="s">
         <v>121</v>
       </c>
@@ -4113,7 +4113,7 @@
       <c r="G105" s="34"/>
     </row>
     <row r="106" spans="2:8" ht="15">
-      <c r="B106" s="116"/>
+      <c r="B106" s="122"/>
       <c r="C106" s="109" t="s">
         <v>121</v>
       </c>
@@ -4130,7 +4130,7 @@
       <c r="G106" s="34"/>
     </row>
     <row r="107" spans="2:8" ht="15">
-      <c r="B107" s="116"/>
+      <c r="B107" s="122"/>
       <c r="C107" s="109" t="s">
         <v>121</v>
       </c>
@@ -4147,7 +4147,7 @@
       <c r="G107" s="34"/>
     </row>
     <row r="108" spans="2:8" ht="15">
-      <c r="B108" s="116"/>
+      <c r="B108" s="122"/>
       <c r="C108" s="109" t="s">
         <v>121</v>
       </c>
@@ -4164,7 +4164,7 @@
       <c r="G108" s="34"/>
     </row>
     <row r="109" spans="2:8" ht="15">
-      <c r="B109" s="116"/>
+      <c r="B109" s="122"/>
       <c r="C109" s="109" t="s">
         <v>153</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="2:8" ht="15">
-      <c r="B110" s="116"/>
+      <c r="B110" s="122"/>
       <c r="C110" s="110" t="s">
         <v>154</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="G110" s="34"/>
     </row>
     <row r="111" spans="2:8" ht="15">
-      <c r="B111" s="116"/>
+      <c r="B111" s="122"/>
       <c r="C111" s="110" t="s">
         <v>155</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="G111" s="34"/>
     </row>
     <row r="112" spans="2:8" ht="15">
-      <c r="B112" s="116"/>
+      <c r="B112" s="122"/>
       <c r="C112" s="110" t="s">
         <v>156</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="G112" s="34"/>
     </row>
     <row r="113" spans="2:9" ht="15">
-      <c r="B113" s="116"/>
+      <c r="B113" s="122"/>
       <c r="C113" s="110" t="s">
         <v>121</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="G113" s="34"/>
     </row>
     <row r="114" spans="2:9" ht="15">
-      <c r="B114" s="116"/>
+      <c r="B114" s="122"/>
       <c r="C114" s="110" t="s">
         <v>157</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="G114" s="34"/>
     </row>
     <row r="115" spans="2:9" ht="15">
-      <c r="B115" s="116"/>
+      <c r="B115" s="122"/>
       <c r="C115" s="111" t="s">
         <v>158</v>
       </c>
@@ -4283,7 +4283,7 @@
       <c r="G115" s="34"/>
     </row>
     <row r="116" spans="2:9" ht="15">
-      <c r="B116" s="116"/>
+      <c r="B116" s="122"/>
       <c r="C116" s="111" t="s">
         <v>159</v>
       </c>
@@ -4300,7 +4300,7 @@
       <c r="G116" s="34"/>
     </row>
     <row r="117" spans="2:9" ht="15">
-      <c r="B117" s="116"/>
+      <c r="B117" s="122"/>
       <c r="C117" s="111" t="s">
         <v>160</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="G117" s="34"/>
     </row>
     <row r="118" spans="2:9" ht="15">
-      <c r="B118" s="116"/>
+      <c r="B118" s="122"/>
       <c r="C118" s="111" t="s">
         <v>161</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="G118" s="34"/>
     </row>
     <row r="119" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B119" s="116"/>
+      <c r="B119" s="122"/>
       <c r="C119" s="27" t="s">
         <v>32</v>
       </c>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="121" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="122" spans="2:9" ht="15" customHeight="1">
-      <c r="B122" s="117" t="s">
+      <c r="B122" s="123" t="s">
         <v>20</v>
       </c>
       <c r="C122" s="42" t="s">
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="123" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B123" s="118"/>
+      <c r="B123" s="124"/>
       <c r="C123" s="27" t="s">
         <v>29</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="G123" s="33"/>
     </row>
     <row r="124" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B124" s="118"/>
+      <c r="B124" s="124"/>
       <c r="C124" s="112" t="s">
         <v>162</v>
       </c>
@@ -4427,7 +4427,7 @@
       <c r="G124" s="34"/>
     </row>
     <row r="125" spans="2:9" ht="15">
-      <c r="B125" s="118"/>
+      <c r="B125" s="124"/>
       <c r="C125" s="112" t="s">
         <v>163</v>
       </c>
@@ -4445,7 +4445,7 @@
       <c r="H125" s="41"/>
     </row>
     <row r="126" spans="2:9" ht="15">
-      <c r="B126" s="118"/>
+      <c r="B126" s="124"/>
       <c r="C126" s="112" t="s">
         <v>164</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="G126" s="34"/>
     </row>
     <row r="127" spans="2:9" ht="15" customHeight="1">
-      <c r="B127" s="118"/>
+      <c r="B127" s="124"/>
       <c r="C127" s="112" t="s">
         <v>165</v>
       </c>
@@ -4477,7 +4477,7 @@
       <c r="G127" s="34"/>
     </row>
     <row r="128" spans="2:9" ht="15">
-      <c r="B128" s="118"/>
+      <c r="B128" s="124"/>
       <c r="C128" s="112" t="s">
         <v>166</v>
       </c>
@@ -4501,7 +4501,7 @@
       </c>
     </row>
     <row r="129" spans="2:9" ht="15">
-      <c r="B129" s="118"/>
+      <c r="B129" s="124"/>
       <c r="C129" s="112" t="s">
         <v>167</v>
       </c>
@@ -4525,7 +4525,7 @@
       </c>
     </row>
     <row r="130" spans="2:9" ht="15">
-      <c r="B130" s="118"/>
+      <c r="B130" s="124"/>
       <c r="C130" s="112" t="s">
         <v>168</v>
       </c>
@@ -4549,7 +4549,7 @@
       </c>
     </row>
     <row r="131" spans="2:9" ht="15">
-      <c r="B131" s="118"/>
+      <c r="B131" s="124"/>
       <c r="C131" s="112" t="s">
         <v>169</v>
       </c>
@@ -4566,7 +4566,7 @@
       <c r="G131" s="34"/>
     </row>
     <row r="132" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B132" s="118"/>
+      <c r="B132" s="124"/>
       <c r="C132" s="27" t="s">
         <v>32</v>
       </c>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="134" spans="2:9" ht="13.5" thickBot="1"/>
     <row r="135" spans="2:9" ht="15" customHeight="1">
-      <c r="B135" s="117" t="s">
+      <c r="B135" s="123" t="s">
         <v>170</v>
       </c>
       <c r="C135" s="42" t="s">
@@ -4625,7 +4625,7 @@
       </c>
     </row>
     <row r="136" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B136" s="118"/>
+      <c r="B136" s="124"/>
       <c r="C136" s="27" t="s">
         <v>29</v>
       </c>
@@ -4642,7 +4642,7 @@
       <c r="G136" s="33"/>
     </row>
     <row r="137" spans="2:9" ht="15.75" thickTop="1">
-      <c r="B137" s="118"/>
+      <c r="B137" s="124"/>
       <c r="C137" s="113" t="s">
         <v>171</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="G137" s="34"/>
     </row>
     <row r="138" spans="2:9" ht="15">
-      <c r="B138" s="118"/>
+      <c r="B138" s="124"/>
       <c r="C138" s="113" t="s">
         <v>172</v>
       </c>
@@ -4679,7 +4679,7 @@
       </c>
     </row>
     <row r="139" spans="2:9" ht="15">
-      <c r="B139" s="118"/>
+      <c r="B139" s="124"/>
       <c r="C139" s="113" t="s">
         <v>174</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="G139" s="34"/>
     </row>
     <row r="140" spans="2:9" ht="15">
-      <c r="B140" s="118"/>
+      <c r="B140" s="124"/>
       <c r="C140" s="113" t="s">
         <v>175</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="G140" s="34"/>
     </row>
     <row r="141" spans="2:9" ht="15">
-      <c r="B141" s="118"/>
+      <c r="B141" s="124"/>
       <c r="C141" s="113" t="s">
         <v>176</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="G141" s="34"/>
     </row>
     <row r="142" spans="2:9" ht="15">
-      <c r="B142" s="118"/>
+      <c r="B142" s="124"/>
       <c r="C142" s="113" t="s">
         <v>177</v>
       </c>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="145" spans="2:7" ht="13.5" thickBot="1"/>
     <row r="146" spans="2:7" ht="15" customHeight="1">
-      <c r="B146" s="115" t="s">
+      <c r="B146" s="121" t="s">
         <v>178</v>
       </c>
       <c r="C146" s="38" t="s">
@@ -4804,7 +4804,7 @@
       </c>
     </row>
     <row r="147" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B147" s="116"/>
+      <c r="B147" s="122"/>
       <c r="C147" s="27" t="s">
         <v>29</v>
       </c>
@@ -4821,7 +4821,7 @@
       <c r="G147" s="33"/>
     </row>
     <row r="148" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B148" s="116"/>
+      <c r="B148" s="122"/>
       <c r="C148" s="114" t="s">
         <v>180</v>
       </c>
@@ -4838,7 +4838,7 @@
       <c r="G148" s="34"/>
     </row>
     <row r="149" spans="2:7" ht="15">
-      <c r="B149" s="116"/>
+      <c r="B149" s="122"/>
       <c r="C149" s="114" t="s">
         <v>181</v>
       </c>
@@ -4855,7 +4855,7 @@
       <c r="G149" s="34"/>
     </row>
     <row r="150" spans="2:7" ht="15">
-      <c r="B150" s="116"/>
+      <c r="B150" s="122"/>
       <c r="C150" s="114" t="s">
         <v>179</v>
       </c>
@@ -4872,7 +4872,7 @@
       <c r="G150" s="34"/>
     </row>
     <row r="151" spans="2:7" ht="15">
-      <c r="B151" s="116"/>
+      <c r="B151" s="122"/>
       <c r="C151" s="114" t="s">
         <v>182</v>
       </c>
@@ -4889,7 +4889,7 @@
       <c r="G151" s="34"/>
     </row>
     <row r="152" spans="2:7" ht="15">
-      <c r="B152" s="116"/>
+      <c r="B152" s="122"/>
       <c r="C152" s="114" t="s">
         <v>183</v>
       </c>
@@ -4906,7 +4906,7 @@
       <c r="G152" s="34"/>
     </row>
     <row r="153" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B153" s="116"/>
+      <c r="B153" s="122"/>
       <c r="C153" s="27" t="s">
         <v>32</v>
       </c>
@@ -4945,6 +4945,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="B122:B132"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B43:B61"/>
+    <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B135:B142"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
@@ -4953,12 +4959,6 @@
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="B81:B87"/>
     <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B146:B153"/>
-    <mergeCell ref="B122:B132"/>
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B43:B61"/>
-    <mergeCell ref="B64:B78"/>
-    <mergeCell ref="B135:B142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6755,22 +6755,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A75:K75"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A107:K107"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A67:K67"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A67:K67"/>
-    <mergeCell ref="A75:K75"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A107:K107"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7282,163 +7282,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="147"/>
+      <c r="B1" s="148"/>
       <c r="C1" s="47"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="144"/>
+      <c r="B2" s="154"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="144"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="150"/>
-      <c r="B4" s="151"/>
+      <c r="A4" s="151"/>
+      <c r="B4" s="152"/>
       <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="148" t="s">
+      <c r="A5" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="149"/>
+      <c r="B5" s="150"/>
       <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="154" t="s">
+      <c r="A7" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="155"/>
+      <c r="B7" s="142"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="49"/>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="152" t="s">
+      <c r="A9" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="153"/>
+      <c r="B9" s="144"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="139"/>
-      <c r="B10" s="140"/>
+      <c r="A10" s="145"/>
+      <c r="B10" s="146"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="141" t="s">
+      <c r="A11" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="142"/>
+      <c r="B11" s="138"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="141" t="s">
+      <c r="A12" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="142"/>
+      <c r="B12" s="138"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="142"/>
+      <c r="B13" s="138"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="141" t="s">
+      <c r="A14" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="142"/>
+      <c r="B14" s="138"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="141" t="s">
+      <c r="A15" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="142"/>
+      <c r="B15" s="138"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="142"/>
+      <c r="B16" s="138"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="137" t="s">
+      <c r="A17" s="139" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="138"/>
+      <c r="B17" s="140"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="154" t="s">
+      <c r="A19" s="141" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="155"/>
+      <c r="B19" s="142"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="152" t="s">
+      <c r="A21" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="153"/>
+      <c r="B21" s="144"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="139"/>
-      <c r="B22" s="140"/>
+      <c r="A22" s="145"/>
+      <c r="B22" s="146"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="141" t="s">
+      <c r="A23" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="142"/>
+      <c r="B23" s="138"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="141"/>
-      <c r="B24" s="142"/>
+      <c r="A24" s="137"/>
+      <c r="B24" s="138"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="141" t="s">
+      <c r="A25" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="142"/>
+      <c r="B25" s="138"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="141" t="s">
+      <c r="A26" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="142"/>
+      <c r="B26" s="138"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="137"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -7449,6 +7436,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>